<commit_message>
Yazilim araclari hafta 3
</commit_message>
<xml_diff>
--- a/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
+++ b/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e048482\Desktop\Medipol\2018bahar\yazilimaraclari\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_SRC\GIT\MY\MyCourses\SoftwareDevEnvAndTools\_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="192">
   <si>
     <t>Adı</t>
   </si>
@@ -638,6 +638,12 @@
   </si>
   <si>
     <t>YUNUS EMRE</t>
+  </si>
+  <si>
+    <t>ELA</t>
+  </si>
+  <si>
+    <t>H5160070</t>
   </si>
 </sst>
 </file>
@@ -1112,6 +1118,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1121,13 +1129,101 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1307,66 +1403,6 @@
         <patternFill>
           <fgColor auto="1"/>
           <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1684,8 +1720,8 @@
   <dimension ref="A1:Y76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O36" sqref="O36"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC27" sqref="AC27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1694,7 +1730,8 @@
     <col min="2" max="2" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="3.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="2.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.88671875" style="1" customWidth="1"/>
     <col min="12" max="12" width="3.109375" style="1" bestFit="1" customWidth="1"/>
@@ -1711,35 +1748,35 @@
   <sheetData>
     <row r="1" spans="1:25" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="29"/>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="45" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="45" t="s">
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="U1" s="46"/>
-      <c r="V1" s="47"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="49"/>
       <c r="W1" s="17" t="s">
         <v>96</v>
       </c>
@@ -1837,24 +1874,24 @@
       <c r="C3" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="48">
-        <v>2</v>
-      </c>
-      <c r="E3" s="49">
-        <v>2</v>
-      </c>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
+      <c r="D3" s="45">
+        <v>2</v>
+      </c>
+      <c r="E3" s="46">
+        <v>2</v>
+      </c>
+      <c r="F3" s="46">
+        <v>2</v>
+      </c>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="16">
-        <f>SUM(D3:J3)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L3" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" ref="K3:K40" si="0">SUM(D3:J3)*50/A$1</f>
+        <v>150</v>
+      </c>
+      <c r="L3" s="14"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -1862,8 +1899,8 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="16">
-        <f>SUM(L3:R3)/A$1</f>
-        <v>100</v>
+        <f t="shared" ref="S3:S15" si="1">SUM(L3:R3)/A$1</f>
+        <v>0</v>
       </c>
       <c r="T3" s="14"/>
       <c r="U3" s="14"/>
@@ -1872,7 +1909,7 @@
       <c r="X3" s="44"/>
       <c r="Y3" s="21">
         <f>K3*0.2+S3*0.25+V3*0.25+W3*0.3+X3*0.15</f>
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1885,24 +1922,24 @@
       <c r="C4" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="48">
-        <v>2</v>
-      </c>
-      <c r="E4" s="49">
-        <v>2</v>
-      </c>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
+      <c r="D4" s="45">
+        <v>2</v>
+      </c>
+      <c r="E4" s="46">
+        <v>2</v>
+      </c>
+      <c r="F4" s="46">
+        <v>2</v>
+      </c>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
       <c r="K4" s="16">
-        <f>SUM(D4:J4)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L4" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L4" s="14"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -1910,8 +1947,8 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="16">
-        <f>SUM(L4:R4)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T4" s="14"/>
       <c r="U4" s="14"/>
@@ -1920,7 +1957,7 @@
       <c r="X4" s="44"/>
       <c r="Y4" s="21">
         <f>K4*0.2+S4*0.25+V4*0.25+W4*0.3+X4*0.15</f>
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1933,24 +1970,24 @@
       <c r="C5" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="48">
-        <v>2</v>
-      </c>
-      <c r="E5" s="49">
-        <v>2</v>
-      </c>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
+      <c r="D5" s="45">
+        <v>2</v>
+      </c>
+      <c r="E5" s="46">
+        <v>2</v>
+      </c>
+      <c r="F5" s="46">
+        <v>2</v>
+      </c>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
       <c r="K5" s="16">
-        <f>SUM(D5:J5)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L5" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L5" s="14"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
@@ -1958,8 +1995,8 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
       <c r="S5" s="16">
-        <f>SUM(L5:R5)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T5" s="14"/>
       <c r="U5" s="14"/>
@@ -1968,7 +2005,7 @@
       <c r="X5" s="44"/>
       <c r="Y5" s="21">
         <f>K5*0.2+S5*0.25+V5*0.25+W5*0.3+X5*0.15</f>
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1981,24 +2018,24 @@
       <c r="C6" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="48">
-        <v>2</v>
-      </c>
-      <c r="E6" s="49">
-        <v>2</v>
-      </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
+      <c r="D6" s="45">
+        <v>2</v>
+      </c>
+      <c r="E6" s="46">
+        <v>2</v>
+      </c>
+      <c r="F6" s="46">
+        <v>2</v>
+      </c>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
       <c r="K6" s="16">
-        <f>SUM(D6:J6)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L6" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L6" s="14"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -2006,8 +2043,8 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="16">
-        <f>SUM(L6:R6)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T6" s="14"/>
       <c r="U6" s="14"/>
@@ -2016,7 +2053,7 @@
       <c r="X6" s="44"/>
       <c r="Y6" s="21">
         <f>K6*0.2+S6*0.25+V6*0.25+W6*0.3+X6*0.15</f>
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2029,24 +2066,24 @@
       <c r="C7" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="48">
-        <v>2</v>
-      </c>
-      <c r="E7" s="49">
-        <v>2</v>
-      </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
+      <c r="D7" s="45">
+        <v>2</v>
+      </c>
+      <c r="E7" s="46">
+        <v>2</v>
+      </c>
+      <c r="F7" s="46">
+        <v>2</v>
+      </c>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
       <c r="K7" s="16">
-        <f>SUM(D7:J7)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L7" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L7" s="14"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
@@ -2054,8 +2091,8 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="16">
-        <f>SUM(L7:R7)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T7" s="14"/>
       <c r="U7" s="14"/>
@@ -2064,7 +2101,7 @@
       <c r="X7" s="44"/>
       <c r="Y7" s="21">
         <f>K7*0.2+S7*0.25+V7*0.25+W7*0.3+X7*0.15</f>
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2077,24 +2114,24 @@
       <c r="C8" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="D8" s="48">
-        <v>2</v>
-      </c>
-      <c r="E8" s="49">
-        <v>2</v>
-      </c>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
+      <c r="D8" s="45">
+        <v>2</v>
+      </c>
+      <c r="E8" s="46">
+        <v>2</v>
+      </c>
+      <c r="F8" s="46">
+        <v>2</v>
+      </c>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
       <c r="K8" s="16">
-        <f>SUM(D8:J8)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L8" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L8" s="14"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -2102,8 +2139,8 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="16">
-        <f>SUM(L8:R8)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
@@ -2111,8 +2148,8 @@
       <c r="W8" s="6"/>
       <c r="X8" s="44"/>
       <c r="Y8" s="21">
-        <f>K8*0.2+S8*0.25+V8*0.25+W8*0.3+X8*0.1</f>
-        <v>65</v>
+        <f t="shared" ref="Y8:Y15" si="2">K8*0.2+S8*0.25+V8*0.25+W8*0.3+X8*0.1</f>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2125,24 +2162,24 @@
       <c r="C9" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="D9" s="48">
-        <v>2</v>
-      </c>
-      <c r="E9" s="49">
-        <v>2</v>
-      </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
+      <c r="D9" s="45">
+        <v>2</v>
+      </c>
+      <c r="E9" s="46">
+        <v>2</v>
+      </c>
+      <c r="F9" s="46">
+        <v>2</v>
+      </c>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
       <c r="K9" s="16">
-        <f>SUM(D9:J9)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L9" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L9" s="14"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
@@ -2150,8 +2187,8 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="16">
-        <f>SUM(L9:R9)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T9" s="14"/>
       <c r="U9" s="14"/>
@@ -2159,8 +2196,8 @@
       <c r="W9" s="6"/>
       <c r="X9" s="44"/>
       <c r="Y9" s="21">
-        <f>K9*0.2+S9*0.25+V9*0.25+W9*0.3+X9*0.1</f>
-        <v>65</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2173,24 +2210,24 @@
       <c r="C10" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="D10" s="48">
-        <v>2</v>
-      </c>
-      <c r="E10" s="49">
-        <v>2</v>
-      </c>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
+      <c r="D10" s="45">
+        <v>2</v>
+      </c>
+      <c r="E10" s="46">
+        <v>2</v>
+      </c>
+      <c r="F10" s="46">
+        <v>2</v>
+      </c>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
       <c r="K10" s="16">
-        <f>SUM(D10:J10)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L10" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L10" s="14"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
@@ -2198,8 +2235,8 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="16">
-        <f>SUM(L10:R10)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T10" s="14"/>
       <c r="U10" s="14"/>
@@ -2207,8 +2244,8 @@
       <c r="W10" s="6"/>
       <c r="X10" s="44"/>
       <c r="Y10" s="21">
-        <f>K10*0.2+S10*0.25+V10*0.25+W10*0.3+X10*0.1</f>
-        <v>65</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2221,24 +2258,24 @@
       <c r="C11" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="D11" s="48">
-        <v>2</v>
-      </c>
-      <c r="E11" s="49">
-        <v>2</v>
-      </c>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
+      <c r="D11" s="45">
+        <v>2</v>
+      </c>
+      <c r="E11" s="46">
+        <v>2</v>
+      </c>
+      <c r="F11" s="46">
+        <v>2</v>
+      </c>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
       <c r="K11" s="16">
-        <f>SUM(D11:J11)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L11" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L11" s="14"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
@@ -2246,8 +2283,8 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="16">
-        <f>SUM(L11:R11)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T11" s="14"/>
       <c r="U11" s="14"/>
@@ -2255,8 +2292,8 @@
       <c r="W11" s="6"/>
       <c r="X11" s="44"/>
       <c r="Y11" s="21">
-        <f>K11*0.2+S11*0.25+V11*0.25+W11*0.3+X11*0.1</f>
-        <v>65</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2269,24 +2306,24 @@
       <c r="C12" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D12" s="48">
-        <v>2</v>
-      </c>
-      <c r="E12" s="49">
-        <v>2</v>
-      </c>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
+      <c r="D12" s="45">
+        <v>2</v>
+      </c>
+      <c r="E12" s="46">
+        <v>2</v>
+      </c>
+      <c r="F12" s="46">
+        <v>2</v>
+      </c>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
       <c r="K12" s="16">
-        <f>SUM(D12:J12)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L12" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L12" s="14"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
@@ -2294,8 +2331,8 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="16">
-        <f>SUM(L12:R12)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
@@ -2303,8 +2340,8 @@
       <c r="W12" s="6"/>
       <c r="X12" s="44"/>
       <c r="Y12" s="21">
-        <f>K12*0.2+S12*0.25+V12*0.25+W12*0.3+X12*0.1</f>
-        <v>65</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2317,24 +2354,24 @@
       <c r="C13" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D13" s="48">
-        <v>2</v>
-      </c>
-      <c r="E13" s="49">
-        <v>2</v>
-      </c>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
+      <c r="D13" s="45">
+        <v>2</v>
+      </c>
+      <c r="E13" s="46">
+        <v>2</v>
+      </c>
+      <c r="F13" s="46">
+        <v>2</v>
+      </c>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
       <c r="K13" s="16">
-        <f>SUM(D13:J13)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L13" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L13" s="14"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
@@ -2342,8 +2379,8 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="16">
-        <f>SUM(L13:R13)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T13" s="14"/>
       <c r="U13" s="14"/>
@@ -2351,8 +2388,8 @@
       <c r="W13" s="6"/>
       <c r="X13" s="44"/>
       <c r="Y13" s="21">
-        <f>K13*0.2+S13*0.25+V13*0.25+W13*0.3+X13*0.1</f>
-        <v>65</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2365,24 +2402,24 @@
       <c r="C14" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="D14" s="48">
-        <v>2</v>
-      </c>
-      <c r="E14" s="49">
-        <v>2</v>
-      </c>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
+      <c r="D14" s="45">
+        <v>2</v>
+      </c>
+      <c r="E14" s="46">
+        <v>2</v>
+      </c>
+      <c r="F14" s="46">
+        <v>2</v>
+      </c>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
       <c r="K14" s="16">
-        <f>SUM(D14:J14)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L14" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L14" s="14"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
@@ -2390,8 +2427,8 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="16">
-        <f>SUM(L14:R14)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
@@ -2399,8 +2436,8 @@
       <c r="W14" s="6"/>
       <c r="X14" s="44"/>
       <c r="Y14" s="21">
-        <f>K14*0.2+S14*0.25+V14*0.25+W14*0.3+X14*0.1</f>
-        <v>65</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2413,24 +2450,24 @@
       <c r="C15" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="45">
         <v>2</v>
       </c>
       <c r="E15" s="7">
         <v>2</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="46">
+        <v>2</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="16">
-        <f>SUM(D15:J15)*50/A$1</f>
-        <v>200</v>
-      </c>
-      <c r="L15" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L15" s="14"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
@@ -2438,8 +2475,8 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="16">
-        <f>SUM(L15:R15)/A$1</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T15" s="14"/>
       <c r="U15" s="14"/>
@@ -2447,8 +2484,8 @@
       <c r="W15" s="6"/>
       <c r="X15" s="44"/>
       <c r="Y15" s="21">
-        <f>K15*0.2+S15*0.25+V15*0.25+W15*0.3+X15*0.1</f>
-        <v>65</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2461,24 +2498,24 @@
       <c r="C16" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="D16" s="48">
-        <v>2</v>
-      </c>
-      <c r="E16" s="49">
+      <c r="D16" s="45">
+        <v>2</v>
+      </c>
+      <c r="E16" s="46">
         <v>1.7</v>
       </c>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="F16" s="46">
+        <v>0</v>
+      </c>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
       <c r="K16" s="16">
-        <f>SUM(D16:J16)*50/A$1</f>
-        <v>185</v>
-      </c>
-      <c r="L16" s="14">
-        <v>100</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>92.5</v>
+      </c>
+      <c r="L16" s="14"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
@@ -2492,8 +2529,8 @@
       <c r="W16" s="6"/>
       <c r="X16" s="44"/>
       <c r="Y16" s="21">
-        <f>K16*0.2+S16*0.25+V16*0.25+W16*0.3+X16*0.15</f>
-        <v>37</v>
+        <f t="shared" ref="Y16:Y33" si="3">K16*0.2+S16*0.25+V16*0.25+W16*0.3+X16*0.15</f>
+        <v>18.5</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2506,19 +2543,21 @@
       <c r="C17" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="48">
-        <v>0</v>
-      </c>
-      <c r="E17" s="49">
-        <v>2</v>
-      </c>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="D17" s="45">
+        <v>0</v>
+      </c>
+      <c r="E17" s="46">
+        <v>2</v>
+      </c>
+      <c r="F17" s="46">
+        <v>2</v>
+      </c>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
       <c r="K17" s="16">
-        <f>SUM(D17:J17)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L17" s="14"/>
@@ -2535,7 +2574,7 @@
       <c r="W17" s="6"/>
       <c r="X17" s="44"/>
       <c r="Y17" s="21">
-        <f>K17*0.2+S17*0.25+V17*0.25+W17*0.3+X17*0.15</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
@@ -2549,24 +2588,24 @@
       <c r="C18" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D18" s="48">
-        <v>0</v>
-      </c>
-      <c r="E18" s="49">
-        <v>2</v>
-      </c>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="D18" s="45">
+        <v>0</v>
+      </c>
+      <c r="E18" s="46">
+        <v>2</v>
+      </c>
+      <c r="F18" s="46">
+        <v>2</v>
+      </c>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
       <c r="K18" s="16">
-        <f>SUM(D18:J18)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L18" s="14">
-        <v>0</v>
-      </c>
+      <c r="L18" s="14"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
@@ -2583,7 +2622,7 @@
       <c r="W18" s="6"/>
       <c r="X18" s="44"/>
       <c r="Y18" s="21">
-        <f>K18*0.2+S18*0.25+V18*0.25+W18*0.3+X18*0.15</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
@@ -2597,24 +2636,24 @@
       <c r="C19" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="D19" s="48">
-        <v>0</v>
-      </c>
-      <c r="E19" s="49">
-        <v>2</v>
-      </c>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
+      <c r="D19" s="45">
+        <v>0</v>
+      </c>
+      <c r="E19" s="46">
+        <v>2</v>
+      </c>
+      <c r="F19" s="46">
+        <v>2</v>
+      </c>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
       <c r="K19" s="16">
-        <f>SUM(D19:J19)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L19" s="14">
-        <v>0</v>
-      </c>
+      <c r="L19" s="14"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
@@ -2631,7 +2670,7 @@
       <c r="W19" s="6"/>
       <c r="X19" s="44"/>
       <c r="Y19" s="21">
-        <f>K19*0.2+S19*0.25+V19*0.25+W19*0.3+X19*0.15</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
@@ -2645,24 +2684,24 @@
       <c r="C20" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="48">
-        <v>0</v>
-      </c>
-      <c r="E20" s="49">
-        <v>2</v>
-      </c>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
+      <c r="D20" s="45">
+        <v>0</v>
+      </c>
+      <c r="E20" s="46">
+        <v>2</v>
+      </c>
+      <c r="F20" s="46">
+        <v>1</v>
+      </c>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
       <c r="K20" s="16">
-        <f>SUM(D20:J20)*50/A$1</f>
-        <v>100</v>
-      </c>
-      <c r="L20" s="14">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="L20" s="14"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
@@ -2679,8 +2718,8 @@
       <c r="W20" s="6"/>
       <c r="X20" s="44"/>
       <c r="Y20" s="21">
-        <f>K20*0.2+S20*0.25+V20*0.25+W20*0.3+X20*0.15</f>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2693,24 +2732,24 @@
       <c r="C21" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="48">
-        <v>0</v>
-      </c>
-      <c r="E21" s="49">
-        <v>2</v>
-      </c>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
+      <c r="D21" s="45">
+        <v>0</v>
+      </c>
+      <c r="E21" s="46">
+        <v>2</v>
+      </c>
+      <c r="F21" s="46">
+        <v>2</v>
+      </c>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
       <c r="K21" s="16">
-        <f>SUM(D21:J21)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L21" s="14">
-        <v>0</v>
-      </c>
+      <c r="L21" s="14"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
@@ -2727,7 +2766,7 @@
       <c r="W21" s="6"/>
       <c r="X21" s="44"/>
       <c r="Y21" s="21">
-        <f>K21*0.2+S21*0.25+V21*0.25+W21*0.3+X21*0.15</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
@@ -2741,24 +2780,24 @@
       <c r="C22" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="48">
-        <v>0</v>
-      </c>
-      <c r="E22" s="48">
-        <v>2</v>
-      </c>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
+      <c r="D22" s="45">
+        <v>0</v>
+      </c>
+      <c r="E22" s="45">
+        <v>2</v>
+      </c>
+      <c r="F22" s="46">
+        <v>2</v>
+      </c>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
       <c r="K22" s="16">
-        <f>SUM(D22:J22)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L22" s="14">
-        <v>0</v>
-      </c>
+      <c r="L22" s="14"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
@@ -2775,7 +2814,7 @@
       <c r="W22" s="6"/>
       <c r="X22" s="44"/>
       <c r="Y22" s="21">
-        <f>K22*0.2+S22*0.25+V22*0.25+W22*0.3+X22*0.15</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
@@ -2789,15 +2828,15 @@
       <c r="C23" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="48"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
       <c r="K23" s="16">
-        <f>SUM(D23:J23)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L23" s="14"/>
@@ -2814,7 +2853,7 @@
       <c r="W23" s="6"/>
       <c r="X23" s="44"/>
       <c r="Y23" s="21">
-        <f>K23*0.2+S23*0.25+V23*0.25+W23*0.3+X23*0.15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2828,15 +2867,15 @@
       <c r="C24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
       <c r="K24" s="16">
-        <f>SUM(D24:J24)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L24" s="14"/>
@@ -2853,7 +2892,7 @@
       <c r="W24" s="6"/>
       <c r="X24" s="44"/>
       <c r="Y24" s="21">
-        <f>K24*0.2+S24*0.25+V24*0.25+W24*0.3+X24*0.15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2867,15 +2906,15 @@
       <c r="C25" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
       <c r="K25" s="16">
-        <f>SUM(D25:J25)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L25" s="14"/>
@@ -2892,7 +2931,7 @@
       <c r="W25" s="6"/>
       <c r="X25" s="44"/>
       <c r="Y25" s="21">
-        <f>K25*0.2+S25*0.25+V25*0.25+W25*0.3+X25*0.15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2906,15 +2945,15 @@
       <c r="C26" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
       <c r="K26" s="16">
-        <f>SUM(D26:J26)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L26" s="14"/>
@@ -2931,7 +2970,7 @@
       <c r="W26" s="6"/>
       <c r="X26" s="44"/>
       <c r="Y26" s="21">
-        <f>K26*0.2+S26*0.25+V26*0.25+W26*0.3+X26*0.15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2945,15 +2984,15 @@
       <c r="C27" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
       <c r="K27" s="16">
-        <f>SUM(D27:J27)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L27" s="14"/>
@@ -2970,7 +3009,7 @@
       <c r="W27" s="6"/>
       <c r="X27" s="44"/>
       <c r="Y27" s="21">
-        <f>K27*0.2+S27*0.25+V27*0.25+W27*0.3+X27*0.15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2984,15 +3023,15 @@
       <c r="C28" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D28" s="48"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
       <c r="K28" s="16">
-        <f>SUM(D28:J28)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L28" s="14"/>
@@ -3009,7 +3048,7 @@
       <c r="W28" s="6"/>
       <c r="X28" s="44"/>
       <c r="Y28" s="21">
-        <f>K28*0.2+S28*0.25+V28*0.25+W28*0.3+X28*0.15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3023,15 +3062,15 @@
       <c r="C29" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="D29" s="48"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
       <c r="K29" s="16">
-        <f>SUM(D29:J29)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L29" s="14"/>
@@ -3048,7 +3087,7 @@
       <c r="W29" s="6"/>
       <c r="X29" s="44"/>
       <c r="Y29" s="21">
-        <f>K29*0.2+S29*0.25+V29*0.25+W29*0.3+X29*0.15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3062,16 +3101,18 @@
       <c r="C30" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D30" s="48"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46">
+        <v>1.5</v>
+      </c>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
       <c r="K30" s="16">
-        <f>SUM(D30:J30)*50/A$1</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>37.5</v>
       </c>
       <c r="L30" s="14"/>
       <c r="M30" s="6"/>
@@ -3087,8 +3128,8 @@
       <c r="W30" s="6"/>
       <c r="X30" s="44"/>
       <c r="Y30" s="21">
-        <f>K30*0.2+S30*0.25+V30*0.25+W30*0.3+X30*0.15</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>7.5</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3101,24 +3142,22 @@
       <c r="C31" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="48">
-        <v>0</v>
-      </c>
-      <c r="E31" s="49">
-        <v>0</v>
-      </c>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
+      <c r="D31" s="45">
+        <v>0</v>
+      </c>
+      <c r="E31" s="46">
+        <v>0</v>
+      </c>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
       <c r="K31" s="16">
-        <f>SUM(D31:J31)*50/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="L31" s="14">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="14"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
@@ -3126,7 +3165,7 @@
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
       <c r="S31" s="16">
-        <f>SUM(L31:R31)/A$1</f>
+        <f t="shared" ref="S31:S44" si="4">SUM(L31:R31)/A$1</f>
         <v>0</v>
       </c>
       <c r="T31" s="14"/>
@@ -3135,7 +3174,7 @@
       <c r="W31" s="6"/>
       <c r="X31" s="44"/>
       <c r="Y31" s="21">
-        <f>K31*0.2+S31*0.25+V31*0.25+W31*0.3+X31*0.15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3149,24 +3188,22 @@
       <c r="C32" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="48">
-        <v>0</v>
-      </c>
-      <c r="E32" s="49">
-        <v>0</v>
-      </c>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
+      <c r="D32" s="45">
+        <v>0</v>
+      </c>
+      <c r="E32" s="46">
+        <v>0</v>
+      </c>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
       <c r="K32" s="16">
-        <f>SUM(D32:J32)*50/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="L32" s="14">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="14"/>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
@@ -3174,7 +3211,7 @@
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
       <c r="S32" s="16">
-        <f>SUM(L32:R32)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T32" s="14"/>
@@ -3183,7 +3220,7 @@
       <c r="W32" s="6"/>
       <c r="X32" s="44"/>
       <c r="Y32" s="21">
-        <f>K32*0.2+S32*0.25+V32*0.25+W32*0.3+X32*0.15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3197,24 +3234,22 @@
       <c r="C33" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="D33" s="48">
-        <v>0</v>
-      </c>
-      <c r="E33" s="49">
-        <v>0</v>
-      </c>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
+      <c r="D33" s="45">
+        <v>0</v>
+      </c>
+      <c r="E33" s="46">
+        <v>0</v>
+      </c>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
       <c r="K33" s="16">
-        <f>SUM(D33:J33)*50/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="L33" s="14">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="14"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
@@ -3222,7 +3257,7 @@
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
       <c r="S33" s="16">
-        <f>SUM(L33:R33)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T33" s="14"/>
@@ -3231,7 +3266,7 @@
       <c r="W33" s="6"/>
       <c r="X33" s="44"/>
       <c r="Y33" s="21">
-        <f>K33*0.2+S33*0.25+V33*0.25+W33*0.3+X33*0.15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3245,24 +3280,22 @@
       <c r="C34" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="D34" s="48">
-        <v>0</v>
-      </c>
-      <c r="E34" s="49">
-        <v>0</v>
-      </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="49"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="49"/>
+      <c r="D34" s="45">
+        <v>0</v>
+      </c>
+      <c r="E34" s="46">
+        <v>0</v>
+      </c>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
       <c r="K34" s="16">
-        <f>SUM(D34:J34)*50/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="14">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="14"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
@@ -3270,7 +3303,7 @@
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
       <c r="S34" s="16">
-        <f>SUM(L34:R34)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T34" s="14"/>
@@ -3279,7 +3312,7 @@
       <c r="W34" s="6"/>
       <c r="X34" s="44"/>
       <c r="Y34" s="21">
-        <f>K34*0.2+S34*0.25+V34*0.25+W34*0.3+X34*0.1</f>
+        <f t="shared" ref="Y34:Y55" si="5">K34*0.2+S34*0.25+V34*0.25+W34*0.3+X34*0.1</f>
         <v>0</v>
       </c>
     </row>
@@ -3293,24 +3326,22 @@
       <c r="C35" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="48">
-        <v>0</v>
-      </c>
-      <c r="E35" s="49">
-        <v>0</v>
-      </c>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
+      <c r="D35" s="45">
+        <v>0</v>
+      </c>
+      <c r="E35" s="46">
+        <v>0</v>
+      </c>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
       <c r="K35" s="16">
-        <f>SUM(D35:J35)*50/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="L35" s="14">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L35" s="14"/>
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
@@ -3318,7 +3349,7 @@
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
       <c r="S35" s="16">
-        <f>SUM(L35:R35)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T35" s="14"/>
@@ -3327,7 +3358,7 @@
       <c r="W35" s="6"/>
       <c r="X35" s="44"/>
       <c r="Y35" s="21">
-        <f>K35*0.2+S35*0.25+V35*0.25+W35*0.3+X35*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3341,24 +3372,22 @@
       <c r="C36" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="48">
-        <v>0</v>
-      </c>
-      <c r="E36" s="49">
-        <v>0</v>
-      </c>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
+      <c r="D36" s="45">
+        <v>0</v>
+      </c>
+      <c r="E36" s="46">
+        <v>0</v>
+      </c>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
       <c r="K36" s="16">
-        <f>SUM(D36:J36)*50/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="L36" s="14">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="14"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
@@ -3366,7 +3395,7 @@
       <c r="Q36" s="6"/>
       <c r="R36" s="6"/>
       <c r="S36" s="16">
-        <f>SUM(L36:R36)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T36" s="14"/>
@@ -3375,7 +3404,7 @@
       <c r="W36" s="6"/>
       <c r="X36" s="44"/>
       <c r="Y36" s="21">
-        <f>K36*0.2+S36*0.25+V36*0.25+W36*0.3+X36*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3395,18 +3424,18 @@
       <c r="E37" s="7">
         <v>0</v>
       </c>
-      <c r="F37" s="7"/>
+      <c r="F37" s="7">
+        <v>2</v>
+      </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="16">
-        <f>SUM(D37:J37)*50/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="L37" s="14">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="L37" s="14"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
@@ -3414,7 +3443,7 @@
       <c r="Q37" s="6"/>
       <c r="R37" s="6"/>
       <c r="S37" s="16">
-        <f>SUM(L37:R37)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T37" s="14"/>
@@ -3423,8 +3452,8 @@
       <c r="W37" s="6"/>
       <c r="X37" s="44"/>
       <c r="Y37" s="21">
-        <f>K37*0.2+S37*0.25+V37*0.25+W37*0.3+X37*0.1</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3443,18 +3472,18 @@
       <c r="E38" s="7">
         <v>2</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F38" s="7">
+        <v>2</v>
+      </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="16">
-        <f>SUM(D38:J38)*50/A$1</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L38" s="14">
-        <v>0</v>
-      </c>
+      <c r="L38" s="14"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
@@ -3462,7 +3491,7 @@
       <c r="Q38" s="6"/>
       <c r="R38" s="6"/>
       <c r="S38" s="16">
-        <f>SUM(L38:R38)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T38" s="14"/>
@@ -3471,7 +3500,7 @@
       <c r="W38" s="6"/>
       <c r="X38" s="44"/>
       <c r="Y38" s="21">
-        <f>K38*0.2+S38*0.25+V38*0.25+W38*0.3+X38*0.1</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
@@ -3497,12 +3526,10 @@
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
       <c r="K39" s="16">
-        <f>SUM(D39:J39)*50/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="L39" s="14">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L39" s="14"/>
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
@@ -3510,7 +3537,7 @@
       <c r="Q39" s="6"/>
       <c r="R39" s="6"/>
       <c r="S39" s="16">
-        <f>SUM(L39:R39)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T39" s="14"/>
@@ -3519,7 +3546,7 @@
       <c r="W39" s="6"/>
       <c r="X39" s="44"/>
       <c r="Y39" s="21">
-        <f>K39*0.2+S39*0.25+V39*0.25+W39*0.3+X39*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3545,12 +3572,10 @@
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
       <c r="K40" s="16">
-        <f>SUM(D40:J40)*50/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="L40" s="14">
-        <v>0</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L40" s="14"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
@@ -3558,7 +3583,7 @@
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
       <c r="S40" s="16">
-        <f>SUM(L40:R40)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T40" s="14"/>
@@ -3567,17 +3592,29 @@
       <c r="W40" s="6"/>
       <c r="X40" s="44"/>
       <c r="Y40" s="21">
-        <f>K40*0.2+S40*0.25+V40*0.25+W40*0.3+X40*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="A41" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="12">
+        <v>0</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0</v>
+      </c>
+      <c r="F41" s="7">
+        <v>2</v>
+      </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
@@ -3591,7 +3628,7 @@
       <c r="Q41" s="6"/>
       <c r="R41" s="6"/>
       <c r="S41" s="16">
-        <f>SUM(L41:R41)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T41" s="14"/>
@@ -3600,7 +3637,7 @@
       <c r="W41" s="6"/>
       <c r="X41" s="44"/>
       <c r="Y41" s="21">
-        <f>K41*0.2+S41*0.25+V41*0.25+W41*0.3+X41*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3624,7 +3661,7 @@
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
       <c r="S42" s="16">
-        <f>SUM(L42:R42)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T42" s="14"/>
@@ -3633,7 +3670,7 @@
       <c r="W42" s="6"/>
       <c r="X42" s="44"/>
       <c r="Y42" s="21">
-        <f>K42*0.2+S42*0.25+V42*0.25+W42*0.3+X42*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3657,7 +3694,7 @@
       <c r="Q43" s="6"/>
       <c r="R43" s="6"/>
       <c r="S43" s="16">
-        <f>SUM(L43:R43)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T43" s="14"/>
@@ -3666,7 +3703,7 @@
       <c r="W43" s="6"/>
       <c r="X43" s="44"/>
       <c r="Y43" s="21">
-        <f>K43*0.2+S43*0.25+V43*0.25+W43*0.3+X43*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3690,7 +3727,7 @@
       <c r="Q44" s="6"/>
       <c r="R44" s="6"/>
       <c r="S44" s="16">
-        <f>SUM(L44:R44)/A$1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T44" s="14"/>
@@ -3699,7 +3736,7 @@
       <c r="W44" s="6"/>
       <c r="X44" s="44"/>
       <c r="Y44" s="21">
-        <f>K44*0.2+S44*0.25+V44*0.25+W44*0.3+X44*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3729,7 +3766,7 @@
       <c r="W45" s="6"/>
       <c r="X45" s="44"/>
       <c r="Y45" s="21">
-        <f>K45*0.2+S45*0.25+V45*0.25+W45*0.3+X45*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3759,7 +3796,7 @@
       <c r="W46" s="6"/>
       <c r="X46" s="44"/>
       <c r="Y46" s="21">
-        <f>K46*0.2+S46*0.25+V46*0.25+W46*0.3+X46*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3789,7 +3826,7 @@
       <c r="W47" s="6"/>
       <c r="X47" s="44"/>
       <c r="Y47" s="21">
-        <f>K47*0.2+S47*0.25+V47*0.25+W47*0.3+X47*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3819,7 +3856,7 @@
       <c r="W48" s="6"/>
       <c r="X48" s="44"/>
       <c r="Y48" s="21">
-        <f>K48*0.2+S48*0.25+V48*0.25+W48*0.3+X48*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3849,7 +3886,7 @@
       <c r="W49" s="6"/>
       <c r="X49" s="44"/>
       <c r="Y49" s="21">
-        <f>K49*0.2+S49*0.25+V49*0.25+W49*0.3+X49*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3879,7 +3916,7 @@
       <c r="W50" s="6"/>
       <c r="X50" s="44"/>
       <c r="Y50" s="21">
-        <f>K50*0.2+S50*0.25+V50*0.25+W50*0.3+X50*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3909,7 +3946,7 @@
       <c r="W51" s="6"/>
       <c r="X51" s="44"/>
       <c r="Y51" s="21">
-        <f>K51*0.2+S51*0.25+V51*0.25+W51*0.3+X51*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3939,7 +3976,7 @@
       <c r="W52" s="6"/>
       <c r="X52" s="44"/>
       <c r="Y52" s="21">
-        <f>K52*0.2+S52*0.25+V52*0.25+W52*0.3+X52*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3969,7 +4006,7 @@
       <c r="W53" s="6"/>
       <c r="X53" s="44"/>
       <c r="Y53" s="21">
-        <f>K53*0.2+S53*0.25+V53*0.25+W53*0.3+X53*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3999,7 +4036,7 @@
       <c r="W54" s="6"/>
       <c r="X54" s="44"/>
       <c r="Y54" s="21">
-        <f>K54*0.2+S54*0.25+V54*0.25+W54*0.3+X54*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4029,7 +4066,7 @@
       <c r="W55" s="6"/>
       <c r="X55" s="44"/>
       <c r="Y55" s="21">
-        <f>K55*0.2+S55*0.25+V55*0.25+W55*0.3+X55*0.1</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4547,47 +4584,47 @@
     <mergeCell ref="L1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:J55">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="19" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:R55 W3:X55">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:U55">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="between">
       <formula>80</formula>
       <formula>200</formula>
     </cfRule>
@@ -4741,22 +4778,22 @@
       <c r="B1" s="18"/>
       <c r="C1" s="34"/>
       <c r="D1" s="40"/>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="45" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="47"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="49"/>
       <c r="Q1" s="33" t="s">
         <v>107</v>
       </c>
@@ -7673,14 +7710,14 @@
     <mergeCell ref="K1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:I33">
-    <cfRule type="cellIs" dxfId="10" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="25" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7727,18 +7764,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:O33">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
@@ -7786,18 +7823,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q33">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThanOrEqual">
       <formula>80</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Yaz. Arac. Hafta 4 guncelleme
</commit_message>
<xml_diff>
--- a/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
+++ b/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
@@ -657,7 +657,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0_);\(0.0\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,6 +694,18 @@
     <font>
       <sz val="8"/>
       <color indexed="81"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -1041,7 +1053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1127,15 +1139,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1175,117 +1178,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1783,7 +1714,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
+      <selection pane="bottomLeft" activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1791,12 +1722,11 @@
     <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="3.21875" style="59" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.88671875" style="59" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.44140625" style="59" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="2.44140625" style="60" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.44140625" style="60" customWidth="1"/>
-    <col min="11" max="11" width="2.88671875" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="3.21875" style="56" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="2.88671875" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="2.44140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.44140625" style="57" customWidth="1"/>
+    <col min="11" max="11" width="2.88671875" style="48" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.88671875" style="1" customWidth="1"/>
     <col min="13" max="13" width="3.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
@@ -1816,30 +1746,30 @@
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="29"/>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="45" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="45" t="s">
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="T1" s="46"/>
-      <c r="U1" s="47"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="60"/>
       <c r="V1" s="17" t="s">
         <v>96</v>
       </c>
@@ -1860,28 +1790,28 @@
       <c r="C2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="52">
+      <c r="D2" s="49">
         <v>1</v>
       </c>
-      <c r="E2" s="53">
-        <v>2</v>
-      </c>
-      <c r="F2" s="53">
+      <c r="E2" s="50">
+        <v>2</v>
+      </c>
+      <c r="F2" s="50">
         <v>3</v>
       </c>
-      <c r="G2" s="53">
+      <c r="G2" s="50">
         <v>4</v>
       </c>
-      <c r="H2" s="53">
+      <c r="H2" s="50">
         <v>5</v>
       </c>
-      <c r="I2" s="53">
+      <c r="I2" s="50">
         <v>6</v>
       </c>
-      <c r="J2" s="53">
+      <c r="J2" s="50">
         <v>7</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="K2" s="45" t="s">
         <v>192</v>
       </c>
       <c r="L2" s="28" t="s">
@@ -1926,33 +1856,35 @@
     </row>
     <row r="3" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>109</v>
+        <v>148</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D3" s="54">
-        <v>2</v>
-      </c>
-      <c r="E3" s="55">
-        <v>2</v>
-      </c>
-      <c r="F3" s="55">
-        <v>2</v>
-      </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="49">
-        <v>0</v>
+        <v>149</v>
+      </c>
+      <c r="D3" s="51">
+        <v>2</v>
+      </c>
+      <c r="E3" s="52">
+        <v>2</v>
+      </c>
+      <c r="F3" s="52">
+        <v>2</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="46">
+        <v>1</v>
       </c>
       <c r="L3" s="16">
         <f>SUM(D3:J3)*50/(A$1-K3)</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="M3" s="14">
         <v>100</v>
@@ -1971,39 +1903,41 @@
       <c r="V3" s="6"/>
       <c r="W3" s="44"/>
       <c r="X3" s="21">
-        <f>L3*0.2+R3*0.25+U3*0.25+V3*0.3+W3*0.1</f>
-        <v>28.333333333333336</v>
+        <f>L3*0.2+R3*0.25+U3*0.25+V3*0.3+W3*0.15</f>
+        <v>38.333333333333336</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>189</v>
+        <v>109</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="54">
-        <v>2</v>
-      </c>
-      <c r="E4" s="56">
-        <v>2</v>
-      </c>
-      <c r="F4" s="55">
-        <v>2</v>
-      </c>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="49">
+        <v>177</v>
+      </c>
+      <c r="D4" s="51">
+        <v>2</v>
+      </c>
+      <c r="E4" s="52">
+        <v>2</v>
+      </c>
+      <c r="F4" s="52">
+        <v>2</v>
+      </c>
+      <c r="G4" s="52">
+        <v>2</v>
+      </c>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="46">
         <v>0</v>
       </c>
       <c r="L4" s="16">
-        <f t="shared" ref="L4:L41" si="0">SUM(D4:J4)*50/(A$1-K4)</f>
-        <v>100</v>
+        <f>SUM(D4:J4)*50/(A$1-K4)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="M4" s="14">
         <v>100</v>
@@ -2023,41 +1957,43 @@
       <c r="W4" s="44"/>
       <c r="X4" s="21">
         <f>L4*0.2+R4*0.25+U4*0.25+V4*0.3+W4*0.1</f>
-        <v>28.333333333333336</v>
+        <v>35.000000000000007</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="54">
-        <v>2</v>
-      </c>
-      <c r="E5" s="55">
-        <v>2</v>
-      </c>
-      <c r="F5" s="55">
-        <v>2</v>
-      </c>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="49">
+        <v>118</v>
+      </c>
+      <c r="D5" s="51">
+        <v>2</v>
+      </c>
+      <c r="E5" s="52">
+        <v>2</v>
+      </c>
+      <c r="F5" s="52">
+        <v>2</v>
+      </c>
+      <c r="G5" s="52">
+        <v>2</v>
+      </c>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="46">
         <v>0</v>
       </c>
       <c r="L5" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D5:J5)*50/(A$1-K5)</f>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="M5" s="14">
         <v>100</v>
-      </c>
-      <c r="M5" s="14">
-        <v>95</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
@@ -2065,7 +2001,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="16">
         <f>SUM(M5:Q5)/A$1</f>
-        <v>31.666666666666668</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="S5" s="14"/>
       <c r="T5" s="14"/>
@@ -2074,41 +2010,43 @@
       <c r="W5" s="44"/>
       <c r="X5" s="21">
         <f>L5*0.2+R5*0.25+U5*0.25+V5*0.3+W5*0.15</f>
-        <v>27.916666666666668</v>
+        <v>35.000000000000007</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>170</v>
+        <v>111</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="D6" s="54">
-        <v>2</v>
-      </c>
-      <c r="E6" s="55">
-        <v>2</v>
-      </c>
-      <c r="F6" s="55">
-        <v>2</v>
-      </c>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="49">
+        <v>110</v>
+      </c>
+      <c r="D6" s="51">
+        <v>2</v>
+      </c>
+      <c r="E6" s="52">
+        <v>2</v>
+      </c>
+      <c r="F6" s="52">
+        <v>2</v>
+      </c>
+      <c r="G6" s="52">
+        <v>2</v>
+      </c>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="46">
         <v>0</v>
       </c>
       <c r="L6" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D6:J6)*50/(A$1-K6)</f>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="M6" s="14">
         <v>100</v>
-      </c>
-      <c r="M6" s="14">
-        <v>85</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -2116,7 +2054,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="16">
         <f>SUM(M6:Q6)/A$1</f>
-        <v>28.333333333333332</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="S6" s="14"/>
       <c r="T6" s="14"/>
@@ -2124,42 +2062,44 @@
       <c r="V6" s="6"/>
       <c r="W6" s="44"/>
       <c r="X6" s="21">
-        <f>L6*0.2+R6*0.25+U6*0.25+V6*0.3+W6*0.1</f>
-        <v>27.083333333333332</v>
+        <f>L6*0.2+R6*0.25+U6*0.25+V6*0.3+W6*0.15</f>
+        <v>35.000000000000007</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>173</v>
+        <v>114</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>179</v>
+        <v>112</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="D7" s="54">
-        <v>2</v>
-      </c>
-      <c r="E7" s="55">
-        <v>2</v>
-      </c>
-      <c r="F7" s="55">
-        <v>2</v>
-      </c>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="49">
+        <v>113</v>
+      </c>
+      <c r="D7" s="51">
+        <v>2</v>
+      </c>
+      <c r="E7" s="52">
+        <v>2</v>
+      </c>
+      <c r="F7" s="52">
+        <v>2</v>
+      </c>
+      <c r="G7" s="52">
+        <v>2</v>
+      </c>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="46">
         <v>0</v>
       </c>
       <c r="L7" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D7:J7)*50/(A$1-K7)</f>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="M7" s="14">
         <v>100</v>
-      </c>
-      <c r="M7" s="14">
-        <v>85</v>
       </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
@@ -2167,7 +2107,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="16">
         <f>SUM(M7:Q7)/A$1</f>
-        <v>28.333333333333332</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="S7" s="14"/>
       <c r="T7" s="14"/>
@@ -2175,42 +2115,44 @@
       <c r="V7" s="6"/>
       <c r="W7" s="44"/>
       <c r="X7" s="21">
-        <f>L7*0.2+R7*0.25+U7*0.25+V7*0.3+W7*0.1</f>
-        <v>27.083333333333332</v>
+        <f>L7*0.2+R7*0.25+U7*0.25+V7*0.3+W7*0.15</f>
+        <v>35.000000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D8" s="54">
-        <v>2</v>
-      </c>
-      <c r="E8" s="55">
-        <v>2</v>
-      </c>
-      <c r="F8" s="55">
-        <v>2</v>
-      </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="49">
+        <v>160</v>
+      </c>
+      <c r="D8" s="51">
+        <v>2</v>
+      </c>
+      <c r="E8" s="52">
+        <v>2</v>
+      </c>
+      <c r="F8" s="52">
+        <v>2</v>
+      </c>
+      <c r="G8" s="52">
+        <v>2</v>
+      </c>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="46">
         <v>0</v>
       </c>
       <c r="L8" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D8:J8)*50/(A$1-K8)</f>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="M8" s="14">
         <v>100</v>
-      </c>
-      <c r="M8" s="14">
-        <v>80</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -2218,7 +2160,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="16">
         <f>SUM(M8:Q8)/A$1</f>
-        <v>26.666666666666668</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="S8" s="14"/>
       <c r="T8" s="14"/>
@@ -2227,38 +2169,40 @@
       <c r="W8" s="44"/>
       <c r="X8" s="21">
         <f>L8*0.2+R8*0.25+U8*0.25+V8*0.3+W8*0.1</f>
-        <v>26.666666666666668</v>
+        <v>35.000000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="54">
-        <v>0</v>
-      </c>
-      <c r="E9" s="55">
-        <v>2</v>
-      </c>
-      <c r="F9" s="55">
-        <v>2</v>
-      </c>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="49">
+        <v>163</v>
+      </c>
+      <c r="D9" s="51">
+        <v>2</v>
+      </c>
+      <c r="E9" s="52">
+        <v>2</v>
+      </c>
+      <c r="F9" s="52">
+        <v>2</v>
+      </c>
+      <c r="G9" s="52">
+        <v>2</v>
+      </c>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="46">
         <v>0</v>
       </c>
       <c r="L9" s="16">
-        <f t="shared" si="0"/>
-        <v>66.666666666666671</v>
+        <f>SUM(D9:J9)*50/(A$1-K9)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="M9" s="14">
         <v>100</v>
@@ -2277,39 +2221,41 @@
       <c r="V9" s="6"/>
       <c r="W9" s="44"/>
       <c r="X9" s="21">
-        <f>L9*0.2+R9*0.25+U9*0.25+V9*0.3+W9*0.15</f>
-        <v>21.666666666666671</v>
+        <f>L9*0.2+R9*0.25+U9*0.25+V9*0.3+W9*0.1</f>
+        <v>35.000000000000007</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="54">
-        <v>0</v>
-      </c>
-      <c r="E10" s="55">
-        <v>2</v>
-      </c>
-      <c r="F10" s="55">
-        <v>2</v>
-      </c>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="49">
+        <v>166</v>
+      </c>
+      <c r="D10" s="51">
+        <v>2</v>
+      </c>
+      <c r="E10" s="52">
+        <v>2</v>
+      </c>
+      <c r="F10" s="52">
+        <v>2</v>
+      </c>
+      <c r="G10" s="52">
+        <v>2</v>
+      </c>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="46">
         <v>0</v>
       </c>
       <c r="L10" s="16">
-        <f t="shared" si="0"/>
-        <v>66.666666666666671</v>
+        <f>SUM(D10:J10)*50/(A$1-K10)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="M10" s="14">
         <v>100</v>
@@ -2328,42 +2274,44 @@
       <c r="V10" s="6"/>
       <c r="W10" s="44"/>
       <c r="X10" s="21">
-        <f>L10*0.2+R10*0.25+U10*0.25+V10*0.3+W10*0.15</f>
-        <v>21.666666666666671</v>
+        <f>L10*0.2+R10*0.25+U10*0.25+V10*0.3+W10*0.1</f>
+        <v>35.000000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>151</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="54">
-        <v>0</v>
-      </c>
-      <c r="E11" s="55">
-        <v>2</v>
-      </c>
-      <c r="F11" s="55">
-        <v>2</v>
-      </c>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="49">
+        <v>152</v>
+      </c>
+      <c r="D11" s="51">
+        <v>2</v>
+      </c>
+      <c r="E11" s="52">
+        <v>2</v>
+      </c>
+      <c r="F11" s="52">
+        <v>2</v>
+      </c>
+      <c r="G11" s="52">
+        <v>2</v>
+      </c>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="46">
         <v>0</v>
       </c>
       <c r="L11" s="16">
-        <f t="shared" si="0"/>
-        <v>66.666666666666671</v>
+        <f>SUM(D11:J11)*50/(A$1-K11)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="M11" s="14">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
@@ -2371,7 +2319,7 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="16">
         <f>SUM(M11:Q11)/A$1</f>
-        <v>33.333333333333336</v>
+        <v>31.666666666666668</v>
       </c>
       <c r="S11" s="14"/>
       <c r="T11" s="14"/>
@@ -2380,41 +2328,43 @@
       <c r="W11" s="44"/>
       <c r="X11" s="21">
         <f>L11*0.2+R11*0.25+U11*0.25+V11*0.3+W11*0.15</f>
-        <v>21.666666666666671</v>
+        <v>34.583333333333336</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" s="54">
-        <v>0</v>
-      </c>
-      <c r="E12" s="55">
-        <v>2</v>
-      </c>
-      <c r="F12" s="55">
-        <v>2</v>
-      </c>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="49">
+        <v>172</v>
+      </c>
+      <c r="D12" s="51">
+        <v>2</v>
+      </c>
+      <c r="E12" s="52">
+        <v>2</v>
+      </c>
+      <c r="F12" s="52">
+        <v>2</v>
+      </c>
+      <c r="G12" s="52">
+        <v>2</v>
+      </c>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="46">
         <v>0</v>
       </c>
       <c r="L12" s="16">
-        <f t="shared" si="0"/>
-        <v>66.666666666666671</v>
+        <f>SUM(D12:J12)*50/(A$1-K12)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="M12" s="14">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
@@ -2422,7 +2372,7 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="16">
         <f>SUM(M12:Q12)/A$1</f>
-        <v>33.333333333333336</v>
+        <v>28.333333333333332</v>
       </c>
       <c r="S12" s="14"/>
       <c r="T12" s="14"/>
@@ -2430,42 +2380,44 @@
       <c r="V12" s="6"/>
       <c r="W12" s="44"/>
       <c r="X12" s="21">
-        <f>L12*0.2+R12*0.25+U12*0.25+V12*0.3+W12*0.15</f>
-        <v>21.666666666666671</v>
+        <f>L12*0.2+R12*0.25+U12*0.25+V12*0.3+W12*0.1</f>
+        <v>33.750000000000007</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>116</v>
+        <v>173</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="54">
-        <v>2</v>
-      </c>
-      <c r="E13" s="55">
-        <v>2</v>
-      </c>
-      <c r="F13" s="55">
-        <v>2</v>
-      </c>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="49">
+        <v>180</v>
+      </c>
+      <c r="D13" s="51">
+        <v>2</v>
+      </c>
+      <c r="E13" s="52">
+        <v>2</v>
+      </c>
+      <c r="F13" s="52">
+        <v>2</v>
+      </c>
+      <c r="G13" s="52">
+        <v>2</v>
+      </c>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="46">
         <v>0</v>
       </c>
       <c r="L13" s="16">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>SUM(D13:J13)*50/(A$1-K13)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="M13" s="14">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
@@ -2473,7 +2425,7 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="16">
         <f>SUM(M13:Q13)/A$1</f>
-        <v>33.333333333333336</v>
+        <v>28.333333333333332</v>
       </c>
       <c r="S13" s="14"/>
       <c r="T13" s="14"/>
@@ -2481,44 +2433,44 @@
       <c r="V13" s="6"/>
       <c r="W13" s="44"/>
       <c r="X13" s="21">
-        <f>L13*0.2+R13*0.25+U13*0.25+V13*0.3+W13*0.15</f>
-        <v>28.333333333333336</v>
+        <f>L13*0.2+R13*0.25+U13*0.25+V13*0.3+W13*0.1</f>
+        <v>33.750000000000007</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D14" s="54">
-        <v>2</v>
-      </c>
-      <c r="E14" s="55">
-        <v>2</v>
-      </c>
-      <c r="F14" s="55">
-        <v>2</v>
-      </c>
-      <c r="G14" s="55" t="s">
-        <v>192</v>
-      </c>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="49">
-        <v>1</v>
+        <v>177</v>
+      </c>
+      <c r="D14" s="51">
+        <v>2</v>
+      </c>
+      <c r="E14" s="52">
+        <v>2</v>
+      </c>
+      <c r="F14" s="52">
+        <v>2</v>
+      </c>
+      <c r="G14" s="52">
+        <v>2</v>
+      </c>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="46">
+        <v>0</v>
       </c>
       <c r="L14" s="16">
-        <f t="shared" si="0"/>
-        <v>150</v>
+        <f>SUM(D14:J14)*50/(A$1-K14)</f>
+        <v>133.33333333333334</v>
       </c>
       <c r="M14" s="14">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
@@ -2526,7 +2478,7 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="16">
         <f>SUM(M14:Q14)/A$1</f>
-        <v>33.333333333333336</v>
+        <v>26.666666666666668</v>
       </c>
       <c r="S14" s="14"/>
       <c r="T14" s="14"/>
@@ -2534,39 +2486,41 @@
       <c r="V14" s="6"/>
       <c r="W14" s="44"/>
       <c r="X14" s="21">
-        <f>L14*0.2+R14*0.25+U14*0.25+V14*0.3+W14*0.15</f>
-        <v>38.333333333333336</v>
+        <f>L14*0.2+R14*0.25+U14*0.25+V14*0.3+W14*0.1</f>
+        <v>33.333333333333336</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>109</v>
+        <v>189</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" s="54">
-        <v>2</v>
-      </c>
-      <c r="E15" s="55">
-        <v>2</v>
-      </c>
-      <c r="F15" s="55">
-        <v>2</v>
-      </c>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="49">
+        <v>83</v>
+      </c>
+      <c r="D15" s="51">
+        <v>2</v>
+      </c>
+      <c r="E15" s="53">
+        <v>2</v>
+      </c>
+      <c r="F15" s="52">
+        <v>2</v>
+      </c>
+      <c r="G15" s="53">
+        <v>1.5</v>
+      </c>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="46">
         <v>0</v>
       </c>
       <c r="L15" s="16">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>SUM(D15:J15)*50/(A$1-K15)</f>
+        <v>125</v>
       </c>
       <c r="M15" s="14">
         <v>100</v>
@@ -2585,38 +2539,40 @@
       <c r="V15" s="6"/>
       <c r="W15" s="44"/>
       <c r="X15" s="21">
-        <f>L15*0.2+R15*0.25+U15*0.25+V15*0.3+W15*0.15</f>
-        <v>28.333333333333336</v>
+        <f>L15*0.2+R15*0.25+U15*0.25+V15*0.3+W15*0.1</f>
+        <v>33.333333333333336</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="54">
-        <v>2</v>
-      </c>
-      <c r="E16" s="55">
-        <v>2</v>
-      </c>
-      <c r="F16" s="55">
-        <v>2</v>
-      </c>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="49">
+        <v>121</v>
+      </c>
+      <c r="D16" s="51">
+        <v>0</v>
+      </c>
+      <c r="E16" s="52">
+        <v>2</v>
+      </c>
+      <c r="F16" s="52">
+        <v>2</v>
+      </c>
+      <c r="G16" s="52">
+        <v>2</v>
+      </c>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="46">
         <v>0</v>
       </c>
       <c r="L16" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D16:J16)*50/(A$1-K16)</f>
         <v>100</v>
       </c>
       <c r="M16" s="14">
@@ -2642,32 +2598,34 @@
     </row>
     <row r="17" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="D17" s="54">
-        <v>2</v>
-      </c>
-      <c r="E17" s="55">
-        <v>2</v>
-      </c>
-      <c r="F17" s="55">
-        <v>2</v>
-      </c>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="49">
+        <v>146</v>
+      </c>
+      <c r="D17" s="51">
+        <v>0</v>
+      </c>
+      <c r="E17" s="52">
+        <v>2</v>
+      </c>
+      <c r="F17" s="52">
+        <v>2</v>
+      </c>
+      <c r="G17" s="52">
+        <v>2</v>
+      </c>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="46">
         <v>0</v>
       </c>
       <c r="L17" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D17:J17)*50/(A$1-K17)</f>
         <v>100</v>
       </c>
       <c r="M17" s="14">
@@ -2687,38 +2645,40 @@
       <c r="V17" s="6"/>
       <c r="W17" s="44"/>
       <c r="X17" s="21">
-        <f>L17*0.2+R17*0.25+U17*0.25+V17*0.3+W17*0.1</f>
+        <f>L17*0.2+R17*0.25+U17*0.25+V17*0.3+W17*0.15</f>
         <v>28.333333333333336</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" s="54">
-        <v>2</v>
-      </c>
-      <c r="E18" s="55">
-        <v>2</v>
-      </c>
-      <c r="F18" s="55">
-        <v>2</v>
-      </c>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="49">
+        <v>123</v>
+      </c>
+      <c r="D18" s="51">
+        <v>0</v>
+      </c>
+      <c r="E18" s="52">
+        <v>2</v>
+      </c>
+      <c r="F18" s="52">
+        <v>2</v>
+      </c>
+      <c r="G18" s="52">
+        <v>2</v>
+      </c>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="46">
         <v>0</v>
       </c>
       <c r="L18" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D18:J18)*50/(A$1-K18)</f>
         <v>100</v>
       </c>
       <c r="M18" s="14">
@@ -2738,38 +2698,40 @@
       <c r="V18" s="6"/>
       <c r="W18" s="44"/>
       <c r="X18" s="21">
-        <f>L18*0.2+R18*0.25+U18*0.25+V18*0.3+W18*0.1</f>
+        <f>L18*0.2+R18*0.25+U18*0.25+V18*0.3+W18*0.15</f>
         <v>28.333333333333336</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="54">
-        <v>2</v>
-      </c>
-      <c r="E19" s="55">
-        <v>2</v>
-      </c>
-      <c r="F19" s="55">
-        <v>2</v>
-      </c>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="49">
+        <v>98</v>
+      </c>
+      <c r="D19" s="51">
+        <v>0</v>
+      </c>
+      <c r="E19" s="52">
+        <v>2</v>
+      </c>
+      <c r="F19" s="52">
+        <v>2</v>
+      </c>
+      <c r="G19" s="52">
+        <v>2</v>
+      </c>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="46">
         <v>0</v>
       </c>
       <c r="L19" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D19:J19)*50/(A$1-K19)</f>
         <v>100</v>
       </c>
       <c r="M19" s="14">
@@ -2789,7 +2751,7 @@
       <c r="V19" s="6"/>
       <c r="W19" s="44"/>
       <c r="X19" s="21">
-        <f>L19*0.2+R19*0.25+U19*0.25+V19*0.3+W19*0.1</f>
+        <f>L19*0.2+R19*0.25+U19*0.25+V19*0.3+W19*0.15</f>
         <v>28.333333333333336</v>
       </c>
     </row>
@@ -2803,25 +2765,27 @@
       <c r="C20" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="57">
-        <v>0</v>
-      </c>
-      <c r="E20" s="56">
-        <v>2</v>
-      </c>
-      <c r="F20" s="56">
-        <v>2</v>
-      </c>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="49">
+      <c r="D20" s="54">
+        <v>0</v>
+      </c>
+      <c r="E20" s="53">
+        <v>2</v>
+      </c>
+      <c r="F20" s="53">
+        <v>2</v>
+      </c>
+      <c r="G20" s="53">
+        <v>2</v>
+      </c>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="46">
         <v>0</v>
       </c>
       <c r="L20" s="16">
-        <f t="shared" si="0"/>
-        <v>66.666666666666671</v>
+        <f>SUM(D20:J20)*50/(A$1-K20)</f>
+        <v>100</v>
       </c>
       <c r="M20" s="14">
         <v>80</v>
@@ -2841,41 +2805,43 @@
       <c r="W20" s="44"/>
       <c r="X20" s="21">
         <f>L20*0.2+R20*0.25+U20*0.25+V20*0.3+W20*0.1</f>
-        <v>20.000000000000004</v>
+        <v>26.666666666666668</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="54">
-        <v>0</v>
-      </c>
-      <c r="E21" s="55">
-        <v>2</v>
-      </c>
-      <c r="F21" s="55">
-        <v>1</v>
-      </c>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="49">
+        <v>131</v>
+      </c>
+      <c r="D21" s="51">
+        <v>0</v>
+      </c>
+      <c r="E21" s="52">
+        <v>2</v>
+      </c>
+      <c r="F21" s="52">
+        <v>2</v>
+      </c>
+      <c r="G21" s="52">
+        <v>1.2</v>
+      </c>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="46">
         <v>0</v>
       </c>
       <c r="L21" s="16">
-        <f t="shared" si="0"/>
-        <v>50</v>
+        <f>SUM(D21:J21)*50/(A$1-K21)</f>
+        <v>86.666666666666671</v>
       </c>
       <c r="M21" s="14">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
@@ -2883,7 +2849,7 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="16">
         <f>SUM(M21:Q21)/A$1</f>
-        <v>16.666666666666668</v>
+        <v>26.666666666666668</v>
       </c>
       <c r="S21" s="14"/>
       <c r="T21" s="14"/>
@@ -2892,91 +2858,96 @@
       <c r="W21" s="44"/>
       <c r="X21" s="21">
         <f>L21*0.2+R21*0.25+U21*0.25+V21*0.3+W21*0.15</f>
-        <v>14.166666666666668</v>
+        <v>24.000000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>129</v>
+        <v>191</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>130</v>
+        <v>190</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>131</v>
+        <v>12</v>
       </c>
       <c r="D22" s="54">
         <v>0</v>
       </c>
       <c r="E22" s="54">
-        <v>2</v>
-      </c>
-      <c r="F22" s="55">
-        <v>2</v>
-      </c>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="49">
+        <v>0</v>
+      </c>
+      <c r="F22" s="53">
+        <v>2</v>
+      </c>
+      <c r="G22" s="53">
+        <v>2</v>
+      </c>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="46">
         <v>0</v>
       </c>
       <c r="L22" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D22:J22)*50/(A$1-K22)</f>
         <v>66.666666666666671</v>
       </c>
       <c r="M22" s="14">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
-      <c r="R22" s="16"/>
+      <c r="R22" s="16">
+        <f>SUM(M22:Q22)/A$1</f>
+        <v>33.333333333333336</v>
+      </c>
       <c r="S22" s="14"/>
       <c r="T22" s="14"/>
       <c r="U22" s="16"/>
       <c r="V22" s="6"/>
       <c r="W22" s="44"/>
       <c r="X22" s="21">
-        <f>L22*0.2+R22*0.25+U22*0.25+V22*0.3+W22*0.15</f>
-        <v>13.333333333333336</v>
+        <f>L22*0.2+R22*0.25+U22*0.25+V22*0.3+W22*0.1</f>
+        <v>21.666666666666671</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>183</v>
+        <v>52</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>184</v>
+        <v>53</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="57">
-        <v>0</v>
-      </c>
-      <c r="E23" s="56">
-        <v>0</v>
-      </c>
-      <c r="F23" s="56">
-        <v>2</v>
-      </c>
-      <c r="G23" s="56" t="s">
-        <v>192</v>
-      </c>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="49">
+        <v>54</v>
+      </c>
+      <c r="D23" s="51">
+        <v>0</v>
+      </c>
+      <c r="E23" s="52">
+        <v>2</v>
+      </c>
+      <c r="F23" s="52">
         <v>1</v>
       </c>
+      <c r="G23" s="52">
+        <v>2</v>
+      </c>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="46">
+        <v>0</v>
+      </c>
       <c r="L23" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D23:J23)*50/(A$1-K23)</f>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="M23" s="14">
         <v>50</v>
-      </c>
-      <c r="M23" s="14">
-        <v>80</v>
       </c>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
@@ -2984,7 +2955,7 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="16">
         <f>SUM(M23:Q23)/A$1</f>
-        <v>26.666666666666668</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="S23" s="14"/>
       <c r="T23" s="14"/>
@@ -2992,8 +2963,8 @@
       <c r="V23" s="6"/>
       <c r="W23" s="44"/>
       <c r="X23" s="21">
-        <f>L23*0.2+R23*0.25+U23*0.25+V23*0.3+W23*0.1</f>
-        <v>16.666666666666668</v>
+        <f>L23*0.2+R23*0.25+U23*0.25+V23*0.3+W23*0.15</f>
+        <v>20.833333333333336</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3006,25 +2977,27 @@
       <c r="C24" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="54">
-        <v>2</v>
-      </c>
-      <c r="E24" s="55">
+      <c r="D24" s="51">
+        <v>2</v>
+      </c>
+      <c r="E24" s="52">
         <v>1.7</v>
       </c>
-      <c r="F24" s="55">
-        <v>0</v>
-      </c>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="49">
+      <c r="F24" s="52">
+        <v>0</v>
+      </c>
+      <c r="G24" s="52">
+        <v>2</v>
+      </c>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="46">
         <v>0</v>
       </c>
       <c r="L24" s="16">
-        <f t="shared" si="0"/>
-        <v>61.666666666666664</v>
+        <f>SUM(D24:J24)*50/(A$1-K24)</f>
+        <v>95</v>
       </c>
       <c r="M24" s="14">
         <v>0</v>
@@ -3044,41 +3017,43 @@
       <c r="W24" s="44"/>
       <c r="X24" s="21">
         <f>L24*0.2+R24*0.25+U24*0.25+V24*0.3+W24*0.15</f>
-        <v>12.333333333333334</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="57">
-        <v>0</v>
-      </c>
-      <c r="E25" s="56">
-        <v>0</v>
-      </c>
-      <c r="F25" s="56">
-        <v>2</v>
-      </c>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="49">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D25" s="54">
+        <v>0</v>
+      </c>
+      <c r="E25" s="53">
+        <v>0</v>
+      </c>
+      <c r="F25" s="53">
+        <v>2</v>
+      </c>
+      <c r="G25" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="46">
+        <v>1</v>
       </c>
       <c r="L25" s="16">
-        <f t="shared" si="0"/>
-        <v>33.333333333333336</v>
+        <f>SUM(D25:J25)*50/(A$1-K25)</f>
+        <v>50</v>
       </c>
       <c r="M25" s="14">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
@@ -3086,7 +3061,7 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="16">
         <f>SUM(M25:Q25)/A$1</f>
-        <v>33.333333333333336</v>
+        <v>26.666666666666668</v>
       </c>
       <c r="S25" s="14"/>
       <c r="T25" s="14"/>
@@ -3095,7 +3070,7 @@
       <c r="W25" s="44"/>
       <c r="X25" s="21">
         <f>L25*0.2+R25*0.25+U25*0.25+V25*0.3+W25*0.1</f>
-        <v>15.000000000000002</v>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3108,25 +3083,27 @@
       <c r="C26" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D26" s="54">
-        <v>0</v>
-      </c>
-      <c r="E26" s="55">
-        <v>0</v>
-      </c>
-      <c r="F26" s="55">
+      <c r="D26" s="51">
+        <v>0</v>
+      </c>
+      <c r="E26" s="52">
+        <v>0</v>
+      </c>
+      <c r="F26" s="52">
         <v>1.5</v>
       </c>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="49">
+      <c r="G26" s="52">
+        <v>2</v>
+      </c>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="46">
         <v>0</v>
       </c>
       <c r="L26" s="16">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>SUM(D26:J26)*50/(A$1-K26)</f>
+        <v>58.333333333333336</v>
       </c>
       <c r="M26" s="14">
         <v>50</v>
@@ -3135,7 +3112,10 @@
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
-      <c r="R26" s="16"/>
+      <c r="R26" s="16">
+        <f>SUM(M26:Q26)/A$1</f>
+        <v>16.666666666666668</v>
+      </c>
       <c r="S26" s="14"/>
       <c r="T26" s="14"/>
       <c r="U26" s="16"/>
@@ -3143,629 +3123,629 @@
       <c r="W26" s="44"/>
       <c r="X26" s="21">
         <f>L26*0.2+R26*0.25+U26*0.25+V26*0.3+W26*0.15</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+        <v>15.833333333333336</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="61" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="54"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="49">
-        <v>0</v>
-      </c>
-      <c r="L27" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="14"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="16"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="44"/>
-      <c r="X27" s="21">
+      <c r="D27" s="64"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="66">
+        <v>0</v>
+      </c>
+      <c r="L27" s="67">
+        <f>SUM(D27:J27)*50/(A$1-K27)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="68"/>
+      <c r="N27" s="69"/>
+      <c r="O27" s="69"/>
+      <c r="P27" s="69"/>
+      <c r="Q27" s="69"/>
+      <c r="R27" s="67"/>
+      <c r="S27" s="68"/>
+      <c r="T27" s="68"/>
+      <c r="U27" s="67"/>
+      <c r="V27" s="69"/>
+      <c r="W27" s="70"/>
+      <c r="X27" s="71">
         <f>L27*0.2+R27*0.25+U27*0.25+V27*0.3+W27*0.15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+    <row r="28" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="54"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="49">
-        <v>0</v>
-      </c>
-      <c r="L28" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M28" s="14"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="16"/>
-      <c r="V28" s="6"/>
-      <c r="W28" s="44"/>
-      <c r="X28" s="21">
+      <c r="D28" s="64"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="66">
+        <v>0</v>
+      </c>
+      <c r="L28" s="67">
+        <f>SUM(D28:J28)*50/(A$1-K28)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="68"/>
+      <c r="N28" s="69"/>
+      <c r="O28" s="69"/>
+      <c r="P28" s="69"/>
+      <c r="Q28" s="69"/>
+      <c r="R28" s="67"/>
+      <c r="S28" s="68"/>
+      <c r="T28" s="68"/>
+      <c r="U28" s="67"/>
+      <c r="V28" s="69"/>
+      <c r="W28" s="70"/>
+      <c r="X28" s="71">
         <f>L28*0.2+R28*0.25+U28*0.25+V28*0.3+W28*0.15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+    <row r="29" spans="1:24" s="73" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="54"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="49">
-        <v>0</v>
-      </c>
-      <c r="L29" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="14"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="6"/>
-      <c r="W29" s="44"/>
-      <c r="X29" s="21">
+      <c r="D29" s="64"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="65"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="66">
+        <v>0</v>
+      </c>
+      <c r="L29" s="67">
+        <f>SUM(D29:J29)*50/(A$1-K29)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="68"/>
+      <c r="N29" s="69"/>
+      <c r="O29" s="69"/>
+      <c r="P29" s="69"/>
+      <c r="Q29" s="69"/>
+      <c r="R29" s="67"/>
+      <c r="S29" s="68"/>
+      <c r="T29" s="68"/>
+      <c r="U29" s="67"/>
+      <c r="V29" s="69"/>
+      <c r="W29" s="70"/>
+      <c r="X29" s="71">
         <f>L29*0.2+R29*0.25+U29*0.25+V29*0.3+W29*0.15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+    <row r="30" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="54"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="49">
-        <v>0</v>
-      </c>
-      <c r="L30" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="14"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="6"/>
-      <c r="W30" s="44"/>
-      <c r="X30" s="21">
+      <c r="D30" s="64"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66">
+        <v>0</v>
+      </c>
+      <c r="L30" s="67">
+        <f>SUM(D30:J30)*50/(A$1-K30)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="68"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="69"/>
+      <c r="P30" s="69"/>
+      <c r="Q30" s="69"/>
+      <c r="R30" s="67"/>
+      <c r="S30" s="68"/>
+      <c r="T30" s="68"/>
+      <c r="U30" s="67"/>
+      <c r="V30" s="69"/>
+      <c r="W30" s="70"/>
+      <c r="X30" s="71">
         <f>L30*0.2+R30*0.25+U30*0.25+V30*0.3+W30*0.15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+    <row r="31" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="54"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="49">
-        <v>0</v>
-      </c>
-      <c r="L31" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="14"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
-      <c r="U31" s="16"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="44"/>
-      <c r="X31" s="21">
+      <c r="D31" s="64"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="66">
+        <v>0</v>
+      </c>
+      <c r="L31" s="67">
+        <f>SUM(D31:J31)*50/(A$1-K31)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="68"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="69"/>
+      <c r="Q31" s="69"/>
+      <c r="R31" s="67"/>
+      <c r="S31" s="68"/>
+      <c r="T31" s="68"/>
+      <c r="U31" s="67"/>
+      <c r="V31" s="69"/>
+      <c r="W31" s="70"/>
+      <c r="X31" s="71">
         <f>L31*0.2+R31*0.25+U31*0.25+V31*0.3+W31*0.15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+    <row r="32" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="63" t="s">
         <v>137</v>
       </c>
-      <c r="D32" s="54"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="49">
-        <v>0</v>
-      </c>
-      <c r="L32" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M32" s="14"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="16"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="44"/>
-      <c r="X32" s="21">
+      <c r="D32" s="64"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="66">
+        <v>0</v>
+      </c>
+      <c r="L32" s="67">
+        <f>SUM(D32:J32)*50/(A$1-K32)</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="68"/>
+      <c r="N32" s="69"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="69"/>
+      <c r="R32" s="67"/>
+      <c r="S32" s="68"/>
+      <c r="T32" s="68"/>
+      <c r="U32" s="67"/>
+      <c r="V32" s="69"/>
+      <c r="W32" s="70"/>
+      <c r="X32" s="71">
         <f>L32*0.2+R32*0.25+U32*0.25+V32*0.3+W32*0.15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+    <row r="33" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="61" t="s">
         <v>138</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="D33" s="54"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="49">
-        <v>0</v>
-      </c>
-      <c r="L33" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="14"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
-      <c r="U33" s="16"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="44"/>
-      <c r="X33" s="21">
+      <c r="D33" s="64"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="65"/>
+      <c r="J33" s="65"/>
+      <c r="K33" s="66">
+        <v>0</v>
+      </c>
+      <c r="L33" s="67">
+        <f>SUM(D33:J33)*50/(A$1-K33)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="68"/>
+      <c r="N33" s="69"/>
+      <c r="O33" s="69"/>
+      <c r="P33" s="69"/>
+      <c r="Q33" s="69"/>
+      <c r="R33" s="67"/>
+      <c r="S33" s="68"/>
+      <c r="T33" s="68"/>
+      <c r="U33" s="67"/>
+      <c r="V33" s="69"/>
+      <c r="W33" s="70"/>
+      <c r="X33" s="71">
         <f>L33*0.2+R33*0.25+U33*0.25+V33*0.3+W33*0.15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+    <row r="34" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="54"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="49">
-        <v>0</v>
-      </c>
-      <c r="L34" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M34" s="14"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="16">
+      <c r="D34" s="64"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="66">
+        <v>0</v>
+      </c>
+      <c r="L34" s="67">
+        <f>SUM(D34:J34)*50/(A$1-K34)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="68"/>
+      <c r="N34" s="69"/>
+      <c r="O34" s="69"/>
+      <c r="P34" s="69"/>
+      <c r="Q34" s="69"/>
+      <c r="R34" s="67">
         <f>SUM(M34:Q34)/A$1</f>
         <v>0</v>
       </c>
-      <c r="S34" s="14"/>
-      <c r="T34" s="14"/>
-      <c r="U34" s="16"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="44"/>
-      <c r="X34" s="21">
+      <c r="S34" s="68"/>
+      <c r="T34" s="68"/>
+      <c r="U34" s="67"/>
+      <c r="V34" s="69"/>
+      <c r="W34" s="70"/>
+      <c r="X34" s="71">
         <f>L34*0.2+R34*0.25+U34*0.25+V34*0.3+W34*0.15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
+    <row r="35" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="54"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="49">
-        <v>0</v>
-      </c>
-      <c r="L35" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M35" s="14"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="16">
+      <c r="D35" s="64"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="65"/>
+      <c r="K35" s="66">
+        <v>0</v>
+      </c>
+      <c r="L35" s="67">
+        <f>SUM(D35:J35)*50/(A$1-K35)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="68"/>
+      <c r="N35" s="69"/>
+      <c r="O35" s="69"/>
+      <c r="P35" s="69"/>
+      <c r="Q35" s="69"/>
+      <c r="R35" s="67">
         <f>SUM(M35:Q35)/A$1</f>
         <v>0</v>
       </c>
-      <c r="S35" s="14"/>
-      <c r="T35" s="14"/>
-      <c r="U35" s="16"/>
-      <c r="V35" s="6"/>
-      <c r="W35" s="44"/>
-      <c r="X35" s="21">
+      <c r="S35" s="68"/>
+      <c r="T35" s="68"/>
+      <c r="U35" s="67"/>
+      <c r="V35" s="69"/>
+      <c r="W35" s="70"/>
+      <c r="X35" s="71">
         <f>L35*0.2+R35*0.25+U35*0.25+V35*0.3+W35*0.15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
+    <row r="36" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="61" t="s">
         <v>153</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="D36" s="54"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="49">
-        <v>0</v>
-      </c>
-      <c r="L36" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M36" s="14"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="16">
+      <c r="D36" s="64"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="66">
+        <v>0</v>
+      </c>
+      <c r="L36" s="67">
+        <f>SUM(D36:J36)*50/(A$1-K36)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="68"/>
+      <c r="N36" s="69"/>
+      <c r="O36" s="69"/>
+      <c r="P36" s="69"/>
+      <c r="Q36" s="69"/>
+      <c r="R36" s="67">
         <f>SUM(M36:Q36)/A$1</f>
         <v>0</v>
       </c>
-      <c r="S36" s="14"/>
-      <c r="T36" s="14"/>
-      <c r="U36" s="16"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="44"/>
-      <c r="X36" s="21">
+      <c r="S36" s="68"/>
+      <c r="T36" s="68"/>
+      <c r="U36" s="67"/>
+      <c r="V36" s="69"/>
+      <c r="W36" s="70"/>
+      <c r="X36" s="71">
         <f>L36*0.2+R36*0.25+U36*0.25+V36*0.3+W36*0.15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+    <row r="37" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="61" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="D37" s="54"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="49">
-        <v>0</v>
-      </c>
-      <c r="L37" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M37" s="14"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="16">
+      <c r="D37" s="64"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="65"/>
+      <c r="K37" s="66">
+        <v>0</v>
+      </c>
+      <c r="L37" s="67">
+        <f>SUM(D37:J37)*50/(A$1-K37)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="68"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="69"/>
+      <c r="P37" s="69"/>
+      <c r="Q37" s="69"/>
+      <c r="R37" s="67">
         <f>SUM(M37:Q37)/A$1</f>
         <v>0</v>
       </c>
-      <c r="S37" s="14"/>
-      <c r="T37" s="14"/>
-      <c r="U37" s="16"/>
-      <c r="V37" s="6"/>
-      <c r="W37" s="44"/>
-      <c r="X37" s="21">
+      <c r="S37" s="68"/>
+      <c r="T37" s="68"/>
+      <c r="U37" s="67"/>
+      <c r="V37" s="69"/>
+      <c r="W37" s="70"/>
+      <c r="X37" s="71">
         <f>L37*0.2+R37*0.25+U37*0.25+V37*0.3+W37*0.1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
+    <row r="38" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="54"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="49">
-        <v>0</v>
-      </c>
-      <c r="L38" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M38" s="14"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="16">
+      <c r="D38" s="64"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="66">
+        <v>0</v>
+      </c>
+      <c r="L38" s="67">
+        <f>SUM(D38:J38)*50/(A$1-K38)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="68"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="69"/>
+      <c r="P38" s="69"/>
+      <c r="Q38" s="69"/>
+      <c r="R38" s="67">
         <f>SUM(M38:Q38)/A$1</f>
         <v>0</v>
       </c>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
-      <c r="U38" s="16"/>
-      <c r="V38" s="6"/>
-      <c r="W38" s="44"/>
-      <c r="X38" s="21">
+      <c r="S38" s="68"/>
+      <c r="T38" s="68"/>
+      <c r="U38" s="67"/>
+      <c r="V38" s="69"/>
+      <c r="W38" s="70"/>
+      <c r="X38" s="71">
         <f>L38*0.2+R38*0.25+U38*0.25+V38*0.3+W38*0.1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
+    <row r="39" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="62" t="s">
         <v>182</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="54"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="49">
-        <v>0</v>
-      </c>
-      <c r="L39" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M39" s="14"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="16">
+      <c r="D39" s="64"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="65"/>
+      <c r="J39" s="65"/>
+      <c r="K39" s="66">
+        <v>0</v>
+      </c>
+      <c r="L39" s="67">
+        <f>SUM(D39:J39)*50/(A$1-K39)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="68"/>
+      <c r="N39" s="69"/>
+      <c r="O39" s="69"/>
+      <c r="P39" s="69"/>
+      <c r="Q39" s="69"/>
+      <c r="R39" s="67">
         <f>SUM(M39:Q39)/A$1</f>
         <v>0</v>
       </c>
-      <c r="S39" s="14"/>
-      <c r="T39" s="14"/>
-      <c r="U39" s="16"/>
-      <c r="V39" s="6"/>
-      <c r="W39" s="44"/>
-      <c r="X39" s="21">
+      <c r="S39" s="68"/>
+      <c r="T39" s="68"/>
+      <c r="U39" s="67"/>
+      <c r="V39" s="69"/>
+      <c r="W39" s="70"/>
+      <c r="X39" s="71">
         <f>L39*0.2+R39*0.25+U39*0.25+V39*0.3+W39*0.1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
+    <row r="40" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="63" t="s">
         <v>187</v>
       </c>
-      <c r="D40" s="57"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
-      <c r="J40" s="56"/>
-      <c r="K40" s="49">
-        <v>0</v>
-      </c>
-      <c r="L40" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M40" s="14"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="16">
+      <c r="D40" s="74"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="75"/>
+      <c r="I40" s="75"/>
+      <c r="J40" s="75"/>
+      <c r="K40" s="66">
+        <v>0</v>
+      </c>
+      <c r="L40" s="67">
+        <f>SUM(D40:J40)*50/(A$1-K40)</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="68"/>
+      <c r="N40" s="69"/>
+      <c r="O40" s="69"/>
+      <c r="P40" s="69"/>
+      <c r="Q40" s="69"/>
+      <c r="R40" s="67">
         <f>SUM(M40:Q40)/A$1</f>
         <v>0</v>
       </c>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="16"/>
-      <c r="V40" s="6"/>
-      <c r="W40" s="44"/>
-      <c r="X40" s="21">
+      <c r="S40" s="68"/>
+      <c r="T40" s="68"/>
+      <c r="U40" s="67"/>
+      <c r="V40" s="69"/>
+      <c r="W40" s="70"/>
+      <c r="X40" s="71">
         <f>L40*0.2+R40*0.25+U40*0.25+V40*0.3+W40*0.1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
+    <row r="41" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="57"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
-      <c r="J41" s="56"/>
-      <c r="K41" s="49">
-        <v>0</v>
-      </c>
-      <c r="L41" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M41" s="14"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="16">
+      <c r="D41" s="74"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="75"/>
+      <c r="J41" s="75"/>
+      <c r="K41" s="66">
+        <v>0</v>
+      </c>
+      <c r="L41" s="67">
+        <f>SUM(D41:J41)*50/(A$1-K41)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="68"/>
+      <c r="N41" s="69"/>
+      <c r="O41" s="69"/>
+      <c r="P41" s="69"/>
+      <c r="Q41" s="69"/>
+      <c r="R41" s="67">
         <f>SUM(M41:Q41)/A$1</f>
         <v>0</v>
       </c>
-      <c r="S41" s="14"/>
-      <c r="T41" s="14"/>
-      <c r="U41" s="16"/>
-      <c r="V41" s="6"/>
-      <c r="W41" s="44"/>
-      <c r="X41" s="21">
+      <c r="S41" s="68"/>
+      <c r="T41" s="68"/>
+      <c r="U41" s="67"/>
+      <c r="V41" s="69"/>
+      <c r="W41" s="70"/>
+      <c r="X41" s="71">
         <f>L41*0.2+R41*0.25+U41*0.25+V41*0.3+W41*0.1</f>
         <v>0</v>
       </c>
@@ -3774,14 +3754,14 @@
       <c r="A42" s="20"/>
       <c r="B42" s="3"/>
       <c r="C42" s="11"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="56"/>
-      <c r="H42" s="56"/>
-      <c r="I42" s="56"/>
-      <c r="J42" s="56"/>
-      <c r="K42" s="49"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="46"/>
       <c r="L42" s="16"/>
       <c r="M42" s="14"/>
       <c r="N42" s="6"/>
@@ -3806,14 +3786,14 @@
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="50"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="55"/>
+      <c r="K43" s="47"/>
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
@@ -3829,14 +3809,14 @@
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
-      <c r="K44" s="50"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="47"/>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
@@ -3852,14 +3832,14 @@
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="58"/>
-      <c r="K45" s="50"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="47"/>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
@@ -3875,14 +3855,14 @@
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
-      <c r="J46" s="58"/>
-      <c r="K46" s="50"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="55"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="55"/>
+      <c r="J46" s="55"/>
+      <c r="K46" s="47"/>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
       <c r="N46" s="9"/>
@@ -3898,14 +3878,14 @@
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
-      <c r="K47" s="50"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="55"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="47"/>
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
       <c r="N47" s="9"/>
@@ -3921,14 +3901,14 @@
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
-      <c r="J48" s="58"/>
-      <c r="K48" s="50"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="55"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="47"/>
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
       <c r="N48" s="9"/>
@@ -3944,14 +3924,14 @@
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="58"/>
-      <c r="K49" s="50"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
+      <c r="F49" s="55"/>
+      <c r="G49" s="55"/>
+      <c r="H49" s="55"/>
+      <c r="I49" s="55"/>
+      <c r="J49" s="55"/>
+      <c r="K49" s="47"/>
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
       <c r="N49" s="9"/>
@@ -3967,14 +3947,14 @@
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-      <c r="J50" s="58"/>
-      <c r="K50" s="50"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="55"/>
+      <c r="I50" s="55"/>
+      <c r="J50" s="55"/>
+      <c r="K50" s="47"/>
       <c r="L50" s="9"/>
       <c r="M50" s="9"/>
       <c r="N50" s="9"/>
@@ -3990,14 +3970,14 @@
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
-      <c r="J51" s="58"/>
-      <c r="K51" s="50"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="55"/>
+      <c r="I51" s="55"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="47"/>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
@@ -4013,14 +3993,14 @@
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="58"/>
-      <c r="I52" s="58"/>
-      <c r="J52" s="58"/>
-      <c r="K52" s="50"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="55"/>
+      <c r="G52" s="55"/>
+      <c r="H52" s="55"/>
+      <c r="I52" s="55"/>
+      <c r="J52" s="55"/>
+      <c r="K52" s="47"/>
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
       <c r="N52" s="9"/>
@@ -4036,14 +4016,14 @@
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="58"/>
-      <c r="J53" s="58"/>
-      <c r="K53" s="50"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="55"/>
+      <c r="H53" s="55"/>
+      <c r="I53" s="55"/>
+      <c r="J53" s="55"/>
+      <c r="K53" s="47"/>
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
@@ -4059,14 +4039,14 @@
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="J54" s="58"/>
-      <c r="K54" s="50"/>
+      <c r="D54" s="55"/>
+      <c r="E54" s="55"/>
+      <c r="F54" s="55"/>
+      <c r="G54" s="55"/>
+      <c r="H54" s="55"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="47"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
       <c r="N54" s="9"/>
@@ -4082,14 +4062,14 @@
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="58"/>
-      <c r="J55" s="58"/>
-      <c r="K55" s="50"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="55"/>
+      <c r="G55" s="55"/>
+      <c r="H55" s="55"/>
+      <c r="I55" s="55"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="47"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
       <c r="N55" s="9"/>
@@ -4105,14 +4085,14 @@
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="58"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="58"/>
-      <c r="J56" s="58"/>
-      <c r="K56" s="50"/>
+      <c r="D56" s="55"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="55"/>
+      <c r="G56" s="55"/>
+      <c r="H56" s="55"/>
+      <c r="I56" s="55"/>
+      <c r="J56" s="55"/>
+      <c r="K56" s="47"/>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
       <c r="N56" s="9"/>
@@ -4128,14 +4108,14 @@
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="58"/>
-      <c r="J57" s="58"/>
-      <c r="K57" s="50"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="55"/>
+      <c r="G57" s="55"/>
+      <c r="H57" s="55"/>
+      <c r="I57" s="55"/>
+      <c r="J57" s="55"/>
+      <c r="K57" s="47"/>
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
@@ -4151,14 +4131,14 @@
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="58"/>
-      <c r="F58" s="58"/>
-      <c r="G58" s="58"/>
-      <c r="H58" s="58"/>
-      <c r="I58" s="58"/>
-      <c r="J58" s="58"/>
-      <c r="K58" s="50"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="55"/>
+      <c r="G58" s="55"/>
+      <c r="H58" s="55"/>
+      <c r="I58" s="55"/>
+      <c r="J58" s="55"/>
+      <c r="K58" s="47"/>
       <c r="L58" s="9"/>
       <c r="M58" s="9"/>
       <c r="N58" s="9"/>
@@ -4174,14 +4154,14 @@
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
-      <c r="J59" s="58"/>
-      <c r="K59" s="50"/>
+      <c r="D59" s="55"/>
+      <c r="E59" s="55"/>
+      <c r="F59" s="55"/>
+      <c r="G59" s="55"/>
+      <c r="H59" s="55"/>
+      <c r="I59" s="55"/>
+      <c r="J59" s="55"/>
+      <c r="K59" s="47"/>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
       <c r="N59" s="9"/>
@@ -4197,14 +4177,14 @@
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="58"/>
-      <c r="E60" s="58"/>
-      <c r="F60" s="58"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="58"/>
-      <c r="J60" s="58"/>
-      <c r="K60" s="50"/>
+      <c r="D60" s="55"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="55"/>
+      <c r="G60" s="55"/>
+      <c r="H60" s="55"/>
+      <c r="I60" s="55"/>
+      <c r="J60" s="55"/>
+      <c r="K60" s="47"/>
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
       <c r="N60" s="9"/>
@@ -4220,14 +4200,14 @@
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
-      <c r="D61" s="58"/>
-      <c r="E61" s="58"/>
-      <c r="F61" s="58"/>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="58"/>
-      <c r="J61" s="58"/>
-      <c r="K61" s="50"/>
+      <c r="D61" s="55"/>
+      <c r="E61" s="55"/>
+      <c r="F61" s="55"/>
+      <c r="G61" s="55"/>
+      <c r="H61" s="55"/>
+      <c r="I61" s="55"/>
+      <c r="J61" s="55"/>
+      <c r="K61" s="47"/>
       <c r="L61" s="9"/>
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
@@ -4243,14 +4223,14 @@
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
-      <c r="D62" s="58"/>
-      <c r="E62" s="58"/>
-      <c r="F62" s="58"/>
-      <c r="G62" s="58"/>
-      <c r="H62" s="58"/>
-      <c r="I62" s="58"/>
-      <c r="J62" s="58"/>
-      <c r="K62" s="50"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="55"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="55"/>
+      <c r="I62" s="55"/>
+      <c r="J62" s="55"/>
+      <c r="K62" s="47"/>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
       <c r="N62" s="9"/>
@@ -4266,14 +4246,14 @@
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
-      <c r="D63" s="58"/>
-      <c r="E63" s="58"/>
-      <c r="F63" s="58"/>
-      <c r="G63" s="58"/>
-      <c r="H63" s="58"/>
-      <c r="I63" s="58"/>
-      <c r="J63" s="58"/>
-      <c r="K63" s="50"/>
+      <c r="D63" s="55"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="55"/>
+      <c r="G63" s="55"/>
+      <c r="H63" s="55"/>
+      <c r="I63" s="55"/>
+      <c r="J63" s="55"/>
+      <c r="K63" s="47"/>
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
@@ -4286,8 +4266,8 @@
       <c r="U63" s="9"/>
     </row>
   </sheetData>
-  <sortState ref="A3:Z55">
-    <sortCondition descending="1" ref="X2"/>
+  <sortState ref="A3:X42">
+    <sortCondition descending="1" ref="X3"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="S1:U1"/>
@@ -4489,22 +4469,22 @@
       <c r="B1" s="18"/>
       <c r="C1" s="34"/>
       <c r="D1" s="40"/>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="45" t="s">
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="47"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="60"/>
       <c r="Q1" s="33" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
Yazilim araclari not guncelleme
</commit_message>
<xml_diff>
--- a/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
+++ b/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
@@ -1178,15 +1178,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1211,6 +1202,15 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1714,7 +1714,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z8" sqref="Z8"/>
+      <selection pane="bottomLeft" activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1724,7 +1724,8 @@
     <col min="3" max="3" width="9.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="3.21875" style="56" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2.88671875" style="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="2.44140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.88671875" style="57" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.44140625" style="57" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.44140625" style="57" customWidth="1"/>
     <col min="11" max="11" width="2.88671875" style="48" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.88671875" style="1" customWidth="1"/>
@@ -1733,7 +1734,7 @@
     <col min="17" max="17" width="2.5546875" style="1" customWidth="1"/>
     <col min="18" max="18" width="4.77734375" style="1" customWidth="1"/>
     <col min="19" max="20" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7" style="1" customWidth="1"/>
     <col min="24" max="24" width="5.77734375" style="1" customWidth="1"/>
@@ -1742,34 +1743,34 @@
   <sheetData>
     <row r="1" spans="1:24" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="29"/>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="58" t="s">
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="58" t="s">
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="T1" s="59"/>
-      <c r="U1" s="60"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="75"/>
       <c r="V1" s="17" t="s">
         <v>96</v>
       </c>
@@ -1876,7 +1877,9 @@
       <c r="G3" s="52" t="s">
         <v>192</v>
       </c>
-      <c r="H3" s="52"/>
+      <c r="H3" s="52">
+        <v>2</v>
+      </c>
       <c r="I3" s="52"/>
       <c r="J3" s="52"/>
       <c r="K3" s="46">
@@ -1884,7 +1887,7 @@
       </c>
       <c r="L3" s="16">
         <f>SUM(D3:J3)*50/(A$1-K3)</f>
-        <v>150</v>
+        <v>133.33333333333334</v>
       </c>
       <c r="M3" s="14">
         <v>100</v>
@@ -1895,27 +1898,32 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="16">
         <f>SUM(M3:Q3)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S3" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S3" s="14">
+        <v>60</v>
+      </c>
       <c r="T3" s="14"/>
-      <c r="U3" s="16"/>
+      <c r="U3" s="16">
+        <f>SUM(S3:T3)/1</f>
+        <v>60</v>
+      </c>
       <c r="V3" s="6"/>
       <c r="W3" s="44"/>
       <c r="X3" s="21">
         <f>L3*0.2+R3*0.25+U3*0.25+V3*0.3+W3*0.15</f>
-        <v>38.333333333333336</v>
+        <v>47.916666666666671</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>177</v>
+        <v>118</v>
       </c>
       <c r="D4" s="51">
         <v>2</v>
@@ -1929,7 +1937,9 @@
       <c r="G4" s="52">
         <v>2</v>
       </c>
-      <c r="H4" s="52"/>
+      <c r="H4" s="52">
+        <v>2</v>
+      </c>
       <c r="I4" s="52"/>
       <c r="J4" s="52"/>
       <c r="K4" s="46">
@@ -1937,7 +1947,7 @@
       </c>
       <c r="L4" s="16">
         <f>SUM(D4:J4)*50/(A$1-K4)</f>
-        <v>133.33333333333334</v>
+        <v>125</v>
       </c>
       <c r="M4" s="14">
         <v>100</v>
@@ -1948,27 +1958,32 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="16">
         <f>SUM(M4:Q4)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S4" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S4" s="14">
+        <v>60</v>
+      </c>
       <c r="T4" s="14"/>
-      <c r="U4" s="16"/>
+      <c r="U4" s="16">
+        <f>SUM(S4:T4)/1</f>
+        <v>60</v>
+      </c>
       <c r="V4" s="6"/>
       <c r="W4" s="44"/>
       <c r="X4" s="21">
-        <f>L4*0.2+R4*0.25+U4*0.25+V4*0.3+W4*0.1</f>
-        <v>35.000000000000007</v>
+        <f>L4*0.2+R4*0.25+U4*0.25+V4*0.3+W4*0.15</f>
+        <v>46.25</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="D5" s="51">
         <v>2</v>
@@ -1982,7 +1997,9 @@
       <c r="G5" s="52">
         <v>2</v>
       </c>
-      <c r="H5" s="52"/>
+      <c r="H5" s="52">
+        <v>2</v>
+      </c>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="46">
@@ -1990,7 +2007,7 @@
       </c>
       <c r="L5" s="16">
         <f>SUM(D5:J5)*50/(A$1-K5)</f>
-        <v>133.33333333333334</v>
+        <v>125</v>
       </c>
       <c r="M5" s="14">
         <v>100</v>
@@ -2001,27 +2018,32 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="16">
         <f>SUM(M5:Q5)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S5" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S5" s="14">
+        <v>60</v>
+      </c>
       <c r="T5" s="14"/>
-      <c r="U5" s="16"/>
+      <c r="U5" s="16">
+        <f>SUM(S5:T5)/1</f>
+        <v>60</v>
+      </c>
       <c r="V5" s="6"/>
       <c r="W5" s="44"/>
       <c r="X5" s="21">
-        <f>L5*0.2+R5*0.25+U5*0.25+V5*0.3+W5*0.15</f>
-        <v>35.000000000000007</v>
+        <f>L5*0.2+R5*0.25+U5*0.25+V5*0.3+W5*0.1</f>
+        <v>46.25</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>109</v>
+        <v>165</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>110</v>
+        <v>166</v>
       </c>
       <c r="D6" s="51">
         <v>2</v>
@@ -2035,7 +2057,9 @@
       <c r="G6" s="52">
         <v>2</v>
       </c>
-      <c r="H6" s="52"/>
+      <c r="H6" s="52">
+        <v>2</v>
+      </c>
       <c r="I6" s="52"/>
       <c r="J6" s="52"/>
       <c r="K6" s="46">
@@ -2043,7 +2067,7 @@
       </c>
       <c r="L6" s="16">
         <f>SUM(D6:J6)*50/(A$1-K6)</f>
-        <v>133.33333333333334</v>
+        <v>125</v>
       </c>
       <c r="M6" s="14">
         <v>100</v>
@@ -2054,27 +2078,32 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="16">
         <f>SUM(M6:Q6)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S6" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S6" s="14">
+        <v>60</v>
+      </c>
       <c r="T6" s="14"/>
-      <c r="U6" s="16"/>
+      <c r="U6" s="16">
+        <f>SUM(S6:T6)/1</f>
+        <v>60</v>
+      </c>
       <c r="V6" s="6"/>
       <c r="W6" s="44"/>
       <c r="X6" s="21">
-        <f>L6*0.2+R6*0.25+U6*0.25+V6*0.3+W6*0.15</f>
-        <v>35.000000000000007</v>
+        <f>L6*0.2+R6*0.25+U6*0.25+V6*0.3+W6*0.1</f>
+        <v>46.25</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>114</v>
+        <v>178</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
       <c r="D7" s="51">
         <v>2</v>
@@ -2088,7 +2117,9 @@
       <c r="G7" s="52">
         <v>2</v>
       </c>
-      <c r="H7" s="52"/>
+      <c r="H7" s="52">
+        <v>2</v>
+      </c>
       <c r="I7" s="52"/>
       <c r="J7" s="52"/>
       <c r="K7" s="46">
@@ -2096,7 +2127,7 @@
       </c>
       <c r="L7" s="16">
         <f>SUM(D7:J7)*50/(A$1-K7)</f>
-        <v>133.33333333333334</v>
+        <v>125</v>
       </c>
       <c r="M7" s="14">
         <v>100</v>
@@ -2107,27 +2138,32 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="16">
         <f>SUM(M7:Q7)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S7" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S7" s="14">
+        <v>60</v>
+      </c>
       <c r="T7" s="14"/>
-      <c r="U7" s="16"/>
+      <c r="U7" s="16">
+        <f>SUM(S7:T7)/1</f>
+        <v>60</v>
+      </c>
       <c r="V7" s="6"/>
       <c r="W7" s="44"/>
       <c r="X7" s="21">
-        <f>L7*0.2+R7*0.25+U7*0.25+V7*0.3+W7*0.15</f>
-        <v>35.000000000000007</v>
+        <f>L7*0.2+R7*0.25+U7*0.25+V7*0.3+W7*0.1</f>
+        <v>46.25</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="D8" s="51">
         <v>2</v>
@@ -2141,7 +2177,9 @@
       <c r="G8" s="52">
         <v>2</v>
       </c>
-      <c r="H8" s="52"/>
+      <c r="H8" s="52">
+        <v>1.9</v>
+      </c>
       <c r="I8" s="52"/>
       <c r="J8" s="52"/>
       <c r="K8" s="46">
@@ -2149,7 +2187,7 @@
       </c>
       <c r="L8" s="16">
         <f>SUM(D8:J8)*50/(A$1-K8)</f>
-        <v>133.33333333333334</v>
+        <v>123.75</v>
       </c>
       <c r="M8" s="14">
         <v>100</v>
@@ -2160,27 +2198,32 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="16">
         <f>SUM(M8:Q8)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S8" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S8" s="14">
+        <v>60</v>
+      </c>
       <c r="T8" s="14"/>
-      <c r="U8" s="16"/>
+      <c r="U8" s="16">
+        <f>SUM(S8:T8)/1</f>
+        <v>60</v>
+      </c>
       <c r="V8" s="6"/>
       <c r="W8" s="44"/>
       <c r="X8" s="21">
-        <f>L8*0.2+R8*0.25+U8*0.25+V8*0.3+W8*0.1</f>
-        <v>35.000000000000007</v>
+        <f>L8*0.2+R8*0.25+U8*0.25+V8*0.3+W8*0.15</f>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="D9" s="51">
         <v>2</v>
@@ -2194,7 +2237,9 @@
       <c r="G9" s="52">
         <v>2</v>
       </c>
-      <c r="H9" s="52"/>
+      <c r="H9" s="52">
+        <v>1.9</v>
+      </c>
       <c r="I9" s="52"/>
       <c r="J9" s="52"/>
       <c r="K9" s="46">
@@ -2202,7 +2247,7 @@
       </c>
       <c r="L9" s="16">
         <f>SUM(D9:J9)*50/(A$1-K9)</f>
-        <v>133.33333333333334</v>
+        <v>123.75</v>
       </c>
       <c r="M9" s="14">
         <v>100</v>
@@ -2213,27 +2258,32 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="16">
         <f>SUM(M9:Q9)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S9" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S9" s="14">
+        <v>60</v>
+      </c>
       <c r="T9" s="14"/>
-      <c r="U9" s="16"/>
+      <c r="U9" s="16">
+        <f>SUM(S9:T9)/1</f>
+        <v>60</v>
+      </c>
       <c r="V9" s="6"/>
       <c r="W9" s="44"/>
       <c r="X9" s="21">
-        <f>L9*0.2+R9*0.25+U9*0.25+V9*0.3+W9*0.1</f>
-        <v>35.000000000000007</v>
+        <f>L9*0.2+R9*0.25+U9*0.25+V9*0.3+W9*0.15</f>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="D10" s="51">
         <v>2</v>
@@ -2247,7 +2297,9 @@
       <c r="G10" s="52">
         <v>2</v>
       </c>
-      <c r="H10" s="52"/>
+      <c r="H10" s="52">
+        <v>2</v>
+      </c>
       <c r="I10" s="52"/>
       <c r="J10" s="52"/>
       <c r="K10" s="46">
@@ -2255,10 +2307,10 @@
       </c>
       <c r="L10" s="16">
         <f>SUM(D10:J10)*50/(A$1-K10)</f>
-        <v>133.33333333333334</v>
+        <v>125</v>
       </c>
       <c r="M10" s="14">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
@@ -2266,27 +2318,32 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="16">
         <f>SUM(M10:Q10)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S10" s="14"/>
+        <v>23.75</v>
+      </c>
+      <c r="S10" s="14">
+        <v>60</v>
+      </c>
       <c r="T10" s="14"/>
-      <c r="U10" s="16"/>
+      <c r="U10" s="16">
+        <f>SUM(S10:T10)/1</f>
+        <v>60</v>
+      </c>
       <c r="V10" s="6"/>
       <c r="W10" s="44"/>
       <c r="X10" s="21">
-        <f>L10*0.2+R10*0.25+U10*0.25+V10*0.3+W10*0.1</f>
-        <v>35.000000000000007</v>
+        <f>L10*0.2+R10*0.25+U10*0.25+V10*0.3+W10*0.15</f>
+        <v>45.9375</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="D11" s="51">
         <v>2</v>
@@ -2300,7 +2357,9 @@
       <c r="G11" s="52">
         <v>2</v>
       </c>
-      <c r="H11" s="52"/>
+      <c r="H11" s="52">
+        <v>1.8</v>
+      </c>
       <c r="I11" s="52"/>
       <c r="J11" s="52"/>
       <c r="K11" s="46">
@@ -2308,10 +2367,10 @@
       </c>
       <c r="L11" s="16">
         <f>SUM(D11:J11)*50/(A$1-K11)</f>
-        <v>133.33333333333334</v>
+        <v>122.50000000000001</v>
       </c>
       <c r="M11" s="14">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
@@ -2319,16 +2378,21 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="16">
         <f>SUM(M11:Q11)/A$1</f>
-        <v>31.666666666666668</v>
-      </c>
-      <c r="S11" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S11" s="14">
+        <v>60</v>
+      </c>
       <c r="T11" s="14"/>
-      <c r="U11" s="16"/>
+      <c r="U11" s="16">
+        <f>SUM(S11:T11)/1</f>
+        <v>60</v>
+      </c>
       <c r="V11" s="6"/>
       <c r="W11" s="44"/>
       <c r="X11" s="21">
-        <f>L11*0.2+R11*0.25+U11*0.25+V11*0.3+W11*0.15</f>
-        <v>34.583333333333336</v>
+        <f>L11*0.2+R11*0.25+U11*0.25+V11*0.3+W11*0.1</f>
+        <v>45.75</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2353,7 +2417,9 @@
       <c r="G12" s="52">
         <v>2</v>
       </c>
-      <c r="H12" s="52"/>
+      <c r="H12" s="52">
+        <v>2</v>
+      </c>
       <c r="I12" s="52"/>
       <c r="J12" s="52"/>
       <c r="K12" s="46">
@@ -2361,7 +2427,7 @@
       </c>
       <c r="L12" s="16">
         <f>SUM(D12:J12)*50/(A$1-K12)</f>
-        <v>133.33333333333334</v>
+        <v>125</v>
       </c>
       <c r="M12" s="14">
         <v>85</v>
@@ -2372,27 +2438,32 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="16">
         <f>SUM(M12:Q12)/A$1</f>
-        <v>28.333333333333332</v>
-      </c>
-      <c r="S12" s="14"/>
+        <v>21.25</v>
+      </c>
+      <c r="S12" s="14">
+        <v>60</v>
+      </c>
       <c r="T12" s="14"/>
-      <c r="U12" s="16"/>
+      <c r="U12" s="16">
+        <f>SUM(S12:T12)/1</f>
+        <v>60</v>
+      </c>
       <c r="V12" s="6"/>
       <c r="W12" s="44"/>
       <c r="X12" s="21">
         <f>L12*0.2+R12*0.25+U12*0.25+V12*0.3+W12*0.1</f>
-        <v>33.750000000000007</v>
+        <v>45.3125</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D13" s="51">
         <v>2</v>
@@ -2406,7 +2477,9 @@
       <c r="G13" s="52">
         <v>2</v>
       </c>
-      <c r="H13" s="52"/>
+      <c r="H13" s="52">
+        <v>2</v>
+      </c>
       <c r="I13" s="52"/>
       <c r="J13" s="52"/>
       <c r="K13" s="46">
@@ -2414,10 +2487,10 @@
       </c>
       <c r="L13" s="16">
         <f>SUM(D13:J13)*50/(A$1-K13)</f>
-        <v>133.33333333333334</v>
+        <v>125</v>
       </c>
       <c r="M13" s="14">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
@@ -2425,30 +2498,35 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="16">
         <f>SUM(M13:Q13)/A$1</f>
-        <v>28.333333333333332</v>
-      </c>
-      <c r="S13" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="S13" s="14">
+        <v>60</v>
+      </c>
       <c r="T13" s="14"/>
-      <c r="U13" s="16"/>
+      <c r="U13" s="16">
+        <f>SUM(S13:T13)/1</f>
+        <v>60</v>
+      </c>
       <c r="V13" s="6"/>
       <c r="W13" s="44"/>
       <c r="X13" s="21">
         <f>L13*0.2+R13*0.25+U13*0.25+V13*0.3+W13*0.1</f>
-        <v>33.750000000000007</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="D14" s="51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="52">
         <v>2</v>
@@ -2459,7 +2537,9 @@
       <c r="G14" s="52">
         <v>2</v>
       </c>
-      <c r="H14" s="52"/>
+      <c r="H14" s="52">
+        <v>2</v>
+      </c>
       <c r="I14" s="52"/>
       <c r="J14" s="52"/>
       <c r="K14" s="46">
@@ -2467,10 +2547,10 @@
       </c>
       <c r="L14" s="16">
         <f>SUM(D14:J14)*50/(A$1-K14)</f>
-        <v>133.33333333333334</v>
+        <v>100</v>
       </c>
       <c r="M14" s="14">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
@@ -2478,49 +2558,56 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="16">
         <f>SUM(M14:Q14)/A$1</f>
-        <v>26.666666666666668</v>
-      </c>
-      <c r="S14" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S14" s="14">
+        <v>60</v>
+      </c>
       <c r="T14" s="14"/>
-      <c r="U14" s="16"/>
+      <c r="U14" s="16">
+        <f>SUM(S14:T14)/1</f>
+        <v>60</v>
+      </c>
       <c r="V14" s="6"/>
       <c r="W14" s="44"/>
       <c r="X14" s="21">
-        <f>L14*0.2+R14*0.25+U14*0.25+V14*0.3+W14*0.1</f>
-        <v>33.333333333333336</v>
+        <f>L14*0.2+R14*0.25+U14*0.25+V14*0.3+W14*0.15</f>
+        <v>41.25</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>188</v>
+        <v>122</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="D15" s="51">
-        <v>2</v>
-      </c>
-      <c r="E15" s="53">
+        <v>0</v>
+      </c>
+      <c r="E15" s="52">
         <v>2</v>
       </c>
       <c r="F15" s="52">
         <v>2</v>
       </c>
-      <c r="G15" s="53">
-        <v>1.5</v>
-      </c>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
+      <c r="G15" s="52">
+        <v>2</v>
+      </c>
+      <c r="H15" s="52">
+        <v>2</v>
+      </c>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
       <c r="K15" s="46">
         <v>0</v>
       </c>
       <c r="L15" s="16">
         <f>SUM(D15:J15)*50/(A$1-K15)</f>
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="M15" s="14">
         <v>100</v>
@@ -2531,27 +2618,32 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="16">
         <f>SUM(M15:Q15)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S15" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S15" s="14">
+        <v>60</v>
+      </c>
       <c r="T15" s="14"/>
-      <c r="U15" s="16"/>
+      <c r="U15" s="16">
+        <f>SUM(S15:T15)/1</f>
+        <v>60</v>
+      </c>
       <c r="V15" s="6"/>
       <c r="W15" s="44"/>
       <c r="X15" s="21">
-        <f>L15*0.2+R15*0.25+U15*0.25+V15*0.3+W15*0.1</f>
-        <v>33.333333333333336</v>
+        <f>L15*0.2+R15*0.25+U15*0.25+V15*0.3+W15*0.15</f>
+        <v>41.25</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D16" s="51">
         <v>0</v>
@@ -2565,7 +2657,9 @@
       <c r="G16" s="52">
         <v>2</v>
       </c>
-      <c r="H16" s="52"/>
+      <c r="H16" s="52">
+        <v>2</v>
+      </c>
       <c r="I16" s="52"/>
       <c r="J16" s="52"/>
       <c r="K16" s="46">
@@ -2584,52 +2678,59 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="16">
         <f>SUM(M16:Q16)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S16" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S16" s="14">
+        <v>60</v>
+      </c>
       <c r="T16" s="14"/>
-      <c r="U16" s="16"/>
+      <c r="U16" s="16">
+        <f>SUM(S16:T16)/1</f>
+        <v>60</v>
+      </c>
       <c r="V16" s="6"/>
       <c r="W16" s="44"/>
       <c r="X16" s="21">
         <f>L16*0.2+R16*0.25+U16*0.25+V16*0.3+W16*0.15</f>
-        <v>28.333333333333336</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>144</v>
+        <v>85</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>145</v>
+        <v>86</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D17" s="51">
-        <v>0</v>
-      </c>
-      <c r="E17" s="52">
-        <v>2</v>
-      </c>
-      <c r="F17" s="52">
-        <v>2</v>
-      </c>
-      <c r="G17" s="52">
-        <v>2</v>
-      </c>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
+        <v>87</v>
+      </c>
+      <c r="D17" s="54">
+        <v>0</v>
+      </c>
+      <c r="E17" s="53">
+        <v>2</v>
+      </c>
+      <c r="F17" s="53">
+        <v>2</v>
+      </c>
+      <c r="G17" s="53">
+        <v>2</v>
+      </c>
+      <c r="H17" s="53">
+        <v>0</v>
+      </c>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
       <c r="K17" s="46">
         <v>0</v>
       </c>
       <c r="L17" s="16">
         <f>SUM(D17:J17)*50/(A$1-K17)</f>
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="M17" s="14">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
@@ -2637,27 +2738,32 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="16">
         <f>SUM(M17:Q17)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S17" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="S17" s="14">
+        <v>60</v>
+      </c>
       <c r="T17" s="14"/>
-      <c r="U17" s="16"/>
+      <c r="U17" s="16">
+        <f>SUM(S17:T17)/1</f>
+        <v>60</v>
+      </c>
       <c r="V17" s="6"/>
       <c r="W17" s="44"/>
       <c r="X17" s="21">
-        <f>L17*0.2+R17*0.25+U17*0.25+V17*0.3+W17*0.15</f>
-        <v>28.333333333333336</v>
+        <f>L17*0.2+R17*0.25+U17*0.25+V17*0.3+W17*0.1</f>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>122</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="D18" s="51">
         <v>0</v>
@@ -2666,12 +2772,14 @@
         <v>2</v>
       </c>
       <c r="F18" s="52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="52">
         <v>2</v>
       </c>
-      <c r="H18" s="52"/>
+      <c r="H18" s="52">
+        <v>0</v>
+      </c>
       <c r="I18" s="52"/>
       <c r="J18" s="52"/>
       <c r="K18" s="46">
@@ -2679,10 +2787,10 @@
       </c>
       <c r="L18" s="16">
         <f>SUM(D18:J18)*50/(A$1-K18)</f>
-        <v>100</v>
+        <v>62.5</v>
       </c>
       <c r="M18" s="14">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
@@ -2690,49 +2798,56 @@
       <c r="Q18" s="6"/>
       <c r="R18" s="16">
         <f>SUM(M18:Q18)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S18" s="14"/>
+        <v>12.5</v>
+      </c>
+      <c r="S18" s="14">
+        <v>60</v>
+      </c>
       <c r="T18" s="14"/>
-      <c r="U18" s="16"/>
+      <c r="U18" s="16">
+        <f>SUM(S18:T18)/1</f>
+        <v>60</v>
+      </c>
       <c r="V18" s="6"/>
       <c r="W18" s="44"/>
       <c r="X18" s="21">
         <f>L18*0.2+R18*0.25+U18*0.25+V18*0.3+W18*0.15</f>
-        <v>28.333333333333336</v>
+        <v>30.625</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="D19" s="51">
-        <v>0</v>
-      </c>
-      <c r="E19" s="52">
+        <v>2</v>
+      </c>
+      <c r="E19" s="53">
         <v>2</v>
       </c>
       <c r="F19" s="52">
         <v>2</v>
       </c>
-      <c r="G19" s="52">
-        <v>2</v>
-      </c>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
+      <c r="G19" s="53">
+        <v>1.5</v>
+      </c>
+      <c r="H19" s="53">
+        <v>2</v>
+      </c>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
       <c r="K19" s="46">
         <v>0</v>
       </c>
       <c r="L19" s="16">
         <f>SUM(D19:J19)*50/(A$1-K19)</f>
-        <v>100</v>
+        <v>118.75</v>
       </c>
       <c r="M19" s="14">
         <v>100</v>
@@ -2743,43 +2858,50 @@
       <c r="Q19" s="6"/>
       <c r="R19" s="16">
         <f>SUM(M19:Q19)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S19" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S19" s="14">
+        <v>0</v>
+      </c>
       <c r="T19" s="14"/>
-      <c r="U19" s="16"/>
+      <c r="U19" s="16">
+        <f>SUM(S19:T19)/1</f>
+        <v>0</v>
+      </c>
       <c r="V19" s="6"/>
       <c r="W19" s="44"/>
       <c r="X19" s="21">
-        <f>L19*0.2+R19*0.25+U19*0.25+V19*0.3+W19*0.15</f>
-        <v>28.333333333333336</v>
+        <f>L19*0.2+R19*0.25+U19*0.25+V19*0.3+W19*0.1</f>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>85</v>
+        <v>173</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="54">
-        <v>0</v>
-      </c>
-      <c r="E20" s="53">
-        <v>2</v>
-      </c>
-      <c r="F20" s="53">
-        <v>2</v>
-      </c>
-      <c r="G20" s="53">
-        <v>2</v>
-      </c>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+        <v>180</v>
+      </c>
+      <c r="D20" s="51">
+        <v>2</v>
+      </c>
+      <c r="E20" s="52">
+        <v>2</v>
+      </c>
+      <c r="F20" s="52">
+        <v>2</v>
+      </c>
+      <c r="G20" s="52">
+        <v>2</v>
+      </c>
+      <c r="H20" s="52">
+        <v>0</v>
+      </c>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
       <c r="K20" s="46">
         <v>0</v>
       </c>
@@ -2788,7 +2910,7 @@
         <v>100</v>
       </c>
       <c r="M20" s="14">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
@@ -2796,27 +2918,32 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="16">
         <f>SUM(M20:Q20)/A$1</f>
-        <v>26.666666666666668</v>
-      </c>
-      <c r="S20" s="14"/>
+        <v>21.25</v>
+      </c>
+      <c r="S20" s="14">
+        <v>0</v>
+      </c>
       <c r="T20" s="14"/>
-      <c r="U20" s="16"/>
+      <c r="U20" s="16">
+        <f>SUM(S20:T20)/1</f>
+        <v>0</v>
+      </c>
       <c r="V20" s="6"/>
       <c r="W20" s="44"/>
       <c r="X20" s="21">
         <f>L20*0.2+R20*0.25+U20*0.25+V20*0.3+W20*0.1</f>
-        <v>26.666666666666668</v>
+        <v>25.3125</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D21" s="51">
         <v>0</v>
@@ -2828,9 +2955,11 @@
         <v>2</v>
       </c>
       <c r="G21" s="52">
-        <v>1.2</v>
-      </c>
-      <c r="H21" s="52"/>
+        <v>2</v>
+      </c>
+      <c r="H21" s="52">
+        <v>0</v>
+      </c>
       <c r="I21" s="52"/>
       <c r="J21" s="52"/>
       <c r="K21" s="46">
@@ -2838,10 +2967,10 @@
       </c>
       <c r="L21" s="16">
         <f>SUM(D21:J21)*50/(A$1-K21)</f>
-        <v>86.666666666666671</v>
+        <v>75</v>
       </c>
       <c r="M21" s="14">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
@@ -2849,27 +2978,32 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="16">
         <f>SUM(M21:Q21)/A$1</f>
-        <v>26.666666666666668</v>
-      </c>
-      <c r="S21" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S21" s="14">
+        <v>0</v>
+      </c>
       <c r="T21" s="14"/>
-      <c r="U21" s="16"/>
+      <c r="U21" s="16">
+        <f>SUM(S21:T21)/1</f>
+        <v>0</v>
+      </c>
       <c r="V21" s="6"/>
       <c r="W21" s="44"/>
       <c r="X21" s="21">
         <f>L21*0.2+R21*0.25+U21*0.25+V21*0.3+W21*0.15</f>
-        <v>24.000000000000004</v>
+        <v>21.25</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D22" s="54">
         <v>0</v>
@@ -2880,21 +3014,23 @@
       <c r="F22" s="53">
         <v>2</v>
       </c>
-      <c r="G22" s="53">
-        <v>2</v>
-      </c>
-      <c r="H22" s="53"/>
+      <c r="G22" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="H22" s="53">
+        <v>2</v>
+      </c>
       <c r="I22" s="53"/>
       <c r="J22" s="53"/>
       <c r="K22" s="46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="16">
         <f>SUM(D22:J22)*50/(A$1-K22)</f>
         <v>66.666666666666671</v>
       </c>
       <c r="M22" s="14">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
@@ -2902,27 +3038,32 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="16">
         <f>SUM(M22:Q22)/A$1</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="S22" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="S22" s="14">
+        <v>0</v>
+      </c>
       <c r="T22" s="14"/>
-      <c r="U22" s="16"/>
+      <c r="U22" s="16">
+        <f>SUM(S22:T22)/1</f>
+        <v>0</v>
+      </c>
       <c r="V22" s="6"/>
       <c r="W22" s="44"/>
       <c r="X22" s="21">
         <f>L22*0.2+R22*0.25+U22*0.25+V22*0.3+W22*0.1</f>
-        <v>21.666666666666671</v>
+        <v>18.333333333333336</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="D23" s="51">
         <v>0</v>
@@ -2931,12 +3072,14 @@
         <v>2</v>
       </c>
       <c r="F23" s="52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" s="52">
-        <v>2</v>
-      </c>
-      <c r="H23" s="52"/>
+        <v>1.2</v>
+      </c>
+      <c r="H23" s="52">
+        <v>0</v>
+      </c>
       <c r="I23" s="52"/>
       <c r="J23" s="52"/>
       <c r="K23" s="46">
@@ -2944,10 +3087,10 @@
       </c>
       <c r="L23" s="16">
         <f>SUM(D23:J23)*50/(A$1-K23)</f>
-        <v>83.333333333333329</v>
+        <v>65</v>
       </c>
       <c r="M23" s="14">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
@@ -2955,52 +3098,59 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="16">
         <f>SUM(M23:Q23)/A$1</f>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="S23" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="S23" s="14">
+        <v>0</v>
+      </c>
       <c r="T23" s="14"/>
-      <c r="U23" s="16"/>
+      <c r="U23" s="16">
+        <f>SUM(S23:T23)/1</f>
+        <v>0</v>
+      </c>
       <c r="V23" s="6"/>
       <c r="W23" s="44"/>
       <c r="X23" s="21">
         <f>L23*0.2+R23*0.25+U23*0.25+V23*0.3+W23*0.15</f>
-        <v>20.833333333333336</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>132</v>
+        <v>191</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" s="51">
-        <v>2</v>
-      </c>
-      <c r="E24" s="52">
-        <v>1.7</v>
-      </c>
-      <c r="F24" s="52">
-        <v>0</v>
-      </c>
-      <c r="G24" s="52">
-        <v>2</v>
-      </c>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
+        <v>12</v>
+      </c>
+      <c r="D24" s="54">
+        <v>0</v>
+      </c>
+      <c r="E24" s="53">
+        <v>0</v>
+      </c>
+      <c r="F24" s="53">
+        <v>2</v>
+      </c>
+      <c r="G24" s="53">
+        <v>2</v>
+      </c>
+      <c r="H24" s="53">
+        <v>0</v>
+      </c>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
       <c r="K24" s="46">
         <v>0</v>
       </c>
       <c r="L24" s="16">
         <f>SUM(D24:J24)*50/(A$1-K24)</f>
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="M24" s="14">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
@@ -3008,52 +3158,59 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="16">
         <f>SUM(M24:Q24)/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="S24" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="S24" s="14">
+        <v>0</v>
+      </c>
       <c r="T24" s="14"/>
-      <c r="U24" s="16"/>
+      <c r="U24" s="16">
+        <f>SUM(S24:T24)/1</f>
+        <v>0</v>
+      </c>
       <c r="V24" s="6"/>
       <c r="W24" s="44"/>
       <c r="X24" s="21">
-        <f>L24*0.2+R24*0.25+U24*0.25+V24*0.3+W24*0.15</f>
-        <v>19</v>
+        <f>L24*0.2+R24*0.25+U24*0.25+V24*0.3+W24*0.1</f>
+        <v>16.25</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>184</v>
+        <v>133</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="54">
-        <v>0</v>
-      </c>
-      <c r="E25" s="53">
-        <v>0</v>
-      </c>
-      <c r="F25" s="53">
-        <v>2</v>
-      </c>
-      <c r="G25" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
+        <v>134</v>
+      </c>
+      <c r="D25" s="51">
+        <v>2</v>
+      </c>
+      <c r="E25" s="52">
+        <v>1.7</v>
+      </c>
+      <c r="F25" s="52">
+        <v>0</v>
+      </c>
+      <c r="G25" s="52">
+        <v>2</v>
+      </c>
+      <c r="H25" s="52">
+        <v>0</v>
+      </c>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
       <c r="K25" s="46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="16">
         <f>SUM(D25:J25)*50/(A$1-K25)</f>
-        <v>50</v>
+        <v>71.25</v>
       </c>
       <c r="M25" s="14">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
@@ -3061,16 +3218,21 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="16">
         <f>SUM(M25:Q25)/A$1</f>
-        <v>26.666666666666668</v>
-      </c>
-      <c r="S25" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="S25" s="14">
+        <v>0</v>
+      </c>
       <c r="T25" s="14"/>
-      <c r="U25" s="16"/>
+      <c r="U25" s="16">
+        <f>SUM(S25:T25)/1</f>
+        <v>0</v>
+      </c>
       <c r="V25" s="6"/>
       <c r="W25" s="44"/>
       <c r="X25" s="21">
-        <f>L25*0.2+R25*0.25+U25*0.25+V25*0.3+W25*0.1</f>
-        <v>16.666666666666668</v>
+        <f>L25*0.2+R25*0.25+U25*0.25+V25*0.3+W25*0.15</f>
+        <v>14.25</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3095,7 +3257,9 @@
       <c r="G26" s="52">
         <v>2</v>
       </c>
-      <c r="H26" s="52"/>
+      <c r="H26" s="52">
+        <v>0</v>
+      </c>
       <c r="I26" s="52"/>
       <c r="J26" s="52"/>
       <c r="K26" s="46">
@@ -3103,7 +3267,7 @@
       </c>
       <c r="L26" s="16">
         <f>SUM(D26:J26)*50/(A$1-K26)</f>
-        <v>58.333333333333336</v>
+        <v>43.75</v>
       </c>
       <c r="M26" s="14">
         <v>50</v>
@@ -3114,638 +3278,660 @@
       <c r="Q26" s="6"/>
       <c r="R26" s="16">
         <f>SUM(M26:Q26)/A$1</f>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="S26" s="14"/>
+        <v>12.5</v>
+      </c>
+      <c r="S26" s="14">
+        <v>0</v>
+      </c>
       <c r="T26" s="14"/>
-      <c r="U26" s="16"/>
+      <c r="U26" s="16">
+        <f>SUM(S26:T26)/1</f>
+        <v>0</v>
+      </c>
       <c r="V26" s="6"/>
       <c r="W26" s="44"/>
       <c r="X26" s="21">
         <f>L26*0.2+R26*0.25+U26*0.25+V26*0.3+W26*0.15</f>
-        <v>15.833333333333336</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="61" t="s">
+        <v>11.875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="54">
+        <v>0</v>
+      </c>
+      <c r="E27" s="53">
+        <v>0</v>
+      </c>
+      <c r="F27" s="53">
+        <v>0</v>
+      </c>
+      <c r="G27" s="53">
+        <v>0</v>
+      </c>
+      <c r="H27" s="53">
+        <v>1.7</v>
+      </c>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="46">
+        <v>0</v>
+      </c>
+      <c r="L27" s="16">
+        <f>SUM(D27:J27)*50/(A$1-K27)</f>
+        <v>21.25</v>
+      </c>
+      <c r="M27" s="14">
+        <v>0</v>
+      </c>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="16">
+        <f>SUM(M27:Q27)/A$1</f>
+        <v>0</v>
+      </c>
+      <c r="S27" s="14">
+        <v>0</v>
+      </c>
+      <c r="T27" s="14"/>
+      <c r="U27" s="16">
+        <f>SUM(S27:T27)/1</f>
+        <v>0</v>
+      </c>
+      <c r="V27" s="6"/>
+      <c r="W27" s="44"/>
+      <c r="X27" s="21">
+        <f>L27*0.2+R27*0.25+U27*0.25+V27*0.3+W27*0.1</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="62" t="s">
+      <c r="B28" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="63" t="s">
+      <c r="C28" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="66">
-        <v>0</v>
-      </c>
-      <c r="L27" s="67">
-        <f>SUM(D27:J27)*50/(A$1-K27)</f>
-        <v>0</v>
-      </c>
-      <c r="M27" s="68"/>
-      <c r="N27" s="69"/>
-      <c r="O27" s="69"/>
-      <c r="P27" s="69"/>
-      <c r="Q27" s="69"/>
-      <c r="R27" s="67"/>
-      <c r="S27" s="68"/>
-      <c r="T27" s="68"/>
-      <c r="U27" s="67"/>
-      <c r="V27" s="69"/>
-      <c r="W27" s="70"/>
-      <c r="X27" s="71">
-        <f>L27*0.2+R27*0.25+U27*0.25+V27*0.3+W27*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="61" t="s">
+      <c r="D28" s="61"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="63">
+        <v>0</v>
+      </c>
+      <c r="L28" s="64">
+        <f>SUM(D28:J28)*50/(A$1-K28)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="65"/>
+      <c r="N28" s="66"/>
+      <c r="O28" s="66"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="64"/>
+      <c r="S28" s="65"/>
+      <c r="T28" s="65"/>
+      <c r="U28" s="64"/>
+      <c r="V28" s="66"/>
+      <c r="W28" s="67"/>
+      <c r="X28" s="68">
+        <f>L28*0.2+R28*0.25+U28*0.25+V28*0.3+W28*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" s="70" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="62" t="s">
+      <c r="B29" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="63" t="s">
+      <c r="C29" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="66">
-        <v>0</v>
-      </c>
-      <c r="L28" s="67">
-        <f>SUM(D28:J28)*50/(A$1-K28)</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="68"/>
-      <c r="N28" s="69"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="69"/>
-      <c r="Q28" s="69"/>
-      <c r="R28" s="67"/>
-      <c r="S28" s="68"/>
-      <c r="T28" s="68"/>
-      <c r="U28" s="67"/>
-      <c r="V28" s="69"/>
-      <c r="W28" s="70"/>
-      <c r="X28" s="71">
-        <f>L28*0.2+R28*0.25+U28*0.25+V28*0.3+W28*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" s="73" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="61" t="s">
+      <c r="D29" s="61"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="63">
+        <v>0</v>
+      </c>
+      <c r="L29" s="64">
+        <f>SUM(D29:J29)*50/(A$1-K29)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="65"/>
+      <c r="N29" s="66"/>
+      <c r="O29" s="66"/>
+      <c r="P29" s="66"/>
+      <c r="Q29" s="66"/>
+      <c r="R29" s="64"/>
+      <c r="S29" s="65"/>
+      <c r="T29" s="65"/>
+      <c r="U29" s="64"/>
+      <c r="V29" s="66"/>
+      <c r="W29" s="67"/>
+      <c r="X29" s="68">
+        <f>L29*0.2+R29*0.25+U29*0.25+V29*0.3+W29*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="62" t="s">
+      <c r="B30" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="63" t="s">
+      <c r="C30" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="65"/>
-      <c r="K29" s="66">
-        <v>0</v>
-      </c>
-      <c r="L29" s="67">
-        <f>SUM(D29:J29)*50/(A$1-K29)</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="68"/>
-      <c r="N29" s="69"/>
-      <c r="O29" s="69"/>
-      <c r="P29" s="69"/>
-      <c r="Q29" s="69"/>
-      <c r="R29" s="67"/>
-      <c r="S29" s="68"/>
-      <c r="T29" s="68"/>
-      <c r="U29" s="67"/>
-      <c r="V29" s="69"/>
-      <c r="W29" s="70"/>
-      <c r="X29" s="71">
-        <f>L29*0.2+R29*0.25+U29*0.25+V29*0.3+W29*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="61" t="s">
+      <c r="D30" s="61"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="63">
+        <v>0</v>
+      </c>
+      <c r="L30" s="64">
+        <f>SUM(D30:J30)*50/(A$1-K30)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="65"/>
+      <c r="N30" s="66"/>
+      <c r="O30" s="66"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="66"/>
+      <c r="R30" s="64"/>
+      <c r="S30" s="65"/>
+      <c r="T30" s="65"/>
+      <c r="U30" s="64"/>
+      <c r="V30" s="66"/>
+      <c r="W30" s="67"/>
+      <c r="X30" s="68">
+        <f>L30*0.2+R30*0.25+U30*0.25+V30*0.3+W30*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="62" t="s">
+      <c r="B31" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C31" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="66">
-        <v>0</v>
-      </c>
-      <c r="L30" s="67">
-        <f>SUM(D30:J30)*50/(A$1-K30)</f>
-        <v>0</v>
-      </c>
-      <c r="M30" s="68"/>
-      <c r="N30" s="69"/>
-      <c r="O30" s="69"/>
-      <c r="P30" s="69"/>
-      <c r="Q30" s="69"/>
-      <c r="R30" s="67"/>
-      <c r="S30" s="68"/>
-      <c r="T30" s="68"/>
-      <c r="U30" s="67"/>
-      <c r="V30" s="69"/>
-      <c r="W30" s="70"/>
-      <c r="X30" s="71">
-        <f>L30*0.2+R30*0.25+U30*0.25+V30*0.3+W30*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="61" t="s">
+      <c r="D31" s="61"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
+      <c r="K31" s="63">
+        <v>0</v>
+      </c>
+      <c r="L31" s="64">
+        <f>SUM(D31:J31)*50/(A$1-K31)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="65"/>
+      <c r="N31" s="66"/>
+      <c r="O31" s="66"/>
+      <c r="P31" s="66"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="64"/>
+      <c r="S31" s="65"/>
+      <c r="T31" s="65"/>
+      <c r="U31" s="64"/>
+      <c r="V31" s="66"/>
+      <c r="W31" s="67"/>
+      <c r="X31" s="68">
+        <f>L31*0.2+R31*0.25+U31*0.25+V31*0.3+W31*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="62" t="s">
+      <c r="B32" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C32" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="66">
-        <v>0</v>
-      </c>
-      <c r="L31" s="67">
-        <f>SUM(D31:J31)*50/(A$1-K31)</f>
-        <v>0</v>
-      </c>
-      <c r="M31" s="68"/>
-      <c r="N31" s="69"/>
-      <c r="O31" s="69"/>
-      <c r="P31" s="69"/>
-      <c r="Q31" s="69"/>
-      <c r="R31" s="67"/>
-      <c r="S31" s="68"/>
-      <c r="T31" s="68"/>
-      <c r="U31" s="67"/>
-      <c r="V31" s="69"/>
-      <c r="W31" s="70"/>
-      <c r="X31" s="71">
-        <f>L31*0.2+R31*0.25+U31*0.25+V31*0.3+W31*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="61" t="s">
+      <c r="D32" s="61"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="63">
+        <v>0</v>
+      </c>
+      <c r="L32" s="64">
+        <f>SUM(D32:J32)*50/(A$1-K32)</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="65"/>
+      <c r="N32" s="66"/>
+      <c r="O32" s="66"/>
+      <c r="P32" s="66"/>
+      <c r="Q32" s="66"/>
+      <c r="R32" s="64"/>
+      <c r="S32" s="65"/>
+      <c r="T32" s="65"/>
+      <c r="U32" s="64"/>
+      <c r="V32" s="66"/>
+      <c r="W32" s="67"/>
+      <c r="X32" s="68">
+        <f>L32*0.2+R32*0.25+U32*0.25+V32*0.3+W32*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="B32" s="62" t="s">
+      <c r="B33" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="63" t="s">
+      <c r="C33" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="D32" s="64"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="66">
-        <v>0</v>
-      </c>
-      <c r="L32" s="67">
-        <f>SUM(D32:J32)*50/(A$1-K32)</f>
-        <v>0</v>
-      </c>
-      <c r="M32" s="68"/>
-      <c r="N32" s="69"/>
-      <c r="O32" s="69"/>
-      <c r="P32" s="69"/>
-      <c r="Q32" s="69"/>
-      <c r="R32" s="67"/>
-      <c r="S32" s="68"/>
-      <c r="T32" s="68"/>
-      <c r="U32" s="67"/>
-      <c r="V32" s="69"/>
-      <c r="W32" s="70"/>
-      <c r="X32" s="71">
-        <f>L32*0.2+R32*0.25+U32*0.25+V32*0.3+W32*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="61" t="s">
+      <c r="D33" s="61"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="63">
+        <v>0</v>
+      </c>
+      <c r="L33" s="64">
+        <f>SUM(D33:J33)*50/(A$1-K33)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="65"/>
+      <c r="N33" s="66"/>
+      <c r="O33" s="66"/>
+      <c r="P33" s="66"/>
+      <c r="Q33" s="66"/>
+      <c r="R33" s="64"/>
+      <c r="S33" s="65"/>
+      <c r="T33" s="65"/>
+      <c r="U33" s="64"/>
+      <c r="V33" s="66"/>
+      <c r="W33" s="67"/>
+      <c r="X33" s="68">
+        <f>L33*0.2+R33*0.25+U33*0.25+V33*0.3+W33*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="B33" s="62" t="s">
+      <c r="B34" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="C33" s="63" t="s">
+      <c r="C34" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="D33" s="64"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="65"/>
-      <c r="J33" s="65"/>
-      <c r="K33" s="66">
-        <v>0</v>
-      </c>
-      <c r="L33" s="67">
-        <f>SUM(D33:J33)*50/(A$1-K33)</f>
-        <v>0</v>
-      </c>
-      <c r="M33" s="68"/>
-      <c r="N33" s="69"/>
-      <c r="O33" s="69"/>
-      <c r="P33" s="69"/>
-      <c r="Q33" s="69"/>
-      <c r="R33" s="67"/>
-      <c r="S33" s="68"/>
-      <c r="T33" s="68"/>
-      <c r="U33" s="67"/>
-      <c r="V33" s="69"/>
-      <c r="W33" s="70"/>
-      <c r="X33" s="71">
-        <f>L33*0.2+R33*0.25+U33*0.25+V33*0.3+W33*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="61" t="s">
+      <c r="D34" s="61"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="63">
+        <v>0</v>
+      </c>
+      <c r="L34" s="64">
+        <f>SUM(D34:J34)*50/(A$1-K34)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="65"/>
+      <c r="N34" s="66"/>
+      <c r="O34" s="66"/>
+      <c r="P34" s="66"/>
+      <c r="Q34" s="66"/>
+      <c r="R34" s="64"/>
+      <c r="S34" s="65"/>
+      <c r="T34" s="65"/>
+      <c r="U34" s="64"/>
+      <c r="V34" s="66"/>
+      <c r="W34" s="67"/>
+      <c r="X34" s="68">
+        <f>L34*0.2+R34*0.25+U34*0.25+V34*0.3+W34*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="62" t="s">
+      <c r="B35" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="63" t="s">
+      <c r="C35" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="64"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="66">
-        <v>0</v>
-      </c>
-      <c r="L34" s="67">
-        <f>SUM(D34:J34)*50/(A$1-K34)</f>
-        <v>0</v>
-      </c>
-      <c r="M34" s="68"/>
-      <c r="N34" s="69"/>
-      <c r="O34" s="69"/>
-      <c r="P34" s="69"/>
-      <c r="Q34" s="69"/>
-      <c r="R34" s="67">
-        <f>SUM(M34:Q34)/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="S34" s="68"/>
-      <c r="T34" s="68"/>
-      <c r="U34" s="67"/>
-      <c r="V34" s="69"/>
-      <c r="W34" s="70"/>
-      <c r="X34" s="71">
-        <f>L34*0.2+R34*0.25+U34*0.25+V34*0.3+W34*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="61" t="s">
+      <c r="D35" s="61"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="63">
+        <v>0</v>
+      </c>
+      <c r="L35" s="64">
+        <f>SUM(D35:J35)*50/(A$1-K35)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="65"/>
+      <c r="N35" s="66"/>
+      <c r="O35" s="66"/>
+      <c r="P35" s="66"/>
+      <c r="Q35" s="66"/>
+      <c r="R35" s="64">
+        <f>SUM(M35:Q35)/A$1</f>
+        <v>0</v>
+      </c>
+      <c r="S35" s="65"/>
+      <c r="T35" s="65"/>
+      <c r="U35" s="64"/>
+      <c r="V35" s="66"/>
+      <c r="W35" s="67"/>
+      <c r="X35" s="68">
+        <f>L35*0.2+R35*0.25+U35*0.25+V35*0.3+W35*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="62" t="s">
+      <c r="B36" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="63" t="s">
+      <c r="C36" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="65"/>
-      <c r="J35" s="65"/>
-      <c r="K35" s="66">
-        <v>0</v>
-      </c>
-      <c r="L35" s="67">
-        <f>SUM(D35:J35)*50/(A$1-K35)</f>
-        <v>0</v>
-      </c>
-      <c r="M35" s="68"/>
-      <c r="N35" s="69"/>
-      <c r="O35" s="69"/>
-      <c r="P35" s="69"/>
-      <c r="Q35" s="69"/>
-      <c r="R35" s="67">
-        <f>SUM(M35:Q35)/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="S35" s="68"/>
-      <c r="T35" s="68"/>
-      <c r="U35" s="67"/>
-      <c r="V35" s="69"/>
-      <c r="W35" s="70"/>
-      <c r="X35" s="71">
-        <f>L35*0.2+R35*0.25+U35*0.25+V35*0.3+W35*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="61" t="s">
+      <c r="D36" s="61"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="63">
+        <v>0</v>
+      </c>
+      <c r="L36" s="64">
+        <f>SUM(D36:J36)*50/(A$1-K36)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="65"/>
+      <c r="N36" s="66"/>
+      <c r="O36" s="66"/>
+      <c r="P36" s="66"/>
+      <c r="Q36" s="66"/>
+      <c r="R36" s="64">
+        <f>SUM(M36:Q36)/A$1</f>
+        <v>0</v>
+      </c>
+      <c r="S36" s="65"/>
+      <c r="T36" s="65"/>
+      <c r="U36" s="64"/>
+      <c r="V36" s="66"/>
+      <c r="W36" s="67"/>
+      <c r="X36" s="68">
+        <f>L36*0.2+R36*0.25+U36*0.25+V36*0.3+W36*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="B36" s="62" t="s">
+      <c r="B37" s="59" t="s">
         <v>154</v>
       </c>
-      <c r="C36" s="63" t="s">
+      <c r="C37" s="60" t="s">
         <v>155</v>
       </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="65"/>
-      <c r="K36" s="66">
-        <v>0</v>
-      </c>
-      <c r="L36" s="67">
-        <f>SUM(D36:J36)*50/(A$1-K36)</f>
-        <v>0</v>
-      </c>
-      <c r="M36" s="68"/>
-      <c r="N36" s="69"/>
-      <c r="O36" s="69"/>
-      <c r="P36" s="69"/>
-      <c r="Q36" s="69"/>
-      <c r="R36" s="67">
-        <f>SUM(M36:Q36)/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="S36" s="68"/>
-      <c r="T36" s="68"/>
-      <c r="U36" s="67"/>
-      <c r="V36" s="69"/>
-      <c r="W36" s="70"/>
-      <c r="X36" s="71">
-        <f>L36*0.2+R36*0.25+U36*0.25+V36*0.3+W36*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="61" t="s">
+      <c r="D37" s="61"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="63">
+        <v>0</v>
+      </c>
+      <c r="L37" s="64">
+        <f>SUM(D37:J37)*50/(A$1-K37)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="65"/>
+      <c r="N37" s="66"/>
+      <c r="O37" s="66"/>
+      <c r="P37" s="66"/>
+      <c r="Q37" s="66"/>
+      <c r="R37" s="64">
+        <f>SUM(M37:Q37)/A$1</f>
+        <v>0</v>
+      </c>
+      <c r="S37" s="65"/>
+      <c r="T37" s="65"/>
+      <c r="U37" s="64"/>
+      <c r="V37" s="66"/>
+      <c r="W37" s="67"/>
+      <c r="X37" s="68">
+        <f>L37*0.2+R37*0.25+U37*0.25+V37*0.3+W37*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="62" t="s">
+      <c r="B38" s="59" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="63" t="s">
+      <c r="C38" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="65"/>
-      <c r="K37" s="66">
-        <v>0</v>
-      </c>
-      <c r="L37" s="67">
-        <f>SUM(D37:J37)*50/(A$1-K37)</f>
-        <v>0</v>
-      </c>
-      <c r="M37" s="68"/>
-      <c r="N37" s="69"/>
-      <c r="O37" s="69"/>
-      <c r="P37" s="69"/>
-      <c r="Q37" s="69"/>
-      <c r="R37" s="67">
-        <f>SUM(M37:Q37)/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="S37" s="68"/>
-      <c r="T37" s="68"/>
-      <c r="U37" s="67"/>
-      <c r="V37" s="69"/>
-      <c r="W37" s="70"/>
-      <c r="X37" s="71">
-        <f>L37*0.2+R37*0.25+U37*0.25+V37*0.3+W37*0.1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="61" t="s">
+      <c r="D38" s="61"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="62"/>
+      <c r="K38" s="63">
+        <v>0</v>
+      </c>
+      <c r="L38" s="64">
+        <f>SUM(D38:J38)*50/(A$1-K38)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="65"/>
+      <c r="N38" s="66"/>
+      <c r="O38" s="66"/>
+      <c r="P38" s="66"/>
+      <c r="Q38" s="66"/>
+      <c r="R38" s="64">
+        <f>SUM(M38:Q38)/A$1</f>
+        <v>0</v>
+      </c>
+      <c r="S38" s="65"/>
+      <c r="T38" s="65"/>
+      <c r="U38" s="64"/>
+      <c r="V38" s="66"/>
+      <c r="W38" s="67"/>
+      <c r="X38" s="68">
+        <f>L38*0.2+R38*0.25+U38*0.25+V38*0.3+W38*0.1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="B38" s="62" t="s">
+      <c r="B39" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="63" t="s">
+      <c r="C39" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="64"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="65"/>
-      <c r="I38" s="65"/>
-      <c r="J38" s="65"/>
-      <c r="K38" s="66">
-        <v>0</v>
-      </c>
-      <c r="L38" s="67">
-        <f>SUM(D38:J38)*50/(A$1-K38)</f>
-        <v>0</v>
-      </c>
-      <c r="M38" s="68"/>
-      <c r="N38" s="69"/>
-      <c r="O38" s="69"/>
-      <c r="P38" s="69"/>
-      <c r="Q38" s="69"/>
-      <c r="R38" s="67">
-        <f>SUM(M38:Q38)/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="S38" s="68"/>
-      <c r="T38" s="68"/>
-      <c r="U38" s="67"/>
-      <c r="V38" s="69"/>
-      <c r="W38" s="70"/>
-      <c r="X38" s="71">
-        <f>L38*0.2+R38*0.25+U38*0.25+V38*0.3+W38*0.1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="61" t="s">
+      <c r="D39" s="61"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="62"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="63">
+        <v>0</v>
+      </c>
+      <c r="L39" s="64">
+        <f>SUM(D39:J39)*50/(A$1-K39)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="65"/>
+      <c r="N39" s="66"/>
+      <c r="O39" s="66"/>
+      <c r="P39" s="66"/>
+      <c r="Q39" s="66"/>
+      <c r="R39" s="64">
+        <f>SUM(M39:Q39)/A$1</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="65"/>
+      <c r="T39" s="65"/>
+      <c r="U39" s="64"/>
+      <c r="V39" s="66"/>
+      <c r="W39" s="67"/>
+      <c r="X39" s="68">
+        <f>L39*0.2+R39*0.25+U39*0.25+V39*0.3+W39*0.1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="58" t="s">
         <v>181</v>
       </c>
-      <c r="B39" s="62" t="s">
+      <c r="B40" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="C39" s="63" t="s">
+      <c r="C40" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="65"/>
-      <c r="I39" s="65"/>
-      <c r="J39" s="65"/>
-      <c r="K39" s="66">
-        <v>0</v>
-      </c>
-      <c r="L39" s="67">
-        <f>SUM(D39:J39)*50/(A$1-K39)</f>
-        <v>0</v>
-      </c>
-      <c r="M39" s="68"/>
-      <c r="N39" s="69"/>
-      <c r="O39" s="69"/>
-      <c r="P39" s="69"/>
-      <c r="Q39" s="69"/>
-      <c r="R39" s="67">
-        <f>SUM(M39:Q39)/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="S39" s="68"/>
-      <c r="T39" s="68"/>
-      <c r="U39" s="67"/>
-      <c r="V39" s="69"/>
-      <c r="W39" s="70"/>
-      <c r="X39" s="71">
-        <f>L39*0.2+R39*0.25+U39*0.25+V39*0.3+W39*0.1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="61" t="s">
+      <c r="D40" s="61"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="63">
+        <v>0</v>
+      </c>
+      <c r="L40" s="64">
+        <f>SUM(D40:J40)*50/(A$1-K40)</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="65"/>
+      <c r="N40" s="66"/>
+      <c r="O40" s="66"/>
+      <c r="P40" s="66"/>
+      <c r="Q40" s="66"/>
+      <c r="R40" s="64">
+        <f>SUM(M40:Q40)/A$1</f>
+        <v>0</v>
+      </c>
+      <c r="S40" s="65"/>
+      <c r="T40" s="65"/>
+      <c r="U40" s="64"/>
+      <c r="V40" s="66"/>
+      <c r="W40" s="67"/>
+      <c r="X40" s="68">
+        <f>L40*0.2+R40*0.25+U40*0.25+V40*0.3+W40*0.1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="B40" s="62" t="s">
+      <c r="B41" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="C40" s="63" t="s">
+      <c r="C41" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="D40" s="74"/>
-      <c r="E40" s="75"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="75"/>
-      <c r="H40" s="75"/>
-      <c r="I40" s="75"/>
-      <c r="J40" s="75"/>
-      <c r="K40" s="66">
-        <v>0</v>
-      </c>
-      <c r="L40" s="67">
-        <f>SUM(D40:J40)*50/(A$1-K40)</f>
-        <v>0</v>
-      </c>
-      <c r="M40" s="68"/>
-      <c r="N40" s="69"/>
-      <c r="O40" s="69"/>
-      <c r="P40" s="69"/>
-      <c r="Q40" s="69"/>
-      <c r="R40" s="67">
-        <f>SUM(M40:Q40)/A$1</f>
-        <v>0</v>
-      </c>
-      <c r="S40" s="68"/>
-      <c r="T40" s="68"/>
-      <c r="U40" s="67"/>
-      <c r="V40" s="69"/>
-      <c r="W40" s="70"/>
-      <c r="X40" s="71">
-        <f>L40*0.2+R40*0.25+U40*0.25+V40*0.3+W40*0.1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" s="72" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="61" t="s">
-        <v>124</v>
-      </c>
-      <c r="B41" s="62" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" s="63" t="s">
-        <v>126</v>
-      </c>
-      <c r="D41" s="74"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="66">
-        <v>0</v>
-      </c>
-      <c r="L41" s="67">
+      <c r="D41" s="71"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="72"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="72"/>
+      <c r="I41" s="72"/>
+      <c r="J41" s="72"/>
+      <c r="K41" s="63">
+        <v>0</v>
+      </c>
+      <c r="L41" s="64">
         <f>SUM(D41:J41)*50/(A$1-K41)</f>
         <v>0</v>
       </c>
-      <c r="M41" s="68"/>
-      <c r="N41" s="69"/>
-      <c r="O41" s="69"/>
-      <c r="P41" s="69"/>
-      <c r="Q41" s="69"/>
-      <c r="R41" s="67">
+      <c r="M41" s="65"/>
+      <c r="N41" s="66"/>
+      <c r="O41" s="66"/>
+      <c r="P41" s="66"/>
+      <c r="Q41" s="66"/>
+      <c r="R41" s="64">
         <f>SUM(M41:Q41)/A$1</f>
         <v>0</v>
       </c>
-      <c r="S41" s="68"/>
-      <c r="T41" s="68"/>
-      <c r="U41" s="67"/>
-      <c r="V41" s="69"/>
-      <c r="W41" s="70"/>
-      <c r="X41" s="71">
+      <c r="S41" s="65"/>
+      <c r="T41" s="65"/>
+      <c r="U41" s="64"/>
+      <c r="V41" s="66"/>
+      <c r="W41" s="67"/>
+      <c r="X41" s="68">
         <f>L41*0.2+R41*0.25+U41*0.25+V41*0.3+W41*0.1</f>
         <v>0</v>
       </c>
@@ -4469,22 +4655,22 @@
       <c r="B1" s="18"/>
       <c r="C1" s="34"/>
       <c r="D1" s="40"/>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="58" t="s">
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="60"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="75"/>
       <c r="Q1" s="33" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
Yazilim araclari final notlari
</commit_message>
<xml_diff>
--- a/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
+++ b/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="135">
   <si>
     <t>Adı</t>
   </si>
@@ -181,9 +181,6 @@
     <t>LAB ÇALIŞMALARI (%25)</t>
   </si>
   <si>
-    <t>FİNAL</t>
-  </si>
-  <si>
     <t>DERS NOTU</t>
   </si>
   <si>
@@ -193,12 +190,6 @@
     <t>BONUS (%15)</t>
   </si>
   <si>
-    <t>LAB ÇALIŞMALARI (%30)</t>
-  </si>
-  <si>
-    <t>SINAV (%50)</t>
-  </si>
-  <si>
     <t>ŞAHİN</t>
   </si>
   <si>
@@ -467,6 +458,21 @@
   </si>
   <si>
     <t>SINAV (%40)</t>
+  </si>
+  <si>
+    <t>Bütünleme</t>
+  </si>
+  <si>
+    <t>Geçti</t>
+  </si>
+  <si>
+    <t>SINAV (%55)</t>
+  </si>
+  <si>
+    <t>Kaldı</t>
+  </si>
+  <si>
+    <t>FİNAL (+14 bonus)</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1025,45 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1568,14 +1612,14 @@
       <c r="P1" s="79"/>
       <c r="Q1" s="78"/>
       <c r="R1" s="77" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="S1" s="78"/>
       <c r="T1" s="14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="U1" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V1" s="16" t="s">
         <v>31</v>
@@ -1613,7 +1657,7 @@
         <v>7</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L2" s="23" t="s">
         <v>30</v>
@@ -1628,7 +1672,7 @@
         <v>7</v>
       </c>
       <c r="P2" s="63" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="Q2" s="23" t="s">
         <v>30</v>
@@ -1643,7 +1687,7 @@
         <v>33</v>
       </c>
       <c r="U2" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V2" s="16" t="s">
         <v>32</v>
@@ -1651,13 +1695,13 @@
     </row>
     <row r="3" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3" s="41">
         <v>2</v>
@@ -1722,10 +1766,10 @@
     </row>
     <row r="4" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>34</v>
@@ -1793,13 +1837,13 @@
     </row>
     <row r="5" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" s="41">
         <v>2</v>
@@ -1811,7 +1855,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H5" s="42">
         <v>2</v>
@@ -1864,13 +1908,13 @@
     </row>
     <row r="6" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D6" s="41">
         <v>2</v>
@@ -1935,13 +1979,13 @@
     </row>
     <row r="7" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D7" s="41">
         <v>2</v>
@@ -2006,13 +2050,13 @@
     </row>
     <row r="8" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D8" s="41">
         <v>0</v>
@@ -2077,13 +2121,13 @@
     </row>
     <row r="9" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D9" s="41">
         <v>2</v>
@@ -2148,13 +2192,13 @@
     </row>
     <row r="10" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10" s="41">
         <v>2</v>
@@ -2175,7 +2219,7 @@
         <v>2</v>
       </c>
       <c r="J10" s="42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K10" s="36">
         <v>0</v>
@@ -2191,7 +2235,7 @@
         <v>95</v>
       </c>
       <c r="O10" s="70" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="P10" s="64">
         <v>1</v>
@@ -2219,10 +2263,10 @@
     </row>
     <row r="11" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>25</v>
@@ -2290,13 +2334,13 @@
     </row>
     <row r="12" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D12" s="41">
         <v>2</v>
@@ -2361,13 +2405,13 @@
     </row>
     <row r="13" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D13" s="41">
         <v>2</v>
@@ -2432,13 +2476,13 @@
     </row>
     <row r="14" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D14" s="41">
         <v>2</v>
@@ -2503,13 +2547,13 @@
     </row>
     <row r="15" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15" s="44">
         <v>0</v>
@@ -2574,13 +2618,13 @@
     </row>
     <row r="16" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D16" s="41">
         <v>2</v>
@@ -2645,13 +2689,13 @@
     </row>
     <row r="17" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D17" s="41">
         <v>2</v>
@@ -2716,13 +2760,13 @@
     </row>
     <row r="18" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D18" s="41">
         <v>0</v>
@@ -2787,13 +2831,13 @@
     </row>
     <row r="19" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D19" s="41">
         <v>0</v>
@@ -2808,7 +2852,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I19" s="42">
         <v>2</v>
@@ -2827,7 +2871,7 @@
         <v>100</v>
       </c>
       <c r="N19" s="65" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="O19" s="70">
         <v>85</v>
@@ -2858,13 +2902,13 @@
     </row>
     <row r="20" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D20" s="41">
         <v>0</v>
@@ -2879,7 +2923,7 @@
         <v>1.2</v>
       </c>
       <c r="H20" s="42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I20" s="42">
         <v>0</v>
@@ -2898,7 +2942,7 @@
         <v>80</v>
       </c>
       <c r="N20" s="65" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="O20" s="70">
         <v>80</v>
@@ -2950,7 +2994,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I21" s="43">
         <v>0</v>
@@ -2969,7 +3013,7 @@
         <v>80</v>
       </c>
       <c r="N21" s="65" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="O21" s="70">
         <v>80</v>
@@ -3000,13 +3044,13 @@
     </row>
     <row r="22" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D22" s="41">
         <v>2</v>
@@ -3071,13 +3115,13 @@
     </row>
     <row r="23" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D23" s="41">
         <v>2</v>
@@ -3092,7 +3136,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I23" s="42">
         <v>2</v>
@@ -3213,10 +3257,10 @@
     </row>
     <row r="25" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>6</v>
@@ -3231,13 +3275,13 @@
         <v>2</v>
       </c>
       <c r="G25" s="43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H25" s="43">
         <v>2</v>
       </c>
       <c r="I25" s="43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J25" s="43">
         <v>0</v>
@@ -3284,13 +3328,13 @@
     </row>
     <row r="26" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D26" s="41">
         <v>0</v>
@@ -3355,10 +3399,10 @@
     </row>
     <row r="27" spans="1:24" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>3</v>
@@ -3426,13 +3470,13 @@
     </row>
     <row r="28" spans="1:24" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D28" s="41"/>
       <c r="E28" s="42"/>
@@ -3468,13 +3512,13 @@
     </row>
     <row r="29" spans="1:24" s="60" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D29" s="44"/>
       <c r="E29" s="43"/>
@@ -3507,13 +3551,13 @@
     </row>
     <row r="30" spans="1:24" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D30" s="41"/>
       <c r="E30" s="42"/>
@@ -3549,7 +3593,7 @@
     </row>
     <row r="31" spans="1:24" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>21</v>
@@ -3626,13 +3670,13 @@
     </row>
     <row r="33" spans="1:22" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B33" s="49" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D33" s="51"/>
       <c r="E33" s="52"/>
@@ -3662,13 +3706,13 @@
     </row>
     <row r="34" spans="1:22" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B34" s="49" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D34" s="51"/>
       <c r="E34" s="52"/>
@@ -3743,7 +3787,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="49" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C36" s="50" t="s">
         <v>3</v>
@@ -3812,13 +3856,13 @@
     </row>
     <row r="38" spans="1:22" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B38" s="49" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D38" s="61"/>
       <c r="E38" s="62"/>
@@ -3926,10 +3970,10 @@
     </row>
     <row r="41" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B41" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C41" s="50" t="s">
         <v>5</v>
@@ -3962,13 +4006,13 @@
     </row>
     <row r="42" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B42" s="49" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C42" s="50" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D42" s="51"/>
       <c r="E42" s="52"/>
@@ -4447,47 +4491,47 @@
     <mergeCell ref="M1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:J42">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="19" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:O42 T3:U42">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R42">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="between">
       <formula>80</formula>
       <formula>200</formula>
     </cfRule>
@@ -4609,11 +4653,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
+      <selection pane="bottomLeft" activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4635,7 +4679,7 @@
     <col min="18" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25">
         <v>4</v>
       </c>
@@ -4653,7 +4697,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="77" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="L1" s="79"/>
       <c r="M1" s="79"/>
@@ -4661,16 +4705,16 @@
         <v>2</v>
       </c>
       <c r="O1" s="69" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="P1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>29</v>
       </c>
@@ -4696,7 +4740,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="73" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J2" s="23" t="s">
         <v>30</v>
@@ -4708,7 +4752,7 @@
         <v>9</v>
       </c>
       <c r="M2" s="73" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>30</v>
@@ -4723,18 +4767,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D3" s="18">
-        <v>95.833333333333343</v>
+        <v>82.275000000000006</v>
       </c>
       <c r="E3" s="29">
         <v>2</v>
@@ -4743,7 +4787,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="7">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="H3" s="7">
         <v>2</v>
@@ -4751,41 +4795,46 @@
       <c r="I3" s="36"/>
       <c r="J3" s="13">
         <f>SUM(E3:H3)*50/(J$1-I3)</f>
-        <v>92.5</v>
+        <v>87.5</v>
       </c>
       <c r="K3" s="12">
         <v>100</v>
       </c>
       <c r="L3" s="6">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="M3" s="36"/>
       <c r="N3" s="13">
         <f>SUM(K3:L3)/(N$1-M3)</f>
-        <v>95</v>
-      </c>
-      <c r="O3" s="6"/>
+        <v>97.5</v>
+      </c>
+      <c r="O3" s="6">
+        <v>80</v>
+      </c>
       <c r="P3" s="18">
-        <f>J3*0.2+N3*0.3+O3*0.5</f>
-        <v>47</v>
+        <f>J3*0.2+N3*0.25+O3*0.55+14</f>
+        <v>99.875</v>
       </c>
       <c r="Q3" s="18">
         <f>D3*0.4+P3*0.6</f>
-        <v>66.533333333333331</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>92.835000000000008</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>105</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>106</v>
+        <v>41</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>107</v>
+        <v>42</v>
       </c>
       <c r="D4" s="18">
-        <v>88.63333333333334</v>
+        <v>95.833333333333343</v>
       </c>
       <c r="E4" s="29">
         <v>2</v>
@@ -4794,49 +4843,54 @@
         <v>2</v>
       </c>
       <c r="G4" s="7">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="H4" s="7">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="I4" s="36"/>
       <c r="J4" s="13">
         <f>SUM(E4:H4)*50/(J$1-I4)</f>
-        <v>89.999999999999986</v>
+        <v>92.5</v>
       </c>
       <c r="K4" s="12">
         <v>100</v>
       </c>
       <c r="L4" s="6">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="M4" s="36"/>
       <c r="N4" s="13">
         <f>SUM(K4:L4)/(N$1-M4)</f>
-        <v>100</v>
-      </c>
-      <c r="O4" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="O4" s="6">
+        <v>54</v>
+      </c>
       <c r="P4" s="18">
-        <f>J4*0.2+N4*0.3+O4*0.5</f>
-        <v>48</v>
+        <f>J4*0.2+N4*0.25+O4*0.55+14</f>
+        <v>85.95</v>
       </c>
       <c r="Q4" s="18">
         <f>D4*0.4+P4*0.6</f>
-        <v>64.25333333333333</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89.903333333333336</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D5" s="18">
-        <v>85.15</v>
+        <v>88.63333333333334</v>
       </c>
       <c r="E5" s="29">
         <v>2</v>
@@ -4845,7 +4899,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="7">
-        <v>1.8</v>
+        <v>1.3</v>
       </c>
       <c r="H5" s="7">
         <v>1.9</v>
@@ -4853,7 +4907,7 @@
       <c r="I5" s="36"/>
       <c r="J5" s="13">
         <f>SUM(E5:H5)*50/(J$1-I5)</f>
-        <v>96.249999999999986</v>
+        <v>89.999999999999986</v>
       </c>
       <c r="K5" s="12">
         <v>100</v>
@@ -4866,37 +4920,42 @@
         <f>SUM(K5:L5)/(N$1-M5)</f>
         <v>100</v>
       </c>
-      <c r="O5" s="6"/>
+      <c r="O5" s="6">
+        <v>53</v>
+      </c>
       <c r="P5" s="18">
-        <f>J5*0.2+N5*0.3+O5*0.5</f>
-        <v>49.25</v>
+        <f>J5*0.2+N5*0.25+O5*0.55+14</f>
+        <v>86.15</v>
       </c>
       <c r="Q5" s="18">
         <f>D5*0.4+P5*0.6</f>
-        <v>63.61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>87.143333333333345</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D6" s="18">
-        <v>88.4</v>
+        <v>90.933333333333337</v>
       </c>
       <c r="E6" s="29">
         <v>2</v>
       </c>
       <c r="F6" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6" s="7">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="H6" s="7">
         <v>2</v>
@@ -4904,96 +4963,102 @@
       <c r="I6" s="36"/>
       <c r="J6" s="13">
         <f>SUM(E6:H6)*50/(J$1-I6)</f>
-        <v>92.5</v>
+        <v>75</v>
       </c>
       <c r="K6" s="12">
         <v>100</v>
       </c>
       <c r="L6" s="6">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="M6" s="36"/>
       <c r="N6" s="13">
         <f>SUM(K6:L6)/(N$1-M6)</f>
-        <v>95</v>
-      </c>
-      <c r="O6" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="O6" s="6">
+        <v>71</v>
+      </c>
       <c r="P6" s="18">
-        <f>J6*0.2+N6*0.3+O6*0.5</f>
-        <v>47</v>
+        <f>J6*0.2+N6*0.25+O6*0.55+14</f>
+        <v>80.550000000000011</v>
       </c>
       <c r="Q6" s="18">
         <f>D6*0.4+P6*0.6</f>
-        <v>63.56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>84.703333333333347</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>124</v>
+        <v>77</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="D7" s="18">
-        <v>81.349999999999994</v>
-      </c>
-      <c r="E7" s="74" t="s">
-        <v>127</v>
+        <v>73.716666666666669</v>
+      </c>
+      <c r="E7" s="29">
+        <v>2</v>
       </c>
       <c r="F7" s="7">
         <v>2</v>
       </c>
       <c r="G7" s="7">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="H7" s="7">
-        <v>1.9</v>
-      </c>
-      <c r="I7" s="36">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I7" s="36"/>
       <c r="J7" s="13">
         <f>SUM(E7:H7)*50/(J$1-I7)</f>
-        <v>93.333333333333329</v>
-      </c>
-      <c r="K7" s="75" t="s">
-        <v>127</v>
+        <v>100</v>
+      </c>
+      <c r="K7" s="12">
+        <v>100</v>
       </c>
       <c r="L7" s="6">
         <v>100</v>
       </c>
-      <c r="M7" s="36">
-        <v>1</v>
-      </c>
+      <c r="M7" s="36"/>
       <c r="N7" s="13">
         <f>SUM(K7:L7)/(N$1-M7)</f>
         <v>100</v>
       </c>
-      <c r="O7" s="6"/>
+      <c r="O7" s="6">
+        <v>60</v>
+      </c>
       <c r="P7" s="18">
-        <f>J7*0.2+N7*0.3+O7*0.5</f>
-        <v>48.666666666666671</v>
+        <f>J7*0.2+N7*0.25+O7*0.55+14</f>
+        <v>92</v>
       </c>
       <c r="Q7" s="18">
         <f>D7*0.4+P7*0.6</f>
-        <v>61.74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>84.686666666666667</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="D8" s="18">
-        <v>90.15</v>
+        <v>86.26666666666668</v>
       </c>
       <c r="E8" s="29">
         <v>2</v>
@@ -5002,49 +5067,54 @@
         <v>2</v>
       </c>
       <c r="G8" s="7">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="H8" s="7">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="I8" s="36"/>
       <c r="J8" s="13">
         <f>SUM(E8:H8)*50/(J$1-I8)</f>
-        <v>81.25</v>
+        <v>100</v>
       </c>
       <c r="K8" s="12">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="L8" s="6">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M8" s="36"/>
       <c r="N8" s="13">
         <f>SUM(K8:L8)/(N$1-M8)</f>
-        <v>87.5</v>
-      </c>
-      <c r="O8" s="6"/>
+        <v>72.5</v>
+      </c>
+      <c r="O8" s="6">
+        <v>37</v>
+      </c>
       <c r="P8" s="18">
-        <f>J8*0.2+N8*0.3+O8*0.5</f>
-        <v>42.5</v>
+        <f>J8*0.2+N8*0.25+O8*0.55+14</f>
+        <v>72.474999999999994</v>
       </c>
       <c r="Q8" s="18">
         <f>D8*0.4+P8*0.6</f>
-        <v>61.56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77.991666666666674</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="D9" s="18">
-        <v>82.275000000000006</v>
+        <v>85.15</v>
       </c>
       <c r="E9" s="29">
         <v>2</v>
@@ -5053,49 +5123,54 @@
         <v>2</v>
       </c>
       <c r="G9" s="7">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="H9" s="7">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="I9" s="36"/>
       <c r="J9" s="13">
         <f>SUM(E9:H9)*50/(J$1-I9)</f>
-        <v>87.5</v>
+        <v>96.249999999999986</v>
       </c>
       <c r="K9" s="12">
         <v>100</v>
       </c>
       <c r="L9" s="6">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="M9" s="36"/>
       <c r="N9" s="13">
         <f>SUM(K9:L9)/(N$1-M9)</f>
-        <v>97.5</v>
-      </c>
-      <c r="O9" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="O9" s="6">
+        <v>26</v>
+      </c>
       <c r="P9" s="18">
-        <f>J9*0.2+N9*0.3+O9*0.5</f>
-        <v>46.75</v>
+        <f>J9*0.2+N9*0.25+O9*0.55+14</f>
+        <v>72.55</v>
       </c>
       <c r="Q9" s="18">
         <f>D9*0.4+P9*0.6</f>
-        <v>60.960000000000008</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77.59</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D10" s="18">
-        <v>78.233333333333334</v>
+        <v>90.15</v>
       </c>
       <c r="E10" s="29">
         <v>2</v>
@@ -5104,18 +5179,18 @@
         <v>2</v>
       </c>
       <c r="G10" s="7">
-        <v>1.8</v>
+        <v>1.3</v>
       </c>
       <c r="H10" s="7">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="I10" s="36"/>
       <c r="J10" s="13">
         <f>SUM(E10:H10)*50/(J$1-I10)</f>
-        <v>88.75</v>
+        <v>81.25</v>
       </c>
       <c r="K10" s="12">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="L10" s="6">
         <v>100</v>
@@ -5123,81 +5198,95 @@
       <c r="M10" s="36"/>
       <c r="N10" s="13">
         <f>SUM(K10:L10)/(N$1-M10)</f>
-        <v>100</v>
-      </c>
-      <c r="O10" s="6"/>
+        <v>87.5</v>
+      </c>
+      <c r="O10" s="6">
+        <v>31</v>
+      </c>
       <c r="P10" s="18">
-        <f>J10*0.2+N10*0.3+O10*0.5</f>
-        <v>47.75</v>
+        <f>J10*0.2+N10*0.25+O10*0.55+14</f>
+        <v>69.174999999999997</v>
       </c>
       <c r="Q10" s="18">
         <f>D10*0.4+P10*0.6</f>
-        <v>59.943333333333335</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77.564999999999998</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="D11" s="18">
-        <v>86.26666666666668</v>
-      </c>
-      <c r="E11" s="29">
-        <v>2</v>
+        <v>81.349999999999994</v>
+      </c>
+      <c r="E11" s="74" t="s">
+        <v>124</v>
       </c>
       <c r="F11" s="7">
         <v>2</v>
       </c>
       <c r="G11" s="7">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="H11" s="7">
-        <v>2</v>
-      </c>
-      <c r="I11" s="36"/>
+        <v>1.9</v>
+      </c>
+      <c r="I11" s="36">
+        <v>1</v>
+      </c>
       <c r="J11" s="13">
         <f>SUM(E11:H11)*50/(J$1-I11)</f>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="K11" s="75" t="s">
+        <v>124</v>
+      </c>
+      <c r="L11" s="6">
         <v>100</v>
       </c>
-      <c r="K11" s="12">
-        <v>50</v>
-      </c>
-      <c r="L11" s="6">
-        <v>95</v>
-      </c>
-      <c r="M11" s="36"/>
+      <c r="M11" s="36">
+        <v>1</v>
+      </c>
       <c r="N11" s="13">
         <f>SUM(K11:L11)/(N$1-M11)</f>
-        <v>72.5</v>
-      </c>
-      <c r="O11" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="O11" s="6">
+        <v>31</v>
+      </c>
       <c r="P11" s="18">
-        <f>J11*0.2+N11*0.3+O11*0.5</f>
-        <v>41.75</v>
+        <f>J11*0.2+N11*0.25+O11*0.55+14</f>
+        <v>74.716666666666669</v>
       </c>
       <c r="Q11" s="18">
         <f>D11*0.4+P11*0.6</f>
-        <v>59.556666666666672</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77.37</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="D12" s="18">
-        <v>73.716666666666669</v>
+        <v>88.4</v>
       </c>
       <c r="E12" s="29">
         <v>2</v>
@@ -5206,7 +5295,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="7">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="H12" s="7">
         <v>2</v>
@@ -5214,44 +5303,49 @@
       <c r="I12" s="36"/>
       <c r="J12" s="13">
         <f>SUM(E12:H12)*50/(J$1-I12)</f>
-        <v>100</v>
+        <v>92.5</v>
       </c>
       <c r="K12" s="12">
         <v>100</v>
       </c>
       <c r="L12" s="6">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="M12" s="36"/>
       <c r="N12" s="13">
         <f>SUM(K12:L12)/(N$1-M12)</f>
-        <v>100</v>
-      </c>
-      <c r="O12" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="O12" s="6">
+        <v>24</v>
+      </c>
       <c r="P12" s="18">
-        <f>J12*0.2+N12*0.3+O12*0.5</f>
-        <v>50</v>
+        <f>J12*0.2+N12*0.25+O12*0.55+14</f>
+        <v>69.45</v>
       </c>
       <c r="Q12" s="18">
         <f>D12*0.4+P12*0.6</f>
-        <v>59.486666666666665</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77.03</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D13" s="18">
-        <v>75.366666666666674</v>
+        <v>78.233333333333334</v>
       </c>
       <c r="E13" s="29">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="F13" s="7">
         <v>2</v>
@@ -5260,12 +5354,12 @@
         <v>1.8</v>
       </c>
       <c r="H13" s="7">
-        <v>0.6</v>
+        <v>1.3</v>
       </c>
       <c r="I13" s="36"/>
       <c r="J13" s="13">
         <f>SUM(E13:H13)*50/(J$1-I13)</f>
-        <v>78.75</v>
+        <v>88.75</v>
       </c>
       <c r="K13" s="12">
         <v>100</v>
@@ -5278,181 +5372,201 @@
         <f>SUM(K13:L13)/(N$1-M13)</f>
         <v>100</v>
       </c>
-      <c r="O13" s="6"/>
+      <c r="O13" s="6">
+        <v>34</v>
+      </c>
       <c r="P13" s="18">
-        <f>J13*0.2+N13*0.3+O13*0.5</f>
-        <v>45.75</v>
+        <f>J13*0.2+N13*0.25+O13*0.55+14</f>
+        <v>75.45</v>
       </c>
       <c r="Q13" s="18">
         <f>D13*0.4+P13*0.6</f>
-        <v>57.596666666666671</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>76.563333333333333</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D14" s="18">
-        <v>75.983333333333334</v>
+        <v>79.033333333333331</v>
       </c>
       <c r="E14" s="29">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="F14" s="7">
         <v>2</v>
       </c>
       <c r="G14" s="7">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="H14" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I14" s="36"/>
       <c r="J14" s="13">
         <f>SUM(E14:H14)*50/(J$1-I14)</f>
-        <v>75</v>
+        <v>71.25</v>
       </c>
       <c r="K14" s="12">
         <v>100</v>
       </c>
       <c r="L14" s="6">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="M14" s="36"/>
       <c r="N14" s="13">
         <f>SUM(K14:L14)/(N$1-M14)</f>
-        <v>97.5</v>
-      </c>
-      <c r="O14" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="O14" s="6">
+        <v>46</v>
+      </c>
       <c r="P14" s="18">
-        <f>J14*0.2+N14*0.3+O14*0.5</f>
-        <v>44.25</v>
+        <f>J14*0.2+N14*0.25+O14*0.55+14</f>
+        <v>73.55</v>
       </c>
       <c r="Q14" s="18">
         <f>D14*0.4+P14*0.6</f>
-        <v>56.943333333333335</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75.743333333333325</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="D15" s="18">
-        <v>79.033333333333331</v>
+        <v>75.666666666666671</v>
       </c>
       <c r="E15" s="29">
-        <v>1.9</v>
+        <v>0</v>
       </c>
       <c r="F15" s="7">
         <v>2</v>
       </c>
       <c r="G15" s="7">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="H15" s="7">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="I15" s="36"/>
       <c r="J15" s="13">
         <f>SUM(E15:H15)*50/(J$1-I15)</f>
-        <v>71.25</v>
+        <v>40</v>
       </c>
       <c r="K15" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L15" s="6">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="M15" s="36"/>
       <c r="N15" s="13">
         <f>SUM(K15:L15)/(N$1-M15)</f>
-        <v>80</v>
-      </c>
-      <c r="O15" s="6"/>
+        <v>42.5</v>
+      </c>
+      <c r="O15" s="6">
+        <v>75</v>
+      </c>
       <c r="P15" s="18">
-        <f>J15*0.2+N15*0.3+O15*0.5</f>
-        <v>38.25</v>
+        <f>J15*0.2+N15*0.25+O15*0.55+14</f>
+        <v>73.875</v>
       </c>
       <c r="Q15" s="18">
         <f>D15*0.4+P15*0.6</f>
-        <v>54.563333333333333</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74.591666666666669</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D16" s="18">
-        <v>90.933333333333337</v>
+        <v>75.366666666666674</v>
       </c>
       <c r="E16" s="29">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="F16" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="7">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="H16" s="7">
-        <v>2</v>
+        <v>0.6</v>
       </c>
       <c r="I16" s="36"/>
       <c r="J16" s="13">
         <f>SUM(E16:H16)*50/(J$1-I16)</f>
-        <v>75</v>
+        <v>78.75</v>
       </c>
       <c r="K16" s="12">
         <v>100</v>
       </c>
       <c r="L16" s="6">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M16" s="36"/>
       <c r="N16" s="13">
         <f>SUM(K16:L16)/(N$1-M16)</f>
-        <v>50</v>
-      </c>
-      <c r="O16" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="O16" s="6">
+        <v>25</v>
+      </c>
       <c r="P16" s="18">
-        <f>J16*0.2+N16*0.3+O16*0.5</f>
-        <v>30</v>
+        <f>J16*0.2+N16*0.25+O16*0.55+14</f>
+        <v>68.5</v>
       </c>
       <c r="Q16" s="18">
         <f>D16*0.4+P16*0.6</f>
-        <v>54.373333333333335</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71.24666666666667</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="D17" s="18">
-        <v>42.533333333333339</v>
+        <v>75.983333333333334</v>
       </c>
       <c r="E17" s="29">
         <v>2</v>
@@ -5461,7 +5575,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="7">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="H17" s="7">
         <v>2</v>
@@ -5469,7 +5583,7 @@
       <c r="I17" s="36"/>
       <c r="J17" s="13">
         <f>SUM(E17:H17)*50/(J$1-I17)</f>
-        <v>97.5</v>
+        <v>75</v>
       </c>
       <c r="K17" s="12">
         <v>100</v>
@@ -5482,34 +5596,39 @@
         <f>SUM(K17:L17)/(N$1-M17)</f>
         <v>97.5</v>
       </c>
-      <c r="O17" s="6"/>
+      <c r="O17" s="6">
+        <v>23</v>
+      </c>
       <c r="P17" s="18">
-        <f>J17*0.2+N17*0.3+O17*0.5</f>
-        <v>48.75</v>
+        <f>J17*0.2+N17*0.25+O17*0.55+14</f>
+        <v>66.025000000000006</v>
       </c>
       <c r="Q17" s="18">
         <f>D17*0.4+P17*0.6</f>
-        <v>46.263333333333335</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>70.00833333333334</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D18" s="18">
-        <v>55.733333333333334</v>
+        <v>75.25</v>
       </c>
       <c r="E18" s="29">
         <v>2</v>
       </c>
       <c r="F18" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G18" s="7">
         <v>0</v>
@@ -5520,47 +5639,52 @@
       <c r="I18" s="36"/>
       <c r="J18" s="13">
         <f>SUM(E18:H18)*50/(J$1-I18)</f>
-        <v>68.75</v>
+        <v>43.75</v>
       </c>
       <c r="K18" s="12">
         <v>100</v>
       </c>
       <c r="L18" s="6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="M18" s="36"/>
       <c r="N18" s="13">
         <f>SUM(K18:L18)/(N$1-M18)</f>
-        <v>80</v>
-      </c>
-      <c r="O18" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="O18" s="6">
+        <v>44</v>
+      </c>
       <c r="P18" s="18">
-        <f>J18*0.2+N18*0.3+O18*0.5</f>
-        <v>37.75</v>
+        <f>J18*0.2+N18*0.25+O18*0.55+14</f>
+        <v>59.45</v>
       </c>
       <c r="Q18" s="18">
         <f>D18*0.4+P18*0.6</f>
-        <v>44.943333333333335</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65.77000000000001</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>112</v>
       </c>
       <c r="D19" s="18">
-        <v>75.25</v>
+        <v>55.733333333333334</v>
       </c>
       <c r="E19" s="29">
         <v>2</v>
       </c>
       <c r="F19" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19" s="7">
         <v>0</v>
@@ -5571,111 +5695,121 @@
       <c r="I19" s="36"/>
       <c r="J19" s="13">
         <f>SUM(E19:H19)*50/(J$1-I19)</f>
-        <v>43.75</v>
+        <v>68.75</v>
       </c>
       <c r="K19" s="12">
         <v>100</v>
       </c>
       <c r="L19" s="6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M19" s="36"/>
       <c r="N19" s="13">
         <f>SUM(K19:L19)/(N$1-M19)</f>
-        <v>50</v>
-      </c>
-      <c r="O19" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="O19" s="6">
+        <v>32</v>
+      </c>
       <c r="P19" s="18">
-        <f>J19*0.2+N19*0.3+O19*0.5</f>
-        <v>23.75</v>
+        <f>J19*0.2+N19*0.25+O19*0.55+14</f>
+        <v>65.349999999999994</v>
       </c>
       <c r="Q19" s="18">
         <f>D19*0.4+P19*0.6</f>
-        <v>44.35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61.50333333333333</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D20" s="18">
-        <v>75.666666666666671</v>
+        <v>70.325000000000003</v>
       </c>
       <c r="E20" s="29">
         <v>0</v>
       </c>
-      <c r="F20" s="7">
-        <v>2</v>
-      </c>
-      <c r="G20" s="7">
-        <v>0</v>
+      <c r="F20" s="32">
+        <v>2</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="H20" s="7">
-        <v>1.2</v>
-      </c>
-      <c r="I20" s="36"/>
+        <v>2</v>
+      </c>
+      <c r="I20" s="36">
+        <v>1</v>
+      </c>
       <c r="J20" s="13">
         <f>SUM(E20:H20)*50/(J$1-I20)</f>
-        <v>40</v>
+        <v>66.666666666666671</v>
       </c>
       <c r="K20" s="12">
         <v>0</v>
       </c>
       <c r="L20" s="6">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="M20" s="36"/>
       <c r="N20" s="13">
         <f>SUM(K20:L20)/(N$1-M20)</f>
-        <v>42.5</v>
-      </c>
-      <c r="O20" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="O20" s="6">
+        <v>36</v>
+      </c>
       <c r="P20" s="18">
-        <f>J20*0.2+N20*0.3+O20*0.5</f>
-        <v>20.75</v>
+        <f>J20*0.2+N20*0.25+O20*0.55+14</f>
+        <v>54.63333333333334</v>
       </c>
       <c r="Q20" s="18">
         <f>D20*0.4+P20*0.6</f>
-        <v>42.716666666666669</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60.910000000000004</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D21" s="18">
-        <v>70.325000000000003</v>
+        <v>67</v>
       </c>
       <c r="E21" s="29">
         <v>0</v>
       </c>
-      <c r="F21" s="32">
-        <v>2</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>127</v>
+      <c r="F21" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="G21" s="7">
+        <v>2</v>
       </c>
       <c r="H21" s="7">
-        <v>2</v>
-      </c>
-      <c r="I21" s="36">
-        <v>1</v>
-      </c>
+        <v>1.2</v>
+      </c>
+      <c r="I21" s="36"/>
       <c r="J21" s="13">
         <f>SUM(E21:H21)*50/(J$1-I21)</f>
-        <v>66.666666666666671</v>
+        <v>61.250000000000007</v>
       </c>
       <c r="K21" s="12">
         <v>0</v>
@@ -5688,76 +5822,86 @@
         <f>SUM(K21:L21)/(N$1-M21)</f>
         <v>30</v>
       </c>
-      <c r="O21" s="6"/>
+      <c r="O21" s="6">
+        <v>40</v>
+      </c>
       <c r="P21" s="18">
-        <f>J21*0.2+N21*0.3+O21*0.5</f>
-        <v>22.333333333333336</v>
+        <f>J21*0.2+N21*0.25+O21*0.55+14</f>
+        <v>55.75</v>
       </c>
       <c r="Q21" s="18">
         <f>D21*0.4+P21*0.6</f>
-        <v>41.53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60.25</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D22" s="18">
-        <v>67</v>
+        <v>42.533333333333339</v>
       </c>
       <c r="E22" s="29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" s="7">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="G22" s="7">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="H22" s="7">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="I22" s="36"/>
       <c r="J22" s="13">
         <f>SUM(E22:H22)*50/(J$1-I22)</f>
-        <v>61.250000000000007</v>
+        <v>97.5</v>
       </c>
       <c r="K22" s="12">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L22" s="6">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="M22" s="36"/>
       <c r="N22" s="13">
         <f>SUM(K22:L22)/(N$1-M22)</f>
-        <v>30</v>
-      </c>
-      <c r="O22" s="6"/>
+        <v>97.5</v>
+      </c>
+      <c r="O22" s="6">
+        <v>25</v>
+      </c>
       <c r="P22" s="18">
-        <f>J22*0.2+N22*0.3+O22*0.5</f>
-        <v>21.25</v>
+        <f>J22*0.2+N22*0.25+O22*0.55+14</f>
+        <v>71.625</v>
       </c>
       <c r="Q22" s="18">
         <f>D22*0.4+P22*0.6</f>
-        <v>39.549999999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59.988333333333337</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D23" s="18">
         <v>54.933333333333337</v>
@@ -5790,17 +5934,22 @@
         <f>SUM(K23:L23)/(N$1-M23)</f>
         <v>37.5</v>
       </c>
-      <c r="O23" s="6"/>
+      <c r="O23" s="6">
+        <v>21</v>
+      </c>
       <c r="P23" s="18">
-        <f>J23*0.2+N23*0.3+O23*0.5</f>
-        <v>22.5</v>
+        <f>J23*0.2+N23*0.25+O23*0.55+14</f>
+        <v>46.174999999999997</v>
       </c>
       <c r="Q23" s="18">
         <f>D23*0.4+P23*0.6</f>
-        <v>35.473333333333336</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>49.678333333333335</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>26</v>
       </c>
@@ -5823,7 +5972,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I24" s="36">
         <v>1</v>
@@ -5843,31 +5992,36 @@
         <f>SUM(K24:L24)/(N$1-M24)</f>
         <v>25</v>
       </c>
-      <c r="O24" s="6"/>
+      <c r="O24" s="6">
+        <v>1</v>
+      </c>
       <c r="P24" s="18">
-        <f>J24*0.2+N24*0.3+O24*0.5</f>
-        <v>14.166666666666668</v>
+        <f>J24*0.2+N24*0.25+O24*0.55+14</f>
+        <v>27.466666666666669</v>
       </c>
       <c r="Q24" s="18">
         <f>D24*0.4+P24*0.6</f>
-        <v>34.78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42.760000000000005</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="D25" s="18">
-        <v>42.150000000000006</v>
+        <v>39.333333333333336</v>
       </c>
       <c r="E25" s="29">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="F25" s="7">
         <v>0</v>
@@ -5876,15 +6030,15 @@
         <v>0</v>
       </c>
       <c r="H25" s="7">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="I25" s="36"/>
       <c r="J25" s="13">
         <f>SUM(E25:H25)*50/(J$1-I25)</f>
-        <v>33.75</v>
+        <v>0</v>
       </c>
       <c r="K25" s="12">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L25" s="6">
         <v>0</v>
@@ -5892,33 +6046,38 @@
       <c r="M25" s="36"/>
       <c r="N25" s="13">
         <f>SUM(K25:L25)/(N$1-M25)</f>
-        <v>25</v>
-      </c>
-      <c r="O25" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="6">
+        <v>31</v>
+      </c>
       <c r="P25" s="18">
-        <f>J25*0.2+N25*0.3+O25*0.5</f>
-        <v>14.25</v>
+        <f>J25*0.2+N25*0.25+O25*0.55+14</f>
+        <v>31.05</v>
       </c>
       <c r="Q25" s="18">
         <f>D25*0.4+P25*0.6</f>
-        <v>25.410000000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34.36333333333333</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="D26" s="18">
-        <v>39.333333333333336</v>
+        <v>42.150000000000006</v>
       </c>
       <c r="E26" s="29">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F26" s="7">
         <v>0</v>
@@ -5927,15 +6086,15 @@
         <v>0</v>
       </c>
       <c r="H26" s="7">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="I26" s="36"/>
       <c r="J26" s="13">
         <f>SUM(E26:H26)*50/(J$1-I26)</f>
-        <v>0</v>
+        <v>33.75</v>
       </c>
       <c r="K26" s="12">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L26" s="6">
         <v>0</v>
@@ -5943,24 +6102,29 @@
       <c r="M26" s="36"/>
       <c r="N26" s="13">
         <f>SUM(K26:L26)/(N$1-M26)</f>
-        <v>0</v>
-      </c>
-      <c r="O26" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="O26" s="6">
+        <v>0</v>
+      </c>
       <c r="P26" s="18">
-        <f>J26*0.2+N26*0.3+O26*0.5</f>
-        <v>0</v>
+        <f>J26*0.2+N26*0.25+O26*0.55+14</f>
+        <v>27</v>
       </c>
       <c r="Q26" s="18">
         <f>D26*0.4+P26*0.6</f>
-        <v>15.733333333333334</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33.06</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>3</v>
@@ -5996,25 +6160,29 @@
         <f>SUM(K27:L27)/(N$1-M27)</f>
         <v>0</v>
       </c>
-      <c r="O27" s="6"/>
+      <c r="O27" s="6">
+        <v>0</v>
+      </c>
       <c r="P27" s="18">
-        <f>J27*0.2+N27*0.3+O27*0.5</f>
         <v>0</v>
       </c>
       <c r="Q27" s="18">
         <f>D27*0.4+P27*0.6</f>
         <v>9.6800000000000015</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R27" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D28" s="18">
         <v>14.4</v>
@@ -6047,25 +6215,29 @@
         <f>SUM(K28:L28)/(N$1-M28)</f>
         <v>0</v>
       </c>
-      <c r="O28" s="6"/>
+      <c r="O28" s="6">
+        <v>0</v>
+      </c>
       <c r="P28" s="18">
-        <f>J28*0.2+N28*0.3+O28*0.5</f>
         <v>0</v>
       </c>
       <c r="Q28" s="18">
         <f>D28*0.4+P28*0.6</f>
         <v>5.7600000000000007</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R28" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D29" s="18">
         <v>14</v>
@@ -6098,25 +6270,29 @@
         <f>SUM(K29:L29)/(N$1-M29)</f>
         <v>0</v>
       </c>
-      <c r="O29" s="6"/>
+      <c r="O29" s="6">
+        <v>0</v>
+      </c>
       <c r="P29" s="18">
-        <f>J29*0.2+N29*0.3+O29*0.5</f>
         <v>0</v>
       </c>
       <c r="Q29" s="18">
         <f>D29*0.4+P29*0.6</f>
         <v>5.6000000000000005</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R29" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D30" s="18">
         <v>12.8</v>
@@ -6149,19 +6325,23 @@
         <f>SUM(K30:L30)/(N$1-M30)</f>
         <v>0</v>
       </c>
-      <c r="O30" s="6"/>
+      <c r="O30" s="6">
+        <v>0</v>
+      </c>
       <c r="P30" s="18">
-        <f>J30*0.2+N30*0.3+O30*0.5</f>
         <v>0</v>
       </c>
       <c r="Q30" s="18">
         <f>D30*0.4+P30*0.6</f>
         <v>5.120000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R30" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>21</v>
@@ -6200,25 +6380,29 @@
         <f>SUM(K31:L31)/(N$1-M31)</f>
         <v>0</v>
       </c>
-      <c r="O31" s="6"/>
+      <c r="O31" s="6">
+        <v>0</v>
+      </c>
       <c r="P31" s="18">
-        <f>J31*0.2+N31*0.3+O31*0.5</f>
         <v>0</v>
       </c>
       <c r="Q31" s="18">
         <f>D31*0.4+P31*0.6</f>
         <v>4.9600000000000009</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R31" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="B32" s="49" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="29">
@@ -6249,25 +6433,29 @@
         <f>SUM(K32:L32)/(N$1-M32)</f>
         <v>0</v>
       </c>
-      <c r="O32" s="6"/>
+      <c r="O32" s="6">
+        <v>0</v>
+      </c>
       <c r="P32" s="18">
-        <f>J32*0.2+N32*0.3+O32*0.5</f>
         <v>0</v>
       </c>
       <c r="Q32" s="18">
         <f>D32*0.4+P32*0.6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R32" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="B33" s="49" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="29">
@@ -6298,25 +6486,29 @@
         <f>SUM(K33:L33)/(N$1-M33)</f>
         <v>0</v>
       </c>
-      <c r="O33" s="6"/>
+      <c r="O33" s="6">
+        <v>0</v>
+      </c>
       <c r="P33" s="18">
-        <f>J33*0.2+N33*0.3+O33*0.5</f>
         <v>0</v>
       </c>
       <c r="Q33" s="18">
         <f>D33*0.4+P33*0.6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R33" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="B34" s="49" t="s">
-        <v>5</v>
+        <v>114</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="29">
@@ -6347,25 +6539,29 @@
         <f>SUM(K34:L34)/(N$1-M34)</f>
         <v>0</v>
       </c>
-      <c r="O34" s="6"/>
+      <c r="O34" s="6">
+        <v>0</v>
+      </c>
       <c r="P34" s="18">
-        <f>J34*0.2+N34*0.3+O34*0.5</f>
         <v>0</v>
       </c>
       <c r="Q34" s="18">
         <f>D34*0.4+P34*0.6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R34" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B35" s="49" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C35" s="50" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="29">
@@ -6396,25 +6592,29 @@
         <f>SUM(K35:L35)/(N$1-M35)</f>
         <v>0</v>
       </c>
-      <c r="O35" s="6"/>
+      <c r="O35" s="6">
+        <v>0</v>
+      </c>
       <c r="P35" s="18">
-        <f>J35*0.2+N35*0.3+O35*0.5</f>
         <v>0</v>
       </c>
       <c r="Q35" s="18">
         <f>D35*0.4+P35*0.6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R35" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B36" s="49" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="C36" s="50" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="29">
@@ -6445,25 +6645,29 @@
         <f>SUM(K36:L36)/(N$1-M36)</f>
         <v>0</v>
       </c>
-      <c r="O36" s="6"/>
+      <c r="O36" s="6">
+        <v>0</v>
+      </c>
       <c r="P36" s="18">
-        <f>J36*0.2+N36*0.3+O36*0.5</f>
         <v>0</v>
       </c>
       <c r="Q36" s="18">
         <f>D36*0.4+P36*0.6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R36" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="B37" s="49" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="C37" s="50" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="29">
@@ -6494,27 +6698,31 @@
         <f>SUM(K37:L37)/(N$1-M37)</f>
         <v>0</v>
       </c>
-      <c r="O37" s="6"/>
+      <c r="O37" s="6">
+        <v>0</v>
+      </c>
       <c r="P37" s="18">
-        <f>J37*0.2+N37*0.3+O37*0.5</f>
         <v>0</v>
       </c>
       <c r="Q37" s="18">
         <f>D37*0.4+P37*0.6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R37" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="B38" s="49" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="18"/>
+        <v>119</v>
+      </c>
+      <c r="D38" s="58"/>
       <c r="E38" s="29">
         <v>0</v>
       </c>
@@ -6543,25 +6751,29 @@
         <f>SUM(K38:L38)/(N$1-M38)</f>
         <v>0</v>
       </c>
-      <c r="O38" s="6"/>
+      <c r="O38" s="6">
+        <v>0</v>
+      </c>
       <c r="P38" s="18">
-        <f>J38*0.2+N38*0.3+O38*0.5</f>
         <v>0</v>
       </c>
       <c r="Q38" s="18">
         <f>D38*0.4+P38*0.6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R38" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B39" s="49" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C39" s="50" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="29">
@@ -6592,17 +6804,21 @@
         <f>SUM(K39:L39)/(N$1-M39)</f>
         <v>0</v>
       </c>
-      <c r="O39" s="6"/>
+      <c r="O39" s="6">
+        <v>0</v>
+      </c>
       <c r="P39" s="18">
-        <f>J39*0.2+N39*0.3+O39*0.5</f>
         <v>0</v>
       </c>
       <c r="Q39" s="18">
         <f>D39*0.4+P39*0.6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R39" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
         <v>22</v>
       </c>
@@ -6641,25 +6857,29 @@
         <f>SUM(K40:L40)/(N$1-M40)</f>
         <v>0</v>
       </c>
-      <c r="O40" s="6"/>
+      <c r="O40" s="6">
+        <v>0</v>
+      </c>
       <c r="P40" s="18">
-        <f>J40*0.2+N40*0.3+O40*0.5</f>
         <v>0</v>
       </c>
       <c r="Q40" s="18">
         <f>D40*0.4+P40*0.6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R40" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="B41" s="49" t="s">
-        <v>117</v>
+        <v>60</v>
       </c>
       <c r="C41" s="50" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="29">
@@ -6690,27 +6910,31 @@
         <f>SUM(K41:L41)/(N$1-M41)</f>
         <v>0</v>
       </c>
-      <c r="O41" s="6"/>
+      <c r="O41" s="6">
+        <v>0</v>
+      </c>
       <c r="P41" s="18">
-        <f>J41*0.2+N41*0.3+O41*0.5</f>
         <v>0</v>
       </c>
       <c r="Q41" s="18">
         <f>D41*0.4+P41*0.6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R41" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="B42" s="49" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="C42" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="D42" s="58"/>
+        <v>72</v>
+      </c>
+      <c r="D42" s="18"/>
       <c r="E42" s="29">
         <v>0</v>
       </c>
@@ -6739,17 +6963,21 @@
         <f>SUM(K42:L42)/(N$1-M42)</f>
         <v>0</v>
       </c>
-      <c r="O42" s="56"/>
+      <c r="O42" s="6">
+        <v>0</v>
+      </c>
       <c r="P42" s="18">
-        <f>J42*0.2+N42*0.3+O42*0.5</f>
         <v>0</v>
       </c>
       <c r="Q42" s="18">
         <f>D42*0.4+P42*0.6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R42" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -6765,7 +6993,7 @@
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
     </row>
-    <row r="44" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -6781,7 +7009,7 @@
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
     </row>
-    <row r="45" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -6797,7 +7025,7 @@
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
     </row>
-    <row r="46" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -6813,7 +7041,7 @@
       <c r="M46" s="9"/>
       <c r="N46" s="9"/>
     </row>
-    <row r="47" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -6829,7 +7057,7 @@
       <c r="M47" s="9"/>
       <c r="N47" s="9"/>
     </row>
-    <row r="48" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -7374,7 +7602,7 @@
       <c r="N81" s="9"/>
     </row>
   </sheetData>
-  <sortState ref="A3:Q42">
+  <sortState ref="A3:R42">
     <sortCondition descending="1" ref="Q3"/>
   </sortState>
   <mergeCells count="2">
@@ -7382,14 +7610,14 @@
     <mergeCell ref="E1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H42">
-    <cfRule type="cellIs" dxfId="10" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="26" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="28" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7436,18 +7664,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L42">
-    <cfRule type="cellIs" dxfId="7" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="20" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
@@ -7495,18 +7723,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O42">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThanOrEqual">
       <formula>80</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ileri java final sonuclar
</commit_message>
<xml_diff>
--- a/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
+++ b/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
@@ -3128,7 +3128,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3155,7 +3155,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="4" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="31"/>
@@ -3286,12 +3286,12 @@
         <v>0</v>
       </c>
       <c r="K3" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L3" s="42"/>
       <c r="M3" s="14">
         <f t="shared" ref="M3:M30" si="0">SUM(E3:K3)*50/(A$1-L3)</f>
-        <v>50</v>
+        <v>57.142857142857146</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="14">
@@ -3301,11 +3301,11 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="18">
         <f t="shared" ref="Q3:Q30" si="2">MIN(100,M3*(0.2+0.25)+O3*(0.25+0.1)+P3*(0.55+0.15))</f>
-        <v>22.5</v>
+        <v>25.714285714285715</v>
       </c>
       <c r="R3" s="18">
         <f t="shared" ref="R3:R30" si="3">ROUND(D3,2)*0.4+Q3*0.6</f>
-        <v>53.5</v>
+        <v>55.428571428571431</v>
       </c>
       <c r="U3" s="18"/>
       <c r="V3" s="18"/>
@@ -3342,12 +3342,12 @@
         <v>0</v>
       </c>
       <c r="K4" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4" s="42"/>
       <c r="M4" s="14">
         <f t="shared" si="0"/>
-        <v>60.833333333333336</v>
+        <v>66.428571428571431</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="14">
@@ -3357,11 +3357,11 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="18">
         <f t="shared" si="2"/>
-        <v>27.375</v>
+        <v>29.892857142857146</v>
       </c>
       <c r="R4" s="18">
         <f t="shared" si="3"/>
-        <v>55.021000000000001</v>
+        <v>56.531714285714287</v>
       </c>
       <c r="U4" s="18"/>
       <c r="V4" s="18"/>
@@ -3398,12 +3398,12 @@
         <v>0</v>
       </c>
       <c r="K5" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L5" s="42"/>
       <c r="M5" s="14">
         <f t="shared" si="0"/>
-        <v>16.666666666666668</v>
+        <v>28.571428571428573</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="14">
@@ -3413,11 +3413,11 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="18">
         <f t="shared" si="2"/>
-        <v>7.5000000000000009</v>
+        <v>12.857142857142858</v>
       </c>
       <c r="R5" s="18">
         <f t="shared" si="3"/>
-        <v>38.580000000000005</v>
+        <v>41.794285714285721</v>
       </c>
       <c r="U5" s="18"/>
       <c r="V5" s="18"/>
@@ -3459,7 +3459,7 @@
       <c r="L6" s="42"/>
       <c r="M6" s="14">
         <f t="shared" si="0"/>
-        <v>33.333333333333336</v>
+        <v>28.571428571428573</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="14">
@@ -3469,11 +3469,11 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="18">
         <f t="shared" si="2"/>
-        <v>15.000000000000002</v>
+        <v>12.857142857142858</v>
       </c>
       <c r="R6" s="18">
         <f t="shared" si="3"/>
-        <v>42.760000000000005</v>
+        <v>41.47428571428572</v>
       </c>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
@@ -3571,7 +3571,7 @@
       <c r="L8" s="42"/>
       <c r="M8" s="14">
         <f t="shared" si="0"/>
-        <v>8.3333333333333339</v>
+        <v>7.1428571428571432</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="14">
@@ -3581,11 +3581,11 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="18">
         <f t="shared" si="2"/>
-        <v>3.7500000000000004</v>
+        <v>3.2142857142857144</v>
       </c>
       <c r="R8" s="18">
         <f t="shared" si="3"/>
-        <v>33.33</v>
+        <v>33.008571428571429</v>
       </c>
       <c r="U8" s="18"/>
       <c r="V8" s="18"/>
@@ -3622,12 +3622,12 @@
         <v>0</v>
       </c>
       <c r="K9" s="7">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="L9" s="42"/>
       <c r="M9" s="14">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>33.571428571428569</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="14">
@@ -3637,11 +3637,11 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="18">
         <f t="shared" si="2"/>
-        <v>11.25</v>
+        <v>15.107142857142856</v>
       </c>
       <c r="R9" s="18">
         <f t="shared" si="3"/>
-        <v>33.67</v>
+        <v>35.984285714285718</v>
       </c>
       <c r="U9" s="18"/>
       <c r="V9" s="18"/>
@@ -3683,7 +3683,7 @@
       <c r="L10" s="42"/>
       <c r="M10" s="14">
         <f t="shared" si="0"/>
-        <v>41.666666666666664</v>
+        <v>35.714285714285715</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="14">
@@ -3693,11 +3693,11 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="18">
         <f t="shared" si="2"/>
-        <v>18.75</v>
+        <v>16.071428571428573</v>
       </c>
       <c r="R10" s="18">
         <f t="shared" si="3"/>
-        <v>37.85</v>
+        <v>36.242857142857147</v>
       </c>
       <c r="U10" s="18"/>
       <c r="V10" s="18"/>
@@ -3795,7 +3795,7 @@
       <c r="L12" s="42"/>
       <c r="M12" s="14">
         <f t="shared" si="0"/>
-        <v>8.3333333333333339</v>
+        <v>7.1428571428571432</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="14">
@@ -3805,11 +3805,11 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="18">
         <f t="shared" si="2"/>
-        <v>3.7500000000000004</v>
+        <v>3.2142857142857144</v>
       </c>
       <c r="R12" s="18">
         <f t="shared" si="3"/>
-        <v>23.69</v>
+        <v>23.368571428571428</v>
       </c>
       <c r="U12" s="18"/>
       <c r="V12" s="18"/>
@@ -4070,12 +4070,12 @@
         <v>2</v>
       </c>
       <c r="K17" s="7">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="L17" s="42"/>
       <c r="M17" s="14">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>56.428571428571431</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="14">
@@ -4085,11 +4085,11 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="18">
         <f t="shared" si="2"/>
-        <v>22.5</v>
+        <v>25.392857142857146</v>
       </c>
       <c r="R17" s="18">
         <f t="shared" si="3"/>
-        <v>26.923999999999999</v>
+        <v>28.659714285714287</v>
       </c>
       <c r="U17" s="18"/>
       <c r="V17" s="18"/>
@@ -4187,7 +4187,7 @@
       <c r="L19" s="42"/>
       <c r="M19" s="14">
         <f t="shared" si="0"/>
-        <v>16.666666666666668</v>
+        <v>14.285714285714286</v>
       </c>
       <c r="N19" s="6"/>
       <c r="O19" s="14">
@@ -4197,11 +4197,11 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="18">
         <f t="shared" si="2"/>
-        <v>7.5000000000000009</v>
+        <v>6.4285714285714288</v>
       </c>
       <c r="R19" s="18">
         <f t="shared" si="3"/>
-        <v>5.2519999999999998</v>
+        <v>4.6091428571428574</v>
       </c>
       <c r="U19" s="18"/>
       <c r="V19" s="18"/>

</xml_diff>

<commit_message>
Yaz. arac. donem sonu notlari
</commit_message>
<xml_diff>
--- a/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
+++ b/SoftwareDevEnvAndTools/_docs/Notlar.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
   <si>
     <t>Adı</t>
   </si>
@@ -113,18 +113,6 @@
   </si>
   <si>
     <t>M</t>
-  </si>
-  <si>
-    <t>DEVAM DURUMU 
-(%20+%25 bonus)</t>
-  </si>
-  <si>
-    <t>ODEV 
-(%25+%10 bonus)</t>
-  </si>
-  <si>
-    <t>PROJE
-(%55+%15 bonus)</t>
   </si>
   <si>
     <t>BÜT PROJESİ</t>
@@ -237,6 +225,21 @@
   <si>
     <t>FURKAN BERAT</t>
   </si>
+  <si>
+    <t>ODEV 
+(yok)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>DEVAM DURUMU 
+(%40)</t>
+  </si>
+  <si>
+    <t>FINAL SINAVI
+(%60 + 13puan)</t>
+  </si>
 </sst>
 </file>
 
@@ -330,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -469,49 +472,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -620,19 +580,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -693,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -713,19 +660,16 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -740,31 +684,27 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -805,16 +745,15 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -834,13 +773,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -852,10 +791,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1370,7 +1309,7 @@
     <col min="3" max="3" width="9.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="3.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.44140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.44140625" style="40" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.77734375" style="1" customWidth="1"/>
@@ -1381,80 +1320,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="40">
+      <c r="A1" s="24"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="33">
         <v>4</v>
       </c>
-      <c r="K1" s="74" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" s="75"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="16" t="s">
+      <c r="K1" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="67"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>21</v>
+      <c r="A2" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="20">
         <v>1</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="21">
         <v>2</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="21">
         <v>3</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="21">
         <v>4</v>
       </c>
-      <c r="H2" s="44">
+      <c r="H2" s="37">
         <v>5</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="12">
         <v>2</v>
@@ -1468,38 +1407,38 @@
       <c r="G3" s="7">
         <v>2</v>
       </c>
-      <c r="H3" s="45">
+      <c r="H3" s="38">
         <v>2</v>
       </c>
-      <c r="I3" s="42">
-        <v>0</v>
-      </c>
-      <c r="J3" s="14">
+      <c r="I3" s="35">
+        <v>0</v>
+      </c>
+      <c r="J3" s="13">
         <f t="shared" ref="J3:J27" si="0">SUM(D3:H3)*50/(J$1-I3)</f>
         <v>125</v>
       </c>
       <c r="K3" s="6">
         <v>86</v>
       </c>
-      <c r="L3" s="42">
+      <c r="L3" s="35">
         <v>14</v>
       </c>
-      <c r="M3" s="39">
+      <c r="M3" s="32">
         <f t="shared" ref="M3:M19" si="1">K3+L3</f>
         <v>100</v>
       </c>
-      <c r="N3" s="18">
+      <c r="N3" s="17">
         <f t="shared" ref="N3:N19" si="2">MIN(100,J3*0.3+M3*0.7+M3*0.1)</f>
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4" s="12">
         <v>0</v>
@@ -1513,33 +1452,33 @@
       <c r="G4" s="7">
         <v>1.5</v>
       </c>
-      <c r="H4" s="45">
-        <v>0</v>
-      </c>
-      <c r="I4" s="42">
-        <v>0</v>
-      </c>
-      <c r="J4" s="14">
+      <c r="H4" s="38">
+        <v>0</v>
+      </c>
+      <c r="I4" s="35">
+        <v>0</v>
+      </c>
+      <c r="J4" s="13">
         <f t="shared" si="0"/>
         <v>65.625</v>
       </c>
       <c r="K4" s="6">
         <v>82</v>
       </c>
-      <c r="L4" s="42">
+      <c r="L4" s="35">
         <v>14</v>
       </c>
-      <c r="M4" s="39">
+      <c r="M4" s="32">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N4" s="17">
         <f t="shared" si="2"/>
         <v>96.487499999999983</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1560,27 +1499,27 @@
       <c r="G5" s="7">
         <v>0</v>
       </c>
-      <c r="H5" s="45">
+      <c r="H5" s="38">
         <v>2</v>
       </c>
-      <c r="I5" s="42">
-        <v>0</v>
-      </c>
-      <c r="J5" s="14">
+      <c r="I5" s="35">
+        <v>0</v>
+      </c>
+      <c r="J5" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="K5" s="6">
         <v>55</v>
       </c>
-      <c r="L5" s="42">
+      <c r="L5" s="35">
         <v>14</v>
       </c>
-      <c r="M5" s="39">
+      <c r="M5" s="32">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="17">
         <f t="shared" si="2"/>
         <v>85.2</v>
       </c>
@@ -1589,12 +1528,12 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" s="12">
         <v>0</v>
@@ -1608,38 +1547,38 @@
       <c r="G6" s="7">
         <v>2</v>
       </c>
-      <c r="H6" s="45">
+      <c r="H6" s="38">
         <v>2</v>
       </c>
-      <c r="I6" s="42">
-        <v>0</v>
-      </c>
-      <c r="J6" s="14">
+      <c r="I6" s="35">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="K6" s="6">
         <v>54</v>
       </c>
-      <c r="L6" s="42">
+      <c r="L6" s="35">
         <v>14</v>
       </c>
-      <c r="M6" s="39">
+      <c r="M6" s="32">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="17">
         <f t="shared" si="2"/>
         <v>84.399999999999991</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" s="12">
         <v>0</v>
@@ -1653,38 +1592,38 @@
       <c r="G7" s="7">
         <v>2</v>
       </c>
-      <c r="H7" s="45">
+      <c r="H7" s="38">
         <v>2</v>
       </c>
-      <c r="I7" s="43">
-        <v>0</v>
-      </c>
-      <c r="J7" s="14">
+      <c r="I7" s="36">
+        <v>0</v>
+      </c>
+      <c r="J7" s="13">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="K7" s="6">
         <v>59</v>
       </c>
-      <c r="L7" s="42">
+      <c r="L7" s="35">
         <v>14</v>
       </c>
-      <c r="M7" s="39">
+      <c r="M7" s="32">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="17">
         <f t="shared" si="2"/>
         <v>80.899999999999991</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D8" s="12">
         <v>0</v>
@@ -1698,38 +1637,38 @@
       <c r="G8" s="7">
         <v>2</v>
       </c>
-      <c r="H8" s="45">
+      <c r="H8" s="38">
         <v>2</v>
       </c>
-      <c r="I8" s="42">
-        <v>0</v>
-      </c>
-      <c r="J8" s="14">
+      <c r="I8" s="35">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="K8" s="6">
         <v>55</v>
       </c>
-      <c r="L8" s="42">
+      <c r="L8" s="35">
         <v>14</v>
       </c>
-      <c r="M8" s="39">
+      <c r="M8" s="32">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="17">
         <f t="shared" si="2"/>
         <v>77.7</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D9" s="12">
         <v>2</v>
@@ -1743,38 +1682,38 @@
       <c r="G9" s="7">
         <v>0</v>
       </c>
-      <c r="H9" s="45">
-        <v>0</v>
-      </c>
-      <c r="I9" s="42">
-        <v>0</v>
-      </c>
-      <c r="J9" s="14">
+      <c r="H9" s="38">
+        <v>0</v>
+      </c>
+      <c r="I9" s="35">
+        <v>0</v>
+      </c>
+      <c r="J9" s="13">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="K9" s="6">
         <v>42</v>
       </c>
-      <c r="L9" s="42">
+      <c r="L9" s="35">
         <v>14</v>
       </c>
-      <c r="M9" s="39">
+      <c r="M9" s="32">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="17">
         <f t="shared" si="2"/>
         <v>67.3</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="12">
         <v>0</v>
@@ -1788,38 +1727,38 @@
       <c r="G10" s="7">
         <v>0</v>
       </c>
-      <c r="H10" s="45">
+      <c r="H10" s="38">
         <v>2</v>
       </c>
-      <c r="I10" s="42">
-        <v>0</v>
-      </c>
-      <c r="J10" s="14">
+      <c r="I10" s="35">
+        <v>0</v>
+      </c>
+      <c r="J10" s="13">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="K10" s="6">
         <v>41</v>
       </c>
-      <c r="L10" s="42">
+      <c r="L10" s="35">
         <v>14</v>
       </c>
-      <c r="M10" s="39">
+      <c r="M10" s="32">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="17">
         <f t="shared" si="2"/>
         <v>66.5</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" s="12">
         <v>0</v>
@@ -1833,38 +1772,38 @@
       <c r="G11" s="7">
         <v>0</v>
       </c>
-      <c r="H11" s="45">
+      <c r="H11" s="38">
         <v>2</v>
       </c>
-      <c r="I11" s="42">
-        <v>0</v>
-      </c>
-      <c r="J11" s="14">
+      <c r="I11" s="35">
+        <v>0</v>
+      </c>
+      <c r="J11" s="13">
         <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
       <c r="K11" s="6">
         <v>48</v>
       </c>
-      <c r="L11" s="42">
+      <c r="L11" s="35">
         <v>14</v>
       </c>
-      <c r="M11" s="39">
+      <c r="M11" s="32">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="17">
         <f t="shared" si="2"/>
         <v>60.85</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D12" s="12">
         <v>0</v>
@@ -1881,35 +1820,35 @@
       <c r="H12" s="7">
         <v>0</v>
       </c>
-      <c r="I12" s="42">
-        <v>0</v>
-      </c>
-      <c r="J12" s="14">
+      <c r="I12" s="35">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K12" s="6">
         <v>53</v>
       </c>
-      <c r="L12" s="42">
+      <c r="L12" s="35">
         <v>14</v>
       </c>
-      <c r="M12" s="39">
+      <c r="M12" s="32">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="17">
         <f t="shared" si="2"/>
         <v>53.6</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D13" s="12">
         <v>0</v>
@@ -1926,35 +1865,35 @@
       <c r="H13" s="7">
         <v>0</v>
       </c>
-      <c r="I13" s="42">
-        <v>0</v>
-      </c>
-      <c r="J13" s="14">
+      <c r="I13" s="35">
+        <v>0</v>
+      </c>
+      <c r="J13" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K13" s="6">
         <v>33</v>
       </c>
-      <c r="L13" s="42">
+      <c r="L13" s="35">
         <v>14</v>
       </c>
-      <c r="M13" s="39">
+      <c r="M13" s="32">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="17">
         <f t="shared" si="2"/>
         <v>37.6</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D14" s="12">
         <v>0</v>
@@ -1971,35 +1910,35 @@
       <c r="H14" s="7">
         <v>0</v>
       </c>
-      <c r="I14" s="42">
-        <v>0</v>
-      </c>
-      <c r="J14" s="14">
+      <c r="I14" s="35">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K14" s="6">
         <v>29</v>
       </c>
-      <c r="L14" s="42">
+      <c r="L14" s="35">
         <v>14</v>
       </c>
-      <c r="M14" s="39">
+      <c r="M14" s="32">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="17">
         <f t="shared" si="2"/>
         <v>34.4</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="12">
         <v>0</v>
@@ -2016,35 +1955,35 @@
       <c r="H15" s="12">
         <v>0</v>
       </c>
-      <c r="I15" s="42">
-        <v>0</v>
-      </c>
-      <c r="J15" s="14">
+      <c r="I15" s="35">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K15" s="6">
         <v>24</v>
       </c>
-      <c r="L15" s="42">
+      <c r="L15" s="35">
         <v>14</v>
       </c>
-      <c r="M15" s="39">
+      <c r="M15" s="32">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="17">
         <f t="shared" si="2"/>
         <v>30.4</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="41" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
+    <row r="16" spans="1:15" s="34" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="42"/>
       <c r="B16" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D16" s="12">
         <v>0</v>
@@ -2061,36 +2000,36 @@
       <c r="H16" s="12">
         <v>0</v>
       </c>
-      <c r="I16" s="42">
-        <v>0</v>
-      </c>
-      <c r="J16" s="14">
+      <c r="I16" s="35">
+        <v>0</v>
+      </c>
+      <c r="J16" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K16" s="6">
         <v>13</v>
       </c>
-      <c r="L16" s="42">
+      <c r="L16" s="35">
         <v>14</v>
       </c>
-      <c r="M16" s="39">
+      <c r="M16" s="32">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="N16" s="18">
+      <c r="N16" s="17">
         <f t="shared" si="2"/>
         <v>21.599999999999998</v>
       </c>
-      <c r="O16" s="58"/>
+      <c r="O16" s="51"/>
     </row>
     <row r="17" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D17" s="12">
         <v>0</v>
@@ -2104,43 +2043,43 @@
       <c r="G17" s="12">
         <v>2</v>
       </c>
-      <c r="H17" s="48">
-        <v>0</v>
-      </c>
-      <c r="I17" s="42">
-        <v>0</v>
-      </c>
-      <c r="J17" s="14">
+      <c r="H17" s="41">
+        <v>0</v>
+      </c>
+      <c r="I17" s="35">
+        <v>0</v>
+      </c>
+      <c r="J17" s="13">
         <f t="shared" si="0"/>
         <v>71.875</v>
       </c>
       <c r="K17" s="6">
         <v>1</v>
       </c>
-      <c r="L17" s="42">
+      <c r="L17" s="35">
         <v>14</v>
       </c>
-      <c r="M17" s="39">
+      <c r="M17" s="32">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="N17" s="18">
+      <c r="N17" s="17">
         <f t="shared" si="2"/>
         <v>33.5625</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D18" s="12">
         <v>0</v>
       </c>
-      <c r="E18" s="48">
+      <c r="E18" s="41">
         <v>0</v>
       </c>
       <c r="F18" s="12">
@@ -2149,34 +2088,34 @@
       <c r="G18" s="12">
         <v>2</v>
       </c>
-      <c r="H18" s="48">
-        <v>0</v>
-      </c>
-      <c r="I18" s="42">
-        <v>0</v>
-      </c>
-      <c r="J18" s="14">
+      <c r="H18" s="41">
+        <v>0</v>
+      </c>
+      <c r="I18" s="35">
+        <v>0</v>
+      </c>
+      <c r="J18" s="13">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="K18" s="6"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="39">
+      <c r="L18" s="35"/>
+      <c r="M18" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N18" s="18">
+      <c r="N18" s="17">
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="58" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+    <row r="19" spans="1:15" s="51" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D19" s="12">
         <v>0</v>
@@ -2190,220 +2129,220 @@
       <c r="G19" s="12">
         <v>0</v>
       </c>
-      <c r="H19" s="48">
-        <v>0</v>
-      </c>
-      <c r="I19" s="42">
-        <v>0</v>
-      </c>
-      <c r="J19" s="14">
+      <c r="H19" s="41">
+        <v>0</v>
+      </c>
+      <c r="I19" s="35">
+        <v>0</v>
+      </c>
+      <c r="J19" s="13">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
       <c r="K19" s="6"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="39">
+      <c r="L19" s="35"/>
+      <c r="M19" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N19" s="18">
+      <c r="N19" s="17">
         <f t="shared" si="2"/>
         <v>1.875</v>
       </c>
       <c r="O19" s="9"/>
     </row>
-    <row r="20" spans="1:15" s="58" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="54">
-        <v>0</v>
-      </c>
-      <c r="J20" s="55">
+    <row r="20" spans="1:15" s="51" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="42"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="47">
+        <v>0</v>
+      </c>
+      <c r="J20" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="71"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="18">
+      <c r="K20" s="63"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="17">
         <f t="shared" ref="N20:N27" si="3">J20*0.3+L20*0.7+M20*0.1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="58" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="54">
-        <v>0</v>
-      </c>
-      <c r="J21" s="55">
+    <row r="21" spans="1:15" s="51" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="47">
+        <v>0</v>
+      </c>
+      <c r="J21" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21" s="71"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="18">
+      <c r="K21" s="63"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="58" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="54">
-        <v>0</v>
-      </c>
-      <c r="J22" s="55">
+    <row r="22" spans="1:15" s="51" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="47">
+        <v>0</v>
+      </c>
+      <c r="J22" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="71"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="18">
+      <c r="K22" s="63"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="58" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="54">
-        <v>0</v>
-      </c>
-      <c r="J23" s="55">
+    <row r="23" spans="1:15" s="51" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="47">
+        <v>0</v>
+      </c>
+      <c r="J23" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="71"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="18">
+      <c r="K23" s="63"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="58" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="54">
-        <v>0</v>
-      </c>
-      <c r="J24" s="55">
+    <row r="24" spans="1:15" s="51" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="47">
+        <v>0</v>
+      </c>
+      <c r="J24" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K24" s="71"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="18">
+      <c r="K24" s="63"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="58" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="54">
-        <v>0</v>
-      </c>
-      <c r="J25" s="55">
+    <row r="25" spans="1:15" s="51" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="42"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="47">
+        <v>0</v>
+      </c>
+      <c r="J25" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K25" s="71"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="18">
+      <c r="K25" s="63"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="58" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="54">
-        <v>0</v>
-      </c>
-      <c r="J26" s="55">
+    <row r="26" spans="1:15" s="51" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="47">
+        <v>0</v>
+      </c>
+      <c r="J26" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K26" s="71"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="18">
+      <c r="K26" s="63"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="54">
-        <v>0</v>
-      </c>
-      <c r="J27" s="55">
+    <row r="27" spans="1:15" s="52" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="47">
+        <v>0</v>
+      </c>
+      <c r="J27" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K27" s="71"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="57"/>
-      <c r="N27" s="18">
+      <c r="K27" s="63"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O27" s="58"/>
+      <c r="O27" s="51"/>
     </row>
     <row r="28" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
@@ -2413,7 +2352,7 @@
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="46"/>
+      <c r="H28" s="39"/>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -2426,7 +2365,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="46"/>
+      <c r="H29" s="39"/>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -2439,7 +2378,7 @@
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
-      <c r="H30" s="46"/>
+      <c r="H30" s="39"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -2452,7 +2391,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="46"/>
+      <c r="H31" s="39"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -2465,7 +2404,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="46"/>
+      <c r="H32" s="39"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -2478,7 +2417,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="46"/>
+      <c r="H33" s="39"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -2491,7 +2430,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="46"/>
+      <c r="H34" s="39"/>
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -2504,7 +2443,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="46"/>
+      <c r="H35" s="39"/>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -2517,7 +2456,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="46"/>
+      <c r="H36" s="39"/>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -2530,7 +2469,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="46"/>
+      <c r="H37" s="39"/>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -2543,7 +2482,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="46"/>
+      <c r="H38" s="39"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
@@ -2556,7 +2495,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="46"/>
+      <c r="H39" s="39"/>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
@@ -2569,7 +2508,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="46"/>
+      <c r="H40" s="39"/>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
@@ -2582,7 +2521,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="46"/>
+      <c r="H41" s="39"/>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
@@ -2595,7 +2534,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
-      <c r="H42" s="46"/>
+      <c r="H42" s="39"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
@@ -2608,7 +2547,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="46"/>
+      <c r="H43" s="39"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
@@ -2621,7 +2560,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="46"/>
+      <c r="H44" s="39"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
@@ -2634,7 +2573,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="46"/>
+      <c r="H45" s="39"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
@@ -2647,7 +2586,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="46"/>
+      <c r="H46" s="39"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
@@ -2660,7 +2599,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="46"/>
+      <c r="H47" s="39"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
@@ -2673,7 +2612,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-      <c r="H48" s="46"/>
+      <c r="H48" s="39"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -2686,7 +2625,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="46"/>
+      <c r="H49" s="39"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
@@ -2699,7 +2638,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="46"/>
+      <c r="H50" s="39"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
@@ -2712,7 +2651,7 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
-      <c r="H51" s="46"/>
+      <c r="H51" s="39"/>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
@@ -2725,7 +2664,7 @@
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
-      <c r="H52" s="46"/>
+      <c r="H52" s="39"/>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
@@ -2738,7 +2677,7 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
-      <c r="H53" s="46"/>
+      <c r="H53" s="39"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
@@ -2751,7 +2690,7 @@
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
-      <c r="H54" s="46"/>
+      <c r="H54" s="39"/>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -2764,7 +2703,7 @@
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
-      <c r="H55" s="46"/>
+      <c r="H55" s="39"/>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
@@ -2777,7 +2716,7 @@
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
-      <c r="H56" s="46"/>
+      <c r="H56" s="39"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
@@ -2790,7 +2729,7 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
-      <c r="H57" s="46"/>
+      <c r="H57" s="39"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -2803,7 +2742,7 @@
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
-      <c r="H58" s="46"/>
+      <c r="H58" s="39"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -2816,7 +2755,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="46"/>
+      <c r="H59" s="39"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -2829,7 +2768,7 @@
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
-      <c r="H60" s="46"/>
+      <c r="H60" s="39"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -2842,7 +2781,7 @@
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
-      <c r="H61" s="46"/>
+      <c r="H61" s="39"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -2855,7 +2794,7 @@
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
-      <c r="H62" s="46"/>
+      <c r="H62" s="39"/>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -2868,7 +2807,7 @@
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
-      <c r="H63" s="46"/>
+      <c r="H63" s="39"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -2881,7 +2820,7 @@
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
-      <c r="H64" s="46"/>
+      <c r="H64" s="39"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -2894,7 +2833,7 @@
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
-      <c r="H65" s="46"/>
+      <c r="H65" s="39"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -2907,7 +2846,7 @@
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
-      <c r="H66" s="46"/>
+      <c r="H66" s="39"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -2920,7 +2859,7 @@
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
-      <c r="H67" s="46"/>
+      <c r="H67" s="39"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -2933,7 +2872,7 @@
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
-      <c r="H68" s="46"/>
+      <c r="H68" s="39"/>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -2946,7 +2885,7 @@
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
-      <c r="H69" s="46"/>
+      <c r="H69" s="39"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -2959,7 +2898,7 @@
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
-      <c r="H70" s="46"/>
+      <c r="H70" s="39"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -2972,7 +2911,7 @@
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
-      <c r="H71" s="46"/>
+      <c r="H71" s="39"/>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -2985,7 +2924,7 @@
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
-      <c r="H72" s="46"/>
+      <c r="H72" s="39"/>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -2998,7 +2937,7 @@
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
-      <c r="H73" s="46"/>
+      <c r="H73" s="39"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -3124,11 +3063,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W81"/>
+  <dimension ref="A1:W78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomLeft" activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3136,7 +3075,7 @@
     <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="64" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="57" customWidth="1"/>
     <col min="5" max="6" width="3.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="2.44140625" style="2" customWidth="1"/>
@@ -3147,127 +3086,127 @@
     <col min="15" max="15" width="4.77734375" style="1" customWidth="1"/>
     <col min="16" max="16" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="5.77734375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.21875" style="69" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.21875" style="61" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.88671875" style="1"/>
     <col min="21" max="23" width="5.77734375" style="1" customWidth="1"/>
     <col min="24" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27">
+    <row r="1" spans="1:23" s="4" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24">
         <v>7</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="77" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="71"/>
+      <c r="P1" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="59"/>
+      <c r="U1" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="78" t="s">
+      <c r="V1" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="79"/>
-      <c r="P1" s="30" t="s">
+      <c r="W1" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="16" t="s">
+    </row>
+    <row r="2" spans="1:23" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="28">
+        <v>6</v>
+      </c>
+      <c r="F2" s="21">
+        <v>7</v>
+      </c>
+      <c r="G2" s="21">
+        <v>8</v>
+      </c>
+      <c r="H2" s="21">
+        <v>9</v>
+      </c>
+      <c r="I2" s="21">
+        <v>10</v>
+      </c>
+      <c r="J2" s="21">
         <v>11</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="K2" s="21">
         <v>12</v>
       </c>
-      <c r="S1" s="67"/>
-      <c r="U1" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="80" t="s">
+      <c r="L2" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="60"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+    </row>
+    <row r="3" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="80" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="61" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="34">
-        <v>6</v>
-      </c>
-      <c r="F2" s="24">
-        <v>7</v>
-      </c>
-      <c r="G2" s="24">
-        <v>8</v>
-      </c>
-      <c r="H2" s="24">
-        <v>9</v>
-      </c>
-      <c r="I2" s="24">
-        <v>10</v>
-      </c>
-      <c r="J2" s="24">
-        <v>11</v>
-      </c>
-      <c r="K2" s="24">
-        <v>12</v>
-      </c>
-      <c r="L2" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="24">
-        <v>1</v>
-      </c>
-      <c r="O2" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="S2" s="68"/>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="81"/>
-    </row>
-    <row r="3" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="62">
+        <v>35</v>
+      </c>
+      <c r="D3" s="55">
         <f>Vize!N3</f>
         <v>100</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="29">
         <v>0</v>
       </c>
       <c r="F3" s="7">
@@ -3288,42 +3227,44 @@
       <c r="K3" s="7">
         <v>2</v>
       </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="14">
-        <f t="shared" ref="M3:M30" si="0">SUM(E3:K3)*50/(A$1-L3)</f>
+      <c r="L3" s="35"/>
+      <c r="M3" s="13">
+        <f t="shared" ref="M3:M19" si="0">SUM(E3:K3)*50/(A$1-L3)</f>
         <v>57.142857142857146</v>
       </c>
       <c r="N3" s="6"/>
-      <c r="O3" s="14">
-        <f t="shared" ref="O3:O30" si="1">N3</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="18">
-        <f t="shared" ref="Q3:Q30" si="2">MIN(100,M3*(0.2+0.25)+O3*(0.25+0.1)+P3*(0.55+0.15))</f>
-        <v>25.714285714285715</v>
-      </c>
-      <c r="R3" s="18">
-        <f t="shared" ref="R3:R30" si="3">ROUND(D3,2)*0.4+Q3*0.6</f>
-        <v>55.428571428571431</v>
-      </c>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
+      <c r="O3" s="13">
+        <f t="shared" ref="O3:O19" si="1">N3</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="6">
+        <v>72</v>
+      </c>
+      <c r="Q3" s="17">
+        <f>MIN(100,M3*(0.4+0.1)+O3*(0)+(P3+13)*(0.6+0.15))</f>
+        <v>92.321428571428569</v>
+      </c>
+      <c r="R3" s="17">
+        <f t="shared" ref="R3:R19" si="2">ROUND(D3,2)*0.4+Q3*0.6</f>
+        <v>95.392857142857139</v>
+      </c>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="62">
+        <v>25</v>
+      </c>
+      <c r="D4" s="55">
         <f>Vize!N4</f>
         <v>96.487499999999983</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="29">
         <v>1</v>
       </c>
       <c r="F4" s="7">
@@ -3344,42 +3285,44 @@
       <c r="K4" s="7">
         <v>2</v>
       </c>
-      <c r="L4" s="42"/>
-      <c r="M4" s="14">
+      <c r="L4" s="35"/>
+      <c r="M4" s="13">
         <f t="shared" si="0"/>
         <v>66.428571428571431</v>
       </c>
       <c r="N4" s="6"/>
-      <c r="O4" s="14">
+      <c r="O4" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="18">
+      <c r="P4" s="6">
+        <v>87</v>
+      </c>
+      <c r="Q4" s="17">
+        <f t="shared" ref="Q4:Q19" si="3">MIN(100,M4*(0.4+0.1)+O4*(0)+(P4+13)*(0.6+0.15))</f>
+        <v>100</v>
+      </c>
+      <c r="R4" s="17">
         <f t="shared" si="2"/>
-        <v>29.892857142857146</v>
-      </c>
-      <c r="R4" s="18">
-        <f t="shared" si="3"/>
-        <v>56.531714285714287</v>
-      </c>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
+        <v>98.596000000000004</v>
+      </c>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
     </row>
     <row r="5" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="62">
+      <c r="D5" s="55">
         <f>Vize!N5</f>
         <v>85.2</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="29">
         <v>0</v>
       </c>
       <c r="F5" s="7">
@@ -3400,42 +3343,44 @@
       <c r="K5" s="7">
         <v>2</v>
       </c>
-      <c r="L5" s="42"/>
-      <c r="M5" s="14">
+      <c r="L5" s="35"/>
+      <c r="M5" s="13">
         <f t="shared" si="0"/>
         <v>28.571428571428573</v>
       </c>
       <c r="N5" s="6"/>
-      <c r="O5" s="14">
+      <c r="O5" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="18">
+      <c r="P5" s="6">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="17">
+        <f t="shared" si="3"/>
+        <v>48.035714285714285</v>
+      </c>
+      <c r="R5" s="17">
         <f t="shared" si="2"/>
-        <v>12.857142857142858</v>
-      </c>
-      <c r="R5" s="18">
-        <f t="shared" si="3"/>
-        <v>41.794285714285721</v>
-      </c>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
+        <v>62.901428571428575</v>
+      </c>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
     </row>
     <row r="6" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="62">
+        <v>27</v>
+      </c>
+      <c r="D6" s="55">
         <f>Vize!N6</f>
         <v>84.399999999999991</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="29">
         <v>0</v>
       </c>
       <c r="F6" s="7">
@@ -3456,42 +3401,44 @@
       <c r="K6" s="7">
         <v>0</v>
       </c>
-      <c r="L6" s="42"/>
-      <c r="M6" s="14">
+      <c r="L6" s="35"/>
+      <c r="M6" s="13">
         <f t="shared" si="0"/>
         <v>28.571428571428573</v>
       </c>
       <c r="N6" s="6"/>
-      <c r="O6" s="14">
+      <c r="O6" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="18">
+      <c r="P6" s="6">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="17">
+        <f t="shared" si="3"/>
+        <v>55.535714285714285</v>
+      </c>
+      <c r="R6" s="17">
         <f t="shared" si="2"/>
-        <v>12.857142857142858</v>
-      </c>
-      <c r="R6" s="18">
-        <f t="shared" si="3"/>
-        <v>41.47428571428572</v>
-      </c>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
+        <v>67.081428571428575</v>
+      </c>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
     </row>
     <row r="7" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="62">
+        <v>32</v>
+      </c>
+      <c r="D7" s="55">
         <f>Vize!N7</f>
         <v>80.899999999999991</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="29">
         <v>0</v>
       </c>
       <c r="F7" s="7">
@@ -3512,42 +3459,44 @@
       <c r="K7" s="7">
         <v>0</v>
       </c>
-      <c r="L7" s="42"/>
-      <c r="M7" s="14">
+      <c r="L7" s="35"/>
+      <c r="M7" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N7" s="6"/>
-      <c r="O7" s="14">
+      <c r="O7" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="18">
+      <c r="P7" s="6">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="17">
+        <f t="shared" si="3"/>
+        <v>38.25</v>
+      </c>
+      <c r="R7" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="18">
-        <f t="shared" si="3"/>
-        <v>32.360000000000007</v>
-      </c>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
+        <v>55.31</v>
+      </c>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
     </row>
     <row r="8" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="62">
+        <v>30</v>
+      </c>
+      <c r="D8" s="55">
         <f>Vize!N8</f>
         <v>77.7</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="29">
         <v>0</v>
       </c>
       <c r="F8" s="7">
@@ -3568,42 +3517,44 @@
       <c r="K8" s="7">
         <v>0</v>
       </c>
-      <c r="L8" s="42"/>
-      <c r="M8" s="14">
+      <c r="L8" s="35"/>
+      <c r="M8" s="13">
         <f t="shared" si="0"/>
         <v>7.1428571428571432</v>
       </c>
       <c r="N8" s="6"/>
-      <c r="O8" s="14">
+      <c r="O8" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="18">
+      <c r="P8" s="6">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="17">
+        <f t="shared" si="3"/>
+        <v>36.571428571428569</v>
+      </c>
+      <c r="R8" s="17">
         <f t="shared" si="2"/>
-        <v>3.2142857142857144</v>
-      </c>
-      <c r="R8" s="18">
-        <f t="shared" si="3"/>
-        <v>33.008571428571429</v>
-      </c>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
+        <v>53.022857142857141</v>
+      </c>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
     </row>
     <row r="9" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="62">
+        <v>50</v>
+      </c>
+      <c r="D9" s="55">
         <f>Vize!N9</f>
         <v>67.3</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="29">
         <v>0</v>
       </c>
       <c r="F9" s="7">
@@ -3624,42 +3575,44 @@
       <c r="K9" s="7">
         <v>1.7</v>
       </c>
-      <c r="L9" s="42"/>
-      <c r="M9" s="14">
+      <c r="L9" s="35"/>
+      <c r="M9" s="13">
         <f t="shared" si="0"/>
         <v>33.571428571428569</v>
       </c>
       <c r="N9" s="6"/>
-      <c r="O9" s="14">
+      <c r="O9" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="18">
+      <c r="P9" s="6">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="17">
+        <f t="shared" si="3"/>
+        <v>56.535714285714285</v>
+      </c>
+      <c r="R9" s="17">
         <f t="shared" si="2"/>
-        <v>15.107142857142856</v>
-      </c>
-      <c r="R9" s="18">
-        <f t="shared" si="3"/>
-        <v>35.984285714285718</v>
-      </c>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
+        <v>60.841428571428573</v>
+      </c>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
     </row>
     <row r="10" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="62">
+        <v>29</v>
+      </c>
+      <c r="D10" s="55">
         <f>Vize!N10</f>
         <v>66.5</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="29">
         <v>0</v>
       </c>
       <c r="F10" s="7">
@@ -3680,42 +3633,44 @@
       <c r="K10" s="7">
         <v>0</v>
       </c>
-      <c r="L10" s="42"/>
-      <c r="M10" s="14">
+      <c r="L10" s="35"/>
+      <c r="M10" s="13">
         <f t="shared" si="0"/>
         <v>35.714285714285715</v>
       </c>
       <c r="N10" s="6"/>
-      <c r="O10" s="14">
+      <c r="O10" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="18">
+      <c r="P10" s="6">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="17">
+        <f t="shared" si="3"/>
+        <v>58.357142857142861</v>
+      </c>
+      <c r="R10" s="17">
         <f t="shared" si="2"/>
-        <v>16.071428571428573</v>
-      </c>
-      <c r="R10" s="18">
-        <f t="shared" si="3"/>
-        <v>36.242857142857147</v>
-      </c>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
+        <v>61.614285714285714</v>
+      </c>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
     </row>
     <row r="11" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="62">
+        <v>23</v>
+      </c>
+      <c r="D11" s="55">
         <f>Vize!N11</f>
         <v>60.85</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="29">
         <v>0</v>
       </c>
       <c r="F11" s="7">
@@ -3736,42 +3691,43 @@
       <c r="K11" s="7">
         <v>0</v>
       </c>
-      <c r="L11" s="42"/>
-      <c r="M11" s="14">
+      <c r="L11" s="35"/>
+      <c r="M11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N11" s="6"/>
-      <c r="O11" s="14">
+      <c r="O11" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="18">
+      <c r="P11" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>0</v>
+      </c>
+      <c r="R11" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="18">
-        <f t="shared" si="3"/>
         <v>24.340000000000003</v>
       </c>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
     </row>
     <row r="12" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="62">
+        <v>45</v>
+      </c>
+      <c r="D12" s="55">
         <f>Vize!N12</f>
         <v>53.6</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="29">
         <v>0</v>
       </c>
       <c r="F12" s="7">
@@ -3792,45 +3748,47 @@
       <c r="K12" s="7">
         <v>0</v>
       </c>
-      <c r="L12" s="42"/>
-      <c r="M12" s="14">
+      <c r="L12" s="35"/>
+      <c r="M12" s="13">
         <f t="shared" si="0"/>
         <v>7.1428571428571432</v>
       </c>
       <c r="N12" s="6"/>
-      <c r="O12" s="14">
+      <c r="O12" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="18">
+      <c r="P12" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q12" s="17">
+        <f t="shared" si="3"/>
+        <v>30.571428571428573</v>
+      </c>
+      <c r="R12" s="17">
         <f t="shared" si="2"/>
-        <v>3.2142857142857144</v>
-      </c>
-      <c r="R12" s="18">
-        <f t="shared" si="3"/>
-        <v>23.368571428571428</v>
-      </c>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
+        <v>39.782857142857139</v>
+      </c>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
     </row>
     <row r="13" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="62">
+        <v>42</v>
+      </c>
+      <c r="D13" s="55">
         <f>Vize!N13</f>
         <v>37.6</v>
       </c>
-      <c r="E13" s="35">
-        <v>0</v>
-      </c>
-      <c r="F13" s="37">
+      <c r="E13" s="29">
+        <v>0</v>
+      </c>
+      <c r="F13" s="30">
         <v>0</v>
       </c>
       <c r="G13" s="7">
@@ -3848,42 +3806,44 @@
       <c r="K13" s="7">
         <v>0</v>
       </c>
-      <c r="L13" s="42"/>
-      <c r="M13" s="14">
+      <c r="L13" s="35"/>
+      <c r="M13" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N13" s="6"/>
-      <c r="O13" s="14">
+      <c r="O13" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="18">
+      <c r="P13" s="6">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="17">
+        <f t="shared" si="3"/>
+        <v>12.75</v>
+      </c>
+      <c r="R13" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="18">
-        <f t="shared" si="3"/>
-        <v>15.040000000000001</v>
-      </c>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
+        <v>22.69</v>
+      </c>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
     </row>
     <row r="14" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="62">
+        <v>39</v>
+      </c>
+      <c r="D14" s="55">
         <f>Vize!N14</f>
         <v>34.4</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="29">
         <v>0</v>
       </c>
       <c r="F14" s="7">
@@ -3904,42 +3864,44 @@
       <c r="K14" s="7">
         <v>0</v>
       </c>
-      <c r="L14" s="42"/>
-      <c r="M14" s="14">
+      <c r="L14" s="35"/>
+      <c r="M14" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="14">
+      <c r="O14" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="18">
+      <c r="P14" s="6">
+        <v>31</v>
+      </c>
+      <c r="Q14" s="17">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="R14" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="18">
-        <f t="shared" si="3"/>
-        <v>13.76</v>
-      </c>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
+        <v>33.56</v>
+      </c>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
     </row>
     <row r="15" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="62">
+        <v>40</v>
+      </c>
+      <c r="D15" s="55">
         <f>Vize!N15</f>
         <v>30.4</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="29">
         <v>0</v>
       </c>
       <c r="F15" s="7">
@@ -3960,42 +3922,43 @@
       <c r="K15" s="7">
         <v>0</v>
       </c>
-      <c r="L15" s="42"/>
-      <c r="M15" s="14">
+      <c r="L15" s="35"/>
+      <c r="M15" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N15" s="6"/>
-      <c r="O15" s="14">
+      <c r="O15" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="18">
+      <c r="P15" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="17">
+        <v>0</v>
+      </c>
+      <c r="R15" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="18">
-        <f t="shared" si="3"/>
         <v>12.16</v>
       </c>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
     </row>
     <row r="16" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="62">
+        <v>47</v>
+      </c>
+      <c r="D16" s="55">
         <f>Vize!N16</f>
         <v>21.599999999999998</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16" s="29">
         <v>0</v>
       </c>
       <c r="F16" s="7">
@@ -4016,42 +3979,44 @@
       <c r="K16" s="7">
         <v>0</v>
       </c>
-      <c r="L16" s="42"/>
-      <c r="M16" s="14">
+      <c r="L16" s="35"/>
+      <c r="M16" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N16" s="6"/>
-      <c r="O16" s="14">
+      <c r="O16" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="18">
+      <c r="P16" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="17">
+        <f t="shared" si="3"/>
+        <v>13.5</v>
+      </c>
+      <c r="R16" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R16" s="18">
-        <f t="shared" si="3"/>
-        <v>8.64</v>
-      </c>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
+        <v>16.740000000000002</v>
+      </c>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
     </row>
     <row r="17" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="62">
+        <v>21</v>
+      </c>
+      <c r="D17" s="55">
         <f>Vize!N17</f>
         <v>33.5625</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="29">
         <v>0</v>
       </c>
       <c r="F17" s="7">
@@ -4072,42 +4037,44 @@
       <c r="K17" s="7">
         <v>1.9</v>
       </c>
-      <c r="L17" s="42"/>
-      <c r="M17" s="14">
+      <c r="L17" s="35"/>
+      <c r="M17" s="13">
         <f t="shared" si="0"/>
         <v>56.428571428571431</v>
       </c>
       <c r="N17" s="6"/>
-      <c r="O17" s="14">
+      <c r="O17" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="18">
+      <c r="P17" s="6">
+        <v>60</v>
+      </c>
+      <c r="Q17" s="17">
+        <f t="shared" si="3"/>
+        <v>82.964285714285722</v>
+      </c>
+      <c r="R17" s="17">
         <f t="shared" si="2"/>
-        <v>25.392857142857146</v>
-      </c>
-      <c r="R17" s="18">
-        <f t="shared" si="3"/>
-        <v>28.659714285714287</v>
-      </c>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
+        <v>63.202571428571432</v>
+      </c>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
     </row>
     <row r="18" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="62">
+        <v>37</v>
+      </c>
+      <c r="D18" s="55">
         <f>Vize!N18</f>
         <v>7.5</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="29">
         <v>0</v>
       </c>
       <c r="F18" s="7">
@@ -4128,42 +4095,43 @@
       <c r="K18" s="7">
         <v>0</v>
       </c>
-      <c r="L18" s="42"/>
-      <c r="M18" s="14">
+      <c r="L18" s="35"/>
+      <c r="M18" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N18" s="6"/>
-      <c r="O18" s="14">
+      <c r="O18" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="18">
+      <c r="P18" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="17">
+        <v>0</v>
+      </c>
+      <c r="R18" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R18" s="18">
-        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
     </row>
     <row r="19" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="62">
+        <v>34</v>
+      </c>
+      <c r="D19" s="55">
         <f>Vize!N19</f>
         <v>1.875</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="29">
         <v>0</v>
       </c>
       <c r="F19" s="7">
@@ -4184,488 +4152,336 @@
       <c r="K19" s="7">
         <v>0</v>
       </c>
-      <c r="L19" s="42"/>
-      <c r="M19" s="14">
+      <c r="L19" s="35"/>
+      <c r="M19" s="13">
         <f t="shared" si="0"/>
         <v>14.285714285714286</v>
       </c>
       <c r="N19" s="6"/>
-      <c r="O19" s="14">
+      <c r="O19" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="18">
+      <c r="P19" s="6">
+        <v>49</v>
+      </c>
+      <c r="Q19" s="17">
+        <f t="shared" si="3"/>
+        <v>53.642857142857146</v>
+      </c>
+      <c r="R19" s="17">
         <f t="shared" si="2"/>
-        <v>6.4285714285714288</v>
-      </c>
-      <c r="R19" s="18">
-        <f t="shared" si="3"/>
-        <v>4.6091428571428574</v>
-      </c>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
+        <v>32.937714285714286</v>
+      </c>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
     </row>
     <row r="20" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="3"/>
       <c r="C20" s="11"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="35"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L20" s="35"/>
+      <c r="M20" s="13"/>
       <c r="N20" s="6"/>
-      <c r="O20" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="O20" s="13"/>
       <c r="P20" s="6"/>
-      <c r="Q20" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R20" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="18"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
     </row>
     <row r="21" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="3"/>
       <c r="C21" s="11"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="35"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L21" s="35"/>
+      <c r="M21" s="13"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="O21" s="13"/>
       <c r="P21" s="6"/>
-      <c r="Q21" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R21" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U21" s="18"/>
-      <c r="V21" s="18"/>
-      <c r="W21" s="18"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="17"/>
     </row>
     <row r="22" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="35"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L22" s="35"/>
+      <c r="M22" s="13"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="O22" s="13"/>
       <c r="P22" s="6"/>
-      <c r="Q22" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R22" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="18"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+      <c r="W22" s="17"/>
     </row>
     <row r="23" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="35"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L23" s="35"/>
+      <c r="M23" s="13"/>
       <c r="N23" s="6"/>
-      <c r="O23" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="O23" s="13"/>
       <c r="P23" s="6"/>
-      <c r="Q23" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U23" s="18"/>
-      <c r="V23" s="18"/>
-      <c r="W23" s="18"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="17"/>
     </row>
     <row r="24" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="35"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L24" s="35"/>
+      <c r="M24" s="13"/>
       <c r="N24" s="6"/>
-      <c r="O24" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="O24" s="13"/>
       <c r="P24" s="6"/>
-      <c r="Q24" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R24" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U24" s="18"/>
-      <c r="V24" s="18"/>
-      <c r="W24" s="18"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="17"/>
     </row>
     <row r="25" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="35"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="12"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L25" s="35"/>
+      <c r="M25" s="13"/>
       <c r="N25" s="6"/>
-      <c r="O25" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="O25" s="13"/>
       <c r="P25" s="6"/>
-      <c r="Q25" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R25" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U25" s="18"/>
-      <c r="V25" s="18"/>
-      <c r="W25" s="18"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
     </row>
     <row r="26" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="35"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="29"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L26" s="35"/>
+      <c r="M26" s="13"/>
       <c r="N26" s="6"/>
-      <c r="O26" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="O26" s="13"/>
       <c r="P26" s="6"/>
-      <c r="Q26" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R26" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U26" s="18"/>
-      <c r="V26" s="18"/>
-      <c r="W26" s="18"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
     </row>
     <row r="27" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="35"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L27" s="35"/>
+      <c r="M27" s="13"/>
       <c r="N27" s="6"/>
-      <c r="O27" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="O27" s="13"/>
       <c r="P27" s="6"/>
-      <c r="Q27" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R27" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U27" s="18"/>
-      <c r="V27" s="18"/>
-      <c r="W27" s="18"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
     </row>
     <row r="28" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="35"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L28" s="35"/>
+      <c r="M28" s="13"/>
       <c r="N28" s="6"/>
-      <c r="O28" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="O28" s="13"/>
       <c r="P28" s="6"/>
-      <c r="Q28" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R28" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U28" s="18"/>
-      <c r="V28" s="18"/>
-      <c r="W28" s="18"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
     </row>
     <row r="29" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="35"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L29" s="35"/>
+      <c r="M29" s="13"/>
       <c r="N29" s="6"/>
-      <c r="O29" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="O29" s="13"/>
       <c r="P29" s="6"/>
-      <c r="Q29" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R29" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U29" s="18"/>
-      <c r="V29" s="18"/>
-      <c r="W29" s="18"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="17"/>
     </row>
     <row r="30" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="35"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L30" s="35"/>
+      <c r="M30" s="13"/>
       <c r="N30" s="6"/>
-      <c r="O30" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="O30" s="13"/>
       <c r="P30" s="6"/>
-      <c r="Q30" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R30" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U30" s="18"/>
-      <c r="V30" s="18"/>
-      <c r="W30" s="18"/>
-    </row>
-    <row r="31" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="66"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="U31" s="18"/>
-      <c r="V31" s="18"/>
-      <c r="W31" s="18"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+    </row>
+    <row r="31" spans="1:23" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="S31" s="62"/>
     </row>
     <row r="32" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="66"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-    </row>
-    <row r="33" spans="1:23" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="66"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="U33" s="18"/>
-      <c r="V33" s="18"/>
-      <c r="W33" s="18"/>
-    </row>
-    <row r="34" spans="1:23" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+    </row>
+    <row r="33" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+    </row>
+    <row r="34" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="63"/>
+      <c r="D34" s="56"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
@@ -4673,14 +4489,15 @@
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="S34" s="70"/>
-    </row>
-    <row r="35" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+    </row>
+    <row r="35" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="63"/>
+      <c r="D35" s="56"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
@@ -4692,11 +4509,11 @@
       <c r="N35" s="9"/>
       <c r="O35" s="9"/>
     </row>
-    <row r="36" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="63"/>
+      <c r="D36" s="56"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
@@ -4708,11 +4525,11 @@
       <c r="N36" s="9"/>
       <c r="O36" s="9"/>
     </row>
-    <row r="37" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="63"/>
+      <c r="D37" s="56"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
@@ -4724,11 +4541,11 @@
       <c r="N37" s="9"/>
       <c r="O37" s="9"/>
     </row>
-    <row r="38" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="63"/>
+      <c r="D38" s="56"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
@@ -4740,11 +4557,11 @@
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
     </row>
-    <row r="39" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="63"/>
+      <c r="D39" s="56"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
@@ -4756,11 +4573,11 @@
       <c r="N39" s="9"/>
       <c r="O39" s="9"/>
     </row>
-    <row r="40" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="63"/>
+      <c r="D40" s="56"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
@@ -4772,11 +4589,11 @@
       <c r="N40" s="9"/>
       <c r="O40" s="9"/>
     </row>
-    <row r="41" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="63"/>
+      <c r="D41" s="56"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
@@ -4788,11 +4605,11 @@
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
     </row>
-    <row r="42" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="63"/>
+      <c r="D42" s="56"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
@@ -4804,11 +4621,11 @@
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
     </row>
-    <row r="43" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="63"/>
+      <c r="D43" s="56"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
@@ -4820,11 +4637,11 @@
       <c r="N43" s="9"/>
       <c r="O43" s="9"/>
     </row>
-    <row r="44" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="63"/>
+      <c r="D44" s="56"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
@@ -4836,11 +4653,11 @@
       <c r="N44" s="9"/>
       <c r="O44" s="9"/>
     </row>
-    <row r="45" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
-      <c r="D45" s="63"/>
+      <c r="D45" s="56"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -4852,11 +4669,11 @@
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
     </row>
-    <row r="46" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="63"/>
+      <c r="D46" s="56"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -4868,11 +4685,11 @@
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
     </row>
-    <row r="47" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="63"/>
+      <c r="D47" s="56"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
@@ -4884,11 +4701,11 @@
       <c r="N47" s="9"/>
       <c r="O47" s="9"/>
     </row>
-    <row r="48" spans="1:23" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="63"/>
+      <c r="D48" s="56"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
@@ -4904,7 +4721,7 @@
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="63"/>
+      <c r="D49" s="56"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
@@ -4920,7 +4737,7 @@
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="63"/>
+      <c r="D50" s="56"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
@@ -4936,7 +4753,7 @@
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="63"/>
+      <c r="D51" s="56"/>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
@@ -4952,7 +4769,7 @@
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="63"/>
+      <c r="D52" s="56"/>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
@@ -4968,7 +4785,7 @@
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
-      <c r="D53" s="63"/>
+      <c r="D53" s="56"/>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
@@ -4984,7 +4801,7 @@
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="63"/>
+      <c r="D54" s="56"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
@@ -5000,7 +4817,7 @@
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
-      <c r="D55" s="63"/>
+      <c r="D55" s="56"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
@@ -5016,7 +4833,7 @@
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="63"/>
+      <c r="D56" s="56"/>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
@@ -5032,7 +4849,7 @@
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
-      <c r="D57" s="63"/>
+      <c r="D57" s="56"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
@@ -5048,7 +4865,7 @@
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
-      <c r="D58" s="63"/>
+      <c r="D58" s="56"/>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
@@ -5064,7 +4881,7 @@
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
-      <c r="D59" s="63"/>
+      <c r="D59" s="56"/>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
@@ -5080,7 +4897,7 @@
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="63"/>
+      <c r="D60" s="56"/>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
@@ -5096,7 +4913,7 @@
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
-      <c r="D61" s="63"/>
+      <c r="D61" s="56"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
@@ -5112,7 +4929,7 @@
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
-      <c r="D62" s="63"/>
+      <c r="D62" s="56"/>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
@@ -5128,7 +4945,7 @@
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
-      <c r="D63" s="63"/>
+      <c r="D63" s="56"/>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
@@ -5144,7 +4961,7 @@
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
-      <c r="D64" s="63"/>
+      <c r="D64" s="56"/>
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
@@ -5160,7 +4977,7 @@
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
-      <c r="D65" s="63"/>
+      <c r="D65" s="56"/>
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
@@ -5176,7 +4993,7 @@
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
-      <c r="D66" s="63"/>
+      <c r="D66" s="56"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
@@ -5192,7 +5009,7 @@
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
-      <c r="D67" s="63"/>
+      <c r="D67" s="56"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
@@ -5208,7 +5025,7 @@
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="63"/>
+      <c r="D68" s="56"/>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
@@ -5224,7 +5041,7 @@
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
-      <c r="D69" s="63"/>
+      <c r="D69" s="56"/>
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
@@ -5240,7 +5057,7 @@
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
-      <c r="D70" s="63"/>
+      <c r="D70" s="56"/>
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
@@ -5256,7 +5073,7 @@
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="63"/>
+      <c r="D71" s="56"/>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
@@ -5272,7 +5089,7 @@
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="63"/>
+      <c r="D72" s="56"/>
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
@@ -5288,7 +5105,7 @@
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
-      <c r="D73" s="63"/>
+      <c r="D73" s="56"/>
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
@@ -5304,7 +5121,7 @@
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="63"/>
+      <c r="D74" s="56"/>
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
@@ -5320,7 +5137,7 @@
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="63"/>
+      <c r="D75" s="56"/>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
@@ -5336,7 +5153,7 @@
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="63"/>
+      <c r="D76" s="56"/>
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
@@ -5352,7 +5169,7 @@
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
-      <c r="D77" s="63"/>
+      <c r="D77" s="56"/>
       <c r="E77" s="8"/>
       <c r="F77" s="8"/>
       <c r="G77" s="8"/>
@@ -5368,7 +5185,7 @@
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="63"/>
+      <c r="D78" s="56"/>
       <c r="E78" s="8"/>
       <c r="F78" s="8"/>
       <c r="G78" s="8"/>
@@ -5379,54 +5196,6 @@
       <c r="M78" s="9"/>
       <c r="N78" s="9"/>
       <c r="O78" s="9"/>
-    </row>
-    <row r="79" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="8"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="63"/>
-      <c r="E79" s="8"/>
-      <c r="F79" s="8"/>
-      <c r="G79" s="8"/>
-      <c r="H79" s="8"/>
-      <c r="I79" s="8"/>
-      <c r="J79" s="8"/>
-      <c r="K79" s="8"/>
-      <c r="M79" s="9"/>
-      <c r="N79" s="9"/>
-      <c r="O79" s="9"/>
-    </row>
-    <row r="80" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="8"/>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="63"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="8"/>
-      <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
-      <c r="I80" s="8"/>
-      <c r="J80" s="8"/>
-      <c r="K80" s="8"/>
-      <c r="M80" s="9"/>
-      <c r="N80" s="9"/>
-      <c r="O80" s="9"/>
-    </row>
-    <row r="81" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="8"/>
-      <c r="B81" s="8"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="63"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="8"/>
-      <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
-      <c r="I81" s="8"/>
-      <c r="J81" s="8"/>
-      <c r="K81" s="8"/>
-      <c r="M81" s="9"/>
-      <c r="N81" s="9"/>
-      <c r="O81" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A3:S30">
@@ -5439,7 +5208,7 @@
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E31:L33 E3:K30">
+  <conditionalFormatting sqref="E3:K30">
     <cfRule type="cellIs" dxfId="10" priority="29" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
@@ -5451,49 +5220,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M33">
-    <cfRule type="dataBar" priority="28">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3F325F88-05E0-41BA-AA33-7B854FBE8033}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O33">
-    <cfRule type="dataBar" priority="27">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{22C9DC09-E768-4CCB-8C68-41B5A3538743}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q33">
-    <cfRule type="dataBar" priority="24">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F9C7B28C-32E1-4B0D-97BC-F416D05D2AA7}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N33">
+  <conditionalFormatting sqref="N3:N30">
     <cfRule type="cellIs" dxfId="7" priority="20" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
@@ -5510,34 +5237,6 @@
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R33">
-    <cfRule type="dataBar" priority="15">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2008DEFA-B118-4E92-B0F8-C5059B874A32}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D33">
-    <cfRule type="dataBar" priority="10">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FF44BC67-0C1D-46A1-8F9C-F95AA3B0ECDF}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D7">
     <cfRule type="dataBar" priority="9">
       <dataBar>
@@ -5552,7 +5251,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P33">
+  <conditionalFormatting sqref="P3:P30">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
@@ -5582,8 +5281,78 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:U33">
-    <cfRule type="dataBar" priority="3">
+  <conditionalFormatting sqref="M3:M30">
+    <cfRule type="dataBar" priority="348">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3F325F88-05E0-41BA-AA33-7B854FBE8033}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O30">
+    <cfRule type="dataBar" priority="349">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{22C9DC09-E768-4CCB-8C68-41B5A3538743}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q30">
+    <cfRule type="dataBar" priority="350">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F9C7B28C-32E1-4B0D-97BC-F416D05D2AA7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3:R30">
+    <cfRule type="dataBar" priority="351">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2008DEFA-B118-4E92-B0F8-C5059B874A32}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D30">
+    <cfRule type="dataBar" priority="352">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FF44BC67-0C1D-46A1-8F9C-F95AA3B0ECDF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3:U30">
+    <cfRule type="dataBar" priority="353">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5596,8 +5365,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V33">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="V3:V30">
+    <cfRule type="dataBar" priority="354">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5610,8 +5379,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W3:W33">
-    <cfRule type="dataBar" priority="1">
+  <conditionalFormatting sqref="W3:W30">
+    <cfRule type="dataBar" priority="355">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5630,61 +5399,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3F325F88-05E0-41BA-AA33-7B854FBE8033}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>M3:M33</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{22C9DC09-E768-4CCB-8C68-41B5A3538743}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>O3:O33</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F9C7B28C-32E1-4B0D-97BC-F416D05D2AA7}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>Q3:Q33</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2008DEFA-B118-4E92-B0F8-C5059B874A32}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>R3:R33</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FF44BC67-0C1D-46A1-8F9C-F95AA3B0ECDF}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D3:D33</xm:sqref>
-        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5152AADF-8FC6-4ED1-821D-0A79F65C7F2C}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
@@ -5710,6 +5424,61 @@
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3F325F88-05E0-41BA-AA33-7B854FBE8033}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M3:M30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{22C9DC09-E768-4CCB-8C68-41B5A3538743}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O3:O30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F9C7B28C-32E1-4B0D-97BC-F416D05D2AA7}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>Q3:Q30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2008DEFA-B118-4E92-B0F8-C5059B874A32}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>R3:R30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FF44BC67-0C1D-46A1-8F9C-F95AA3B0ECDF}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D3:D30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BF843C8A-B269-4D72-852C-A7007E8E7593}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
@@ -5718,7 +5487,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U3:U33</xm:sqref>
+          <xm:sqref>U3:U30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FD11F04D-4F39-4ECF-9A10-1B557EAB081C}">
@@ -5729,7 +5498,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>V3:V33</xm:sqref>
+          <xm:sqref>V3:V30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E17DD4D3-1A79-45E5-85F3-F9DE9D06FB78}">
@@ -5740,7 +5509,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>W3:W33</xm:sqref>
+          <xm:sqref>W3:W30</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>